<commit_message>
Added the tests to test suite and moved the before suite method from all test classes to abstrat base class.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
   <si>
     <t>GET</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>status=200||content=hi</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
       </c>
       <c r="K3"/>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">

</xml_diff>

<commit_message>
Changed the dynamic parameters as they come from system peroperties
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>GET</t>
   </si>
@@ -94,15 +94,9 @@
     <t>POST</t>
   </si>
   <si>
-    <t>X-1P-User=a99ba4dc-45be-4ad2-9c9e-22e78584b82b||Content-Type=application/json</t>
-  </si>
-  <si>
     <t>{"targetType":"TRRecord","targetId":"456539938WOS1","content":"hello"}</t>
   </si>
   <si>
-    <t>/comments/user/a99ba4dc-45be-4ad2-9c9e-22e78584b82b</t>
-  </si>
-  <si>
     <t>status=200||found=true</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>DEPFAIL</t>
-  </si>
-  <si>
     <t>comments.id</t>
   </si>
   <si>
@@ -155,13 +146,18 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>/comments/user/(SYS_USER1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -535,24 +531,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="28.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="80.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="47.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="31.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -610,21 +606,21 @@
         <v>25</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -632,27 +628,24 @@
         <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
-      <c r="G3"/>
       <c r="H3"/>
-      <c r="I3"/>
       <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3"/>
+        <v>27</v>
+      </c>
       <c r="L3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">
@@ -666,27 +659,25 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4"/>
+        <v>44</v>
+      </c>
       <c r="H4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4"/>
+        <v>42</v>
+      </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
@@ -700,27 +691,25 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5"/>
+        <v>44</v>
+      </c>
       <c r="H5" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5"/>
+        <v>31</v>
+      </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
@@ -728,38 +717,36 @@
         <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6"/>
+        <v>44</v>
+      </c>
       <c r="H6" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
         <v>37</v>
-      </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>21</v>
@@ -768,15 +755,14 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7"/>
+        <v>44</v>
+      </c>
       <c r="H7"/>
       <c r="I7" t="s">
         <v>13</v>
@@ -784,9 +770,8 @@
       <c r="J7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K7"/>
       <c r="L7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test cases in to watchlist, type ahead and profile search scenarios Modified old test cases with new validations in to profiles, authoring and follow.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19635" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Authoring" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="64">
   <si>
     <t>GET</t>
   </si>
@@ -97,9 +97,6 @@
     <t>{"targetType":"TRRecord","targetId":"456539938WOS1","content":"hello"}</t>
   </si>
   <si>
-    <t>status=200||found=true</t>
-  </si>
-  <si>
     <t>View comments by user</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>{"appreciate":"UP"}</t>
   </si>
   <si>
-    <t>status=200||hasAppreciated=UP</t>
-  </si>
-  <si>
     <t>S1_TC_T6</t>
   </si>
   <si>
@@ -121,43 +115,104 @@
     <t>{"appreciate":"DOWN"}</t>
   </si>
   <si>
-    <t>status=200||hasAppreciated=DOWN</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
+    <t>comments.id</t>
+  </si>
+  <si>
+    <t>/comments/comment/(S1_TC_T1_comments.id)</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/Comment/(S1_TC_T1_comments.id)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>/comments/user/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>Check comments count for the given TR Record</t>
+  </si>
+  <si>
+    <t>S1_TC_T7</t>
+  </si>
+  <si>
+    <t>/comments/count/456539938WOS1/TRRecord</t>
+  </si>
+  <si>
+    <t>Create comment with bold and italic</t>
+  </si>
+  <si>
+    <t>S1_TC_T8</t>
+  </si>
+  <si>
+    <t>{"targetType":"TRRecord","targetId":"456539938WOS1","content":"mohana.yalamarthi@thomsonreuters.com        http://thomsonreuters.com/en.html         +91 8197818719"}</t>
+  </si>
+  <si>
+    <t>Create comment with link, email and phone</t>
+  </si>
+  <si>
+    <t>S1_TC_T9</t>
+  </si>
+  <si>
+    <t>status=200||found=true||comments.targetType=TRRecord||comments.targetId=456539938WOS1</t>
+  </si>
+  <si>
+    <t>status=200||content=hi||targetType=TRRecord||targetId=456539938WOS1</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1</t>
+  </si>
+  <si>
+    <t>{"targetType":"TRRecord","targetId":"456539938WOS1","content":"Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=DOWN||targetType=Comment||appreciateCount=0</t>
+  </si>
+  <si>
+    <t>S1_TC_T10</t>
+  </si>
+  <si>
+    <t>S1_TC_T11</t>
+  </si>
+  <si>
+    <t>/comments/comment/(S1_TC_T2_comments.id)</t>
+  </si>
+  <si>
+    <t>/comments/comment/(S1_TC_T3_comments.id)</t>
+  </si>
+  <si>
+    <t>S1_TC_T12</t>
+  </si>
+  <si>
+    <t>{"targetType":"TRRecord","targetId":"456539938WOS1","content":"&lt;abcd&gt;Hello&lt;abcd&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=hello</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>comments.id</t>
-  </si>
-  <si>
-    <t>status=200||comments.content=hello</t>
-  </si>
-  <si>
-    <t>/comments/comment/(S1_TC_T1_comments.id)</t>
-  </si>
-  <si>
-    <t>/appreciation/appreciate/Comment/(S1_TC_T1_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||content=hi</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
-  </si>
-  <si>
-    <t>/comments/user/(SYS_USER1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -529,26 +584,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="43.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="80.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="47.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="31.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="89.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -606,118 +661,127 @@
         <v>25</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
+      <c r="J2" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="90">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3"/>
-      <c r="H3"/>
-      <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="6"/>
       <c r="L5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -726,52 +790,244 @@
         <v>41</v>
       </c>
       <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="F8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
         <v>35</v>
       </c>
-      <c r="L6" t="s">
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="30">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7"/>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>37</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test validations
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="67">
   <si>
     <t>GET</t>
   </si>
@@ -160,21 +160,9 @@
     <t>status=200||found=true||comments.targetType=TRRecord||comments.targetId=456539938WOS1</t>
   </si>
   <si>
-    <t>status=200||content=hi||targetType=TRRecord||targetId=456539938WOS1</t>
-  </si>
-  <si>
-    <t>status=200||targetType=TRRecord||targetId=456539938WOS1</t>
-  </si>
-  <si>
     <t>{"targetType":"TRRecord","targetId":"456539938WOS1","content":"Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
   </si>
   <si>
-    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=DOWN||targetType=Comment||appreciateCount=0</t>
-  </si>
-  <si>
     <t>S1_TC_T10</t>
   </si>
   <si>
@@ -196,16 +184,37 @@
     <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=hello</t>
   </si>
   <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
-  </si>
-  <si>
     <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Create comment unsupported html format</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T1_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T2_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T3_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||content=hi||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T1_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(S1_TC_T1_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=DOWN||targetType=Comment||appreciateCount=0||targetId=(S1_TC_T1_comments.id)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
   </si>
 </sst>
 </file>
@@ -586,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -601,7 +610,7 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="5" width="31.28515625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="89.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="108.7109375" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
@@ -669,13 +678,13 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="90">
@@ -695,7 +704,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="4" t="s">
@@ -703,13 +712,13 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60">
@@ -733,17 +742,17 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45">
@@ -751,7 +760,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -767,13 +776,13 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
       <c r="K5" s="6"/>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -801,7 +810,7 @@
       </c>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -829,7 +838,7 @@
       </c>
       <c r="K7"/>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
@@ -859,11 +868,11 @@
         <v>13</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="K8"/>
       <c r="L8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
@@ -893,11 +902,11 @@
         <v>13</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="K9"/>
       <c r="L9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
@@ -927,16 +936,16 @@
         <v>13</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>21</v>
@@ -959,16 +968,16 @@
         <v>13</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>21</v>
@@ -977,13 +986,13 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -991,16 +1000,16 @@
         <v>15</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="K12"/>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>21</v>
@@ -1009,7 +1018,7 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -1023,11 +1032,11 @@
         <v>16</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="K13"/>
       <c r="L13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test cases to Profiles, Follow, Authoring API's Modified Type Ahead  API End point
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="75">
   <si>
     <t>GET</t>
   </si>
@@ -121,12 +121,6 @@
     <t>comments.id</t>
   </si>
   <si>
-    <t>/comments/comment/(S1_TC_T1_comments.id)</t>
-  </si>
-  <si>
-    <t>/appreciation/appreciate/Comment/(S1_TC_T1_comments.id)</t>
-  </si>
-  <si>
     <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
   </si>
   <si>
@@ -172,49 +166,79 @@
     <t>/comments/comment/(S1_TC_T2_comments.id)</t>
   </si>
   <si>
-    <t>/comments/comment/(S1_TC_T3_comments.id)</t>
-  </si>
-  <si>
     <t>S1_TC_T12</t>
   </si>
   <si>
     <t>{"targetType":"TRRecord","targetId":"456539938WOS1","content":"&lt;abcd&gt;Hello&lt;abcd&gt;"}</t>
   </si>
   <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Create comment unsupported html format</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>counterValue</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/Comment/(S1_TC_T2_comments.id)</t>
+  </si>
+  <si>
+    <t>S1_TC_T13</t>
+  </si>
+  <si>
+    <t>Delete a deleted comment</t>
+  </si>
+  <si>
+    <t>status=400</t>
+  </si>
+  <si>
+    <t>S1_TC_T14</t>
+  </si>
+  <si>
+    <t>Modify a deleted comment</t>
+  </si>
+  <si>
     <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=hello</t>
   </si>
   <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+    <t>status=200||content=hi||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T2_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(S1_TC_T2_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=DOWN||targetType=Comment||appreciateCount=0||targetId=(S1_TC_T2_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T2_comments.id)||content=</t>
+  </si>
+  <si>
+    <t>S1_TC_T15</t>
+  </si>
+  <si>
+    <t>status=429</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Create comment unsupported html format</t>
-  </si>
-  <si>
-    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T1_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T2_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T3_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||content=hi||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T1_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(S1_TC_T1_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=DOWN||targetType=Comment||appreciateCount=0||targetId=(S1_TC_T1_comments.id)</t>
-  </si>
-  <si>
-    <t>X-1P-User=(SYS_USER2)||Content-Type=application/json</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=TRRecord||comments.targetId=456539938WOS1||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T4_comments.id)||content=</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T12_comments.id)||content=</t>
+  </si>
+  <si>
+    <t>/comments/comment/(S1_TC_T4_comments.id)</t>
+  </si>
+  <si>
+    <t>/comments/comment/(S1_TC_T12_comments.id)</t>
   </si>
 </sst>
 </file>
@@ -593,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -611,7 +635,7 @@
     <col min="8" max="8" customWidth="true" style="5" width="31.28515625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="108.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
@@ -653,46 +677,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="4" t="s">
-        <v>55</v>
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="90">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -704,29 +724,29 @@
         <v>25</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="4" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="60">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -738,29 +758,27 @@
         <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="4" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="K4" s="6"/>
       <c r="L4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="90">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -772,45 +790,51 @@
         <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="6"/>
+      <c r="J5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="L5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6"/>
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="6"/>
       <c r="L6" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -824,7 +848,7 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -834,16 +858,16 @@
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K7"/>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
@@ -852,32 +876,32 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K8"/>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>20</v>
@@ -886,32 +910,32 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G9"/>
       <c r="H9" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K9"/>
       <c r="L9" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>31</v>
@@ -920,32 +944,32 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G10"/>
       <c r="H10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>21</v>
@@ -954,30 +978,30 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>21</v>
@@ -986,57 +1010,157 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="K12"/>
       <c r="L12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="60">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="F14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14"/>
+      <c r="L14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" t="s">
         <v>61</v>
       </c>
-      <c r="K13"/>
-      <c r="L13" t="s">
-        <v>57</v>
+      <c r="B15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Header field  in to 1PProfile
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="74">
   <si>
     <t>GET</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>status=429</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T4_comments.id)||content=</t>
@@ -245,7 +242,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -620,23 +616,23 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L2" sqref="L2:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="43.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="80.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="47.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="31.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="108.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.42578125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="108.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -694,17 +690,12 @@
         <v>0</v>
       </c>
       <c r="F2"/>
-      <c r="G2"/>
       <c r="H2"/>
-      <c r="I2"/>
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45">
@@ -737,9 +728,6 @@
       <c r="K3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L3" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
@@ -769,9 +757,6 @@
         <v>69</v>
       </c>
       <c r="K4" s="6"/>
-      <c r="L4" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="90">
       <c r="A5" t="s">
@@ -803,9 +788,6 @@
       <c r="K5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L5" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" t="s">
@@ -833,9 +815,6 @@
       <c r="I6" s="1"/>
       <c r="J6" s="4"/>
       <c r="K6" s="6"/>
-      <c r="L6" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
@@ -854,15 +833,9 @@
         <v>0</v>
       </c>
       <c r="F7"/>
-      <c r="G7"/>
       <c r="H7"/>
-      <c r="I7"/>
       <c r="J7" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
@@ -884,7 +857,6 @@
       <c r="F8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G8"/>
       <c r="H8" s="5" t="s">
         <v>28</v>
       </c>
@@ -893,10 +865,6 @@
       </c>
       <c r="J8" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
@@ -918,7 +886,6 @@
       <c r="F9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G9"/>
       <c r="H9" s="5" t="s">
         <v>29</v>
       </c>
@@ -927,10 +894,6 @@
       </c>
       <c r="J9" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
@@ -952,7 +915,6 @@
       <c r="F10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G10"/>
       <c r="H10" s="5" t="s">
         <v>32</v>
       </c>
@@ -961,10 +923,6 @@
       </c>
       <c r="J10" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
@@ -986,7 +944,6 @@
       <c r="F11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G11"/>
       <c r="H11"/>
       <c r="I11" t="s">
         <v>15</v>
@@ -994,10 +951,6 @@
       <c r="J11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
@@ -1010,7 +963,7 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -1018,16 +971,11 @@
       <c r="F12" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G12"/>
       <c r="H12"/>
       <c r="I12" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1061,9 +1009,6 @@
       <c r="K13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L13" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
@@ -1076,7 +1021,7 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -1084,17 +1029,12 @@
       <c r="F14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G14"/>
       <c r="H14"/>
       <c r="I14" t="s">
         <v>48</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K14"/>
-      <c r="L14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
@@ -1116,7 +1056,6 @@
       <c r="F15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G15"/>
       <c r="H15"/>
       <c r="I15" t="s">
         <v>47</v>
@@ -1124,10 +1063,6 @@
       <c r="J15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K15"/>
-      <c r="L15" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="16" spans="1:12" ht="45">
       <c r="A16" t="s">
@@ -1148,7 +1083,6 @@
       <c r="F16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G16"/>
       <c r="H16" s="5" t="s">
         <v>28</v>
       </c>
@@ -1157,10 +1091,6 @@
       </c>
       <c r="J16" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="K16"/>
-      <c r="L16" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Abstractbase class Implemented Sesion Eviction API automation Modified Authoring test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="153">
   <si>
     <t>GET</t>
   </si>
@@ -410,13 +410,76 @@
   </si>
   <si>
     <t>status=200||found=true||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T3_comments.id)</t>
+  </si>
+  <si>
+    <t>Create comment for report testing</t>
+  </si>
+  <si>
+    <t>{"targetType":"TRRecord","targetId":"456539938WOS1","content":"Comment report tesintg"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Down a un reported Comment </t>
+  </si>
+  <si>
+    <t>{"report":"DOWN","reason":"Wrong comment"}</t>
+  </si>
+  <si>
+    <t>Report a Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {"report":"UP","reason":"RR001"}</t>
+  </si>
+  <si>
+    <t>Report a Comment to admin</t>
+  </si>
+  <si>
+    <t>{"adminAction":"DENIED","adminNote":"Test report to admin","override":"false"}</t>
+  </si>
+  <si>
+    <t>Report a deleted Comment</t>
+  </si>
+  <si>
+    <t>{"report":"UP","reason":"Wrong comment"}</t>
+  </si>
+  <si>
+    <t>S1_TC_T34</t>
+  </si>
+  <si>
+    <t>S1_TC_T35</t>
+  </si>
+  <si>
+    <t>S1_TC_T36</t>
+  </si>
+  <si>
+    <t>S1_TC_T37</t>
+  </si>
+  <si>
+    <t>S1_TC_T38</t>
+  </si>
+  <si>
+    <t>S1_TC_T39</t>
+  </si>
+  <si>
+    <t>/report/Comment/(S1_TC_T33_comments.id)</t>
+  </si>
+  <si>
+    <t>/administration/report/Comment/(S1_TC_T33_comments.id)</t>
+  </si>
+  <si>
+    <t>/comments/comment/(S1_TC_T33_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=Comment||targetId=(S1_TC_T33_comments.id)||hasReported=UP||reportCount=1</t>
+  </si>
+  <si>
+    <t>status=200||targetType=Comment||targetId=(S1_TC_T33_comments.id)||hasSucceeded=true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +494,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -474,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -493,6 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G25" workbookViewId="0">
-      <selection activeCell="L34" sqref="L2:L34"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -802,7 +872,7 @@
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="47.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="68.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="119.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -897,7 +967,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -928,7 +998,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -957,7 +1027,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="90">
+    <row r="6" spans="1:12" ht="45">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -988,7 +1058,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45">
+    <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1017,7 +1087,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="45">
+    <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1046,7 +1116,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="45">
+    <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1151,7 +1221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45">
+    <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1177,7 +1247,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45">
+    <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1368,7 +1438,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="60">
+    <row r="21" spans="1:11" ht="30">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -1453,7 +1523,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="45">
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -1681,46 +1751,208 @@
         <v>119</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
         <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="E33" t="s">
         <v>0</v>
       </c>
-      <c r="F33"/>
+      <c r="F33" s="7"/>
       <c r="H33"/>
       <c r="J33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="30">
       <c r="A34" t="s">
         <v>128</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
         <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
-      </c>
-      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="6"/>
+      <c r="H34" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="30">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" t="s">
+        <v>135</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="30">
+      <c r="A36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" t="s">
+        <v>137</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="30">
+      <c r="A38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38"/>
+      <c r="I38" t="s">
+        <v>128</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="30">
+      <c r="A39" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" t="s">
         <v>0</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="H34"/>
-      <c r="J34" s="1" t="s">
-        <v>131</v>
+      <c r="F40"/>
+      <c r="H40"/>
+      <c r="J40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding dependency test cases for authoring Changed validations for Type a head Remove validations for search
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="153">
   <si>
     <t>GET</t>
   </si>
@@ -1821,6 +1821,9 @@
       <c r="H35" t="s">
         <v>135</v>
       </c>
+      <c r="I35" t="s">
+        <v>128</v>
+      </c>
       <c r="J35" s="4" t="s">
         <v>57</v>
       </c>
@@ -1847,6 +1850,9 @@
       <c r="H36" t="s">
         <v>137</v>
       </c>
+      <c r="I36" t="s">
+        <v>128</v>
+      </c>
       <c r="J36" s="4" t="s">
         <v>151</v>
       </c>
@@ -1872,6 +1878,9 @@
       </c>
       <c r="H37" s="8" t="s">
         <v>139</v>
+      </c>
+      <c r="I37" t="s">
+        <v>128</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
Added test cases for posts in authoring Changed validations in follow,notify,profile Added new validation in AbstractBase.java
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="216">
   <si>
     <t>GET</t>
   </si>
@@ -274,12 +274,6 @@
     <t>status=200||hasAppreciated=DOWN||targetType=Comment||appreciateCount=0||targetId=(S1_TC_T3_comments.id)</t>
   </si>
   <si>
-    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T3_comments.id)||content=</t>
-  </si>
-  <si>
-    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T5_comments.id)||content=</t>
-  </si>
-  <si>
     <t>S1_TC_T21</t>
   </si>
   <si>
@@ -394,9 +388,6 @@
     <t>/comments/user/(SYS_USER1)(S1_TC_T9_counterValue)</t>
   </si>
   <si>
-    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T20_comments.id)||content=</t>
-  </si>
-  <si>
     <t>Create comment  by passing wrong  data and testing error status</t>
   </si>
   <si>
@@ -473,12 +464,211 @@
   </si>
   <si>
     <t>status=200||targetType=Comment||targetId=(S1_TC_T33_comments.id)||hasSucceeded=true</t>
+  </si>
+  <si>
+    <t>S1_TC_T40</t>
+  </si>
+  <si>
+    <t>Create a new Post</t>
+  </si>
+  <si>
+    <t>/posts/</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||found=true</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>S1_TC_T41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create post and validate API is allowing to add or not with in 60 sec </t>
+  </si>
+  <si>
+    <t>{"title":"API Test7","content":"Post content creation from API Automation Script6"}</t>
+  </si>
+  <si>
+    <t>S1_TC_T42</t>
+  </si>
+  <si>
+    <t>Get post details by post id</t>
+  </si>
+  <si>
+    <t>/posts/post/(S1_TC_T40_id)</t>
+  </si>
+  <si>
+    <t>status=200||id=(S1_TC_T40_id)||found=true</t>
+  </si>
+  <si>
+    <t>S1_TC_T43</t>
+  </si>
+  <si>
+    <t>Get post details by post id in query string</t>
+  </si>
+  <si>
+    <t>/posts/post</t>
+  </si>
+  <si>
+    <t>?id=(S1_TC_T40_id)</t>
+  </si>
+  <si>
+    <t>S1_TC_T44</t>
+  </si>
+  <si>
+    <t>Get all posts by user id</t>
+  </si>
+  <si>
+    <t>/posts/user/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>status=200||posts[0].id=(S1_TC_T40_id)||found=true</t>
+  </si>
+  <si>
+    <t>S1_TC_T45</t>
+  </si>
+  <si>
+    <t>Get post statistics</t>
+  </si>
+  <si>
+    <t>/statistics/Post</t>
+  </si>
+  <si>
+    <t>status=200||targetId=(S1_TC_T40_id)||targetType=Post</t>
+  </si>
+  <si>
+    <t>S1_TC_T46</t>
+  </si>
+  <si>
+    <t>Check posts count for the given User ID</t>
+  </si>
+  <si>
+    <t>/posts/count/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>S1_TC_T47</t>
+  </si>
+  <si>
+    <t>Edit a post</t>
+  </si>
+  <si>
+    <t>{"title":"API Edit Test","content":"Edit Post content from API Automation Script"}</t>
+  </si>
+  <si>
+    <t>S1_TC_T48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete a post </t>
+  </si>
+  <si>
+    <t>S1_TC_T49</t>
+  </si>
+  <si>
+    <t>Get post details for invalid post id and Check the error status</t>
+  </si>
+  <si>
+    <t>/posts/post/(S1_TC_T40_id)a</t>
+  </si>
+  <si>
+    <t>S1_TC_T50</t>
+  </si>
+  <si>
+    <t>Create a new Post with less parameters and check the error status</t>
+  </si>
+  <si>
+    <t>{"title":"API Test 8"}</t>
+  </si>
+  <si>
+    <t>S1_TC_T51</t>
+  </si>
+  <si>
+    <t>Get all published posts by user id</t>
+  </si>
+  <si>
+    <t>?status=PUBLISHED</t>
+  </si>
+  <si>
+    <t>S1_TC_T52</t>
+  </si>
+  <si>
+    <t>Appreciate a Post</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/Post/(S1_TC_T40_id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Post||appreciateCount=1||targetId=(S1_TC_T40_id)</t>
+  </si>
+  <si>
+    <t>S1_TC_T53</t>
+  </si>
+  <si>
+    <t>Appreciate a Post with wrong data and testing error status</t>
+  </si>
+  <si>
+    <t>S1_TC_T54</t>
+  </si>
+  <si>
+    <t>Appreciate non existing Post and testing error status</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/Post/(S1_TC_T40_id)a</t>
+  </si>
+  <si>
+    <t>S1_TC_T55</t>
+  </si>
+  <si>
+    <t>Un appreciate a Post</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=DOWN||targetType=Post||appreciateCount=0||targetId=(S1_TC_T40_id)</t>
+  </si>
+  <si>
+    <t>S1_TC_T56</t>
+  </si>
+  <si>
+    <t>View all posts without content for the User ID</t>
+  </si>
+  <si>
+    <t>?includeContent=false</t>
+  </si>
+  <si>
+    <t>status=200||posts[0].id=(S1_TC_T40_id)||found=true||posts[0].content=""</t>
+  </si>
+  <si>
+    <t>S1_TC_T57</t>
+  </si>
+  <si>
+    <t>View the post details without content for the Post ID</t>
+  </si>
+  <si>
+    <t>status=200||id=(S1_TC_T40_id)||found=true||content=''</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T3_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T5_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>status=200||targetType=TRRecord||targetId=456539938WOS1||id=(S1_TC_T20_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>{"title":"API Test 20","content":"Post content creation from API Automation Script"}</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -857,26 +1047,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L40"/>
+    <sheetView tabSelected="1" topLeftCell="E24" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.42578125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="68.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="119.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="43.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="80.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="47.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="5" width="68.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="119.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -934,12 +1124,17 @@
         <v>0</v>
       </c>
       <c r="F2"/>
+      <c r="G2"/>
       <c r="H2"/>
+      <c r="I2"/>
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -963,8 +1158,13 @@
         <v>64</v>
       </c>
       <c r="H3"/>
+      <c r="I3"/>
       <c r="J3" t="s">
         <v>65</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
@@ -997,6 +1197,9 @@
       <c r="K4" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="L4" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
@@ -1026,6 +1229,9 @@
         <v>62</v>
       </c>
       <c r="K5" s="6"/>
+      <c r="L5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" t="s">
@@ -1057,13 +1263,16 @@
       <c r="K6" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="L6" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -1075,7 +1284,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="4" t="s">
@@ -1083,9 +1292,12 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K7" s="6"/>
+      <c r="L7" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
@@ -1112,16 +1324,19 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K8" s="6"/>
+      <c r="L8" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -1137,37 +1352,45 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K9" s="6"/>
+      <c r="L9" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
       <c r="F10"/>
+      <c r="G10"/>
       <c r="H10"/>
+      <c r="I10"/>
       <c r="J10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>54</v>
+      </c>
+      <c r="L10" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1187,9 +1410,15 @@
         <v>0</v>
       </c>
       <c r="F11"/>
+      <c r="G11"/>
       <c r="H11"/>
+      <c r="I11"/>
       <c r="J11" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
@@ -1211,6 +1440,7 @@
       <c r="F12" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G12"/>
       <c r="H12" s="5" t="s">
         <v>32</v>
       </c>
@@ -1219,6 +1449,10 @@
       </c>
       <c r="J12" s="1" t="s">
         <v>57</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
@@ -1226,13 +1460,13 @@
         <v>48</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1240,11 +1474,17 @@
       <c r="F13" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G13"/>
       <c r="H13" s="5" t="s">
-        <v>100</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="I13"/>
       <c r="J13" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
@@ -1266,6 +1506,7 @@
       <c r="F14" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G14"/>
       <c r="H14" s="5" t="s">
         <v>28</v>
       </c>
@@ -1274,6 +1515,10 @@
       </c>
       <c r="J14" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="K14"/>
+      <c r="L14" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
@@ -1295,6 +1540,7 @@
       <c r="F15" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G15"/>
       <c r="H15" s="5" t="s">
         <v>29</v>
       </c>
@@ -1303,6 +1549,10 @@
       </c>
       <c r="J15" s="1" t="s">
         <v>72</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
@@ -1310,7 +1560,7 @@
         <v>61</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1322,13 +1572,19 @@
         <v>25</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>95</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="G16"/>
       <c r="H16" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="I16"/>
       <c r="J16" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1350,9 +1606,15 @@
       <c r="F17" t="s">
         <v>68</v>
       </c>
+      <c r="G17"/>
       <c r="H17"/>
+      <c r="I17"/>
       <c r="J17" t="s">
         <v>73</v>
+      </c>
+      <c r="K17"/>
+      <c r="L17" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
@@ -1374,6 +1636,7 @@
       <c r="F18" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G18"/>
       <c r="H18" s="5" t="s">
         <v>32</v>
       </c>
@@ -1382,6 +1645,10 @@
       </c>
       <c r="J18" s="1" t="s">
         <v>85</v>
+      </c>
+      <c r="K18"/>
+      <c r="L18" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30">
@@ -1403,12 +1670,17 @@
       <c r="F19" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G19"/>
       <c r="H19"/>
       <c r="I19" t="s">
         <v>16</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>86</v>
+        <v>210</v>
+      </c>
+      <c r="K19"/>
+      <c r="L19" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="30">
@@ -1430,12 +1702,17 @@
       <c r="F20" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="G20"/>
       <c r="H20"/>
       <c r="I20" t="s">
         <v>18</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>87</v>
+        <v>211</v>
+      </c>
+      <c r="K20"/>
+      <c r="L20" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30">
@@ -1468,10 +1745,13 @@
       <c r="K21" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="L21" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>21</v>
@@ -1480,7 +1760,7 @@
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
@@ -1488,17 +1768,22 @@
       <c r="F22" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G22"/>
       <c r="H22"/>
       <c r="I22" t="s">
         <v>82</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>126</v>
+        <v>212</v>
+      </c>
+      <c r="K22"/>
+      <c r="L22" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>56</v>
@@ -1515,6 +1800,7 @@
       <c r="F23" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G23"/>
       <c r="H23"/>
       <c r="I23" t="s">
         <v>79</v>
@@ -1522,10 +1808,14 @@
       <c r="J23" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="K23"/>
+      <c r="L23" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>59</v>
@@ -1542,6 +1832,7 @@
       <c r="F24" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G24"/>
       <c r="H24" s="5" t="s">
         <v>28</v>
       </c>
@@ -1551,10 +1842,14 @@
       <c r="J24" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="K24"/>
+      <c r="L24" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="30">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>83</v>
@@ -1571,6 +1866,7 @@
       <c r="F25" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G25"/>
       <c r="H25" s="5" t="s">
         <v>29</v>
       </c>
@@ -1580,10 +1876,14 @@
       <c r="J25" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="K25"/>
+      <c r="L25" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>84</v>
@@ -1600,6 +1900,7 @@
       <c r="F26" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G26"/>
       <c r="H26" s="5" t="s">
         <v>32</v>
       </c>
@@ -1609,171 +1910,215 @@
       <c r="J26" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="K26"/>
+      <c r="L26" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="30">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E27" t="s">
         <v>0</v>
       </c>
       <c r="F27"/>
+      <c r="G27"/>
       <c r="H27"/>
+      <c r="I27"/>
       <c r="J27" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K27" s="6"/>
+      <c r="L27" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E28" t="s">
         <v>0</v>
       </c>
       <c r="F28"/>
+      <c r="G28"/>
       <c r="H28"/>
+      <c r="I28"/>
       <c r="J28" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="K28"/>
+      <c r="L28" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="30">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
         <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E29" t="s">
         <v>0</v>
       </c>
       <c r="F29"/>
+      <c r="G29"/>
       <c r="H29"/>
+      <c r="I29"/>
       <c r="J29" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="K29"/>
+      <c r="L29" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="30">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
         <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E30" t="s">
         <v>0</v>
       </c>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H30"/>
+      <c r="I30"/>
       <c r="J30" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="K30"/>
+      <c r="L30" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
         <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E31" t="s">
         <v>0</v>
       </c>
       <c r="F31"/>
+      <c r="G31"/>
       <c r="H31"/>
+      <c r="I31"/>
       <c r="J31" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="K31"/>
+      <c r="L31" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
         <v>0</v>
       </c>
       <c r="F32"/>
+      <c r="G32"/>
       <c r="H32"/>
+      <c r="I32"/>
       <c r="J32" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="K32"/>
+      <c r="L32" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
         <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E33" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="7"/>
+      <c r="G33"/>
       <c r="H33"/>
+      <c r="I33"/>
       <c r="J33" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="K33"/>
+      <c r="L33" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="30">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
         <v>22</v>
@@ -1789,28 +2134,31 @@
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="I34" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="I34"/>
       <c r="J34" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="L34" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="30">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
         <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>25</v>
@@ -1818,28 +2166,33 @@
       <c r="F35" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="G35"/>
       <c r="H35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="K35"/>
+      <c r="L35" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="30">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
         <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>25</v>
@@ -1847,28 +2200,33 @@
       <c r="F36" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="G36"/>
       <c r="H36" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I36" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
+      </c>
+      <c r="K36"/>
+      <c r="L36" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C37" t="s">
         <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>25</v>
@@ -1876,19 +2234,24 @@
       <c r="F37" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="G37"/>
       <c r="H37" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="K37"/>
+      <c r="L37" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="30">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>21</v>
@@ -1897,7 +2260,7 @@
         <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E38" t="s">
         <v>33</v>
@@ -1905,26 +2268,31 @@
       <c r="F38" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="G38"/>
       <c r="H38"/>
       <c r="I38" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="K38"/>
+      <c r="L38" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="30">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C39" t="s">
         <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>25</v>
@@ -1932,16 +2300,24 @@
       <c r="F39" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="G39"/>
       <c r="H39" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="I39" t="s">
+        <v>125</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="K39"/>
+      <c r="L39" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>37</v>
@@ -1956,12 +2332,597 @@
         <v>0</v>
       </c>
       <c r="F40"/>
+      <c r="G40"/>
       <c r="H40"/>
+      <c r="I40"/>
       <c r="J40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K40" s="6" t="s">
         <v>54</v>
+      </c>
+      <c r="L40" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="30">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41"/>
+      <c r="H41" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="I41"/>
+      <c r="J41" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="L41" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30">
+      <c r="A42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="6"/>
+      <c r="H42" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K42" s="6"/>
+      <c r="L42" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>160</v>
+      </c>
+      <c r="E43" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43" t="s">
+        <v>150</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K43"/>
+      <c r="L43" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44"/>
+      <c r="G44" t="s">
+        <v>165</v>
+      </c>
+      <c r="H44"/>
+      <c r="I44" t="s">
+        <v>150</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K44"/>
+      <c r="L44" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45" t="s">
+        <v>150</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K45"/>
+      <c r="L45" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>172</v>
+      </c>
+      <c r="E46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46"/>
+      <c r="G46" t="s">
+        <v>165</v>
+      </c>
+      <c r="H46"/>
+      <c r="I46" t="s">
+        <v>150</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="K46"/>
+      <c r="L46" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>174</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" t="s">
+        <v>176</v>
+      </c>
+      <c r="E47" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47" t="s">
+        <v>150</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L47" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="30">
+      <c r="A48" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>160</v>
+      </c>
+      <c r="E48" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48"/>
+      <c r="H48" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I48" t="s">
+        <v>150</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K48"/>
+      <c r="L48" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>160</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49" t="s">
+        <v>150</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K49"/>
+      <c r="L49" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="30">
+      <c r="A50" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>184</v>
+      </c>
+      <c r="E50" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50" t="s">
+        <v>150</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K50"/>
+      <c r="L50" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="30">
+      <c r="A51" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>152</v>
+      </c>
+      <c r="E51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51"/>
+      <c r="H51" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I51"/>
+      <c r="J51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K51" s="6"/>
+      <c r="L51" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E52" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52"/>
+      <c r="G52" t="s">
+        <v>190</v>
+      </c>
+      <c r="H52"/>
+      <c r="I52" t="s">
+        <v>150</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K52"/>
+      <c r="L52" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="30">
+      <c r="A53" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" t="s">
+        <v>193</v>
+      </c>
+      <c r="E53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53"/>
+      <c r="H53" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I53" t="s">
+        <v>150</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K53"/>
+      <c r="L53" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="30">
+      <c r="A54" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" t="s">
+        <v>193</v>
+      </c>
+      <c r="E54" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54"/>
+      <c r="H54" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I54"/>
+      <c r="J54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K54"/>
+      <c r="L54" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="30">
+      <c r="A55" t="s">
+        <v>197</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" t="s">
+        <v>199</v>
+      </c>
+      <c r="E55" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G55"/>
+      <c r="H55" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I55" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K55"/>
+      <c r="L55" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="30">
+      <c r="A56" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" t="s">
+        <v>193</v>
+      </c>
+      <c r="E56" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56"/>
+      <c r="H56" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I56" t="s">
+        <v>150</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K56"/>
+      <c r="L56" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57"/>
+      <c r="G57" t="s">
+        <v>205</v>
+      </c>
+      <c r="H57"/>
+      <c r="I57" t="s">
+        <v>150</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="K57"/>
+      <c r="L57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="30">
+      <c r="A58" t="s">
+        <v>207</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>160</v>
+      </c>
+      <c r="E58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58"/>
+      <c r="G58" t="s">
+        <v>205</v>
+      </c>
+      <c r="H58"/>
+      <c r="I58" t="s">
+        <v>150</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K58"/>
+      <c r="L58" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test cases for Authoring and WatchList
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -3854,7 +3854,7 @@
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="3" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="J82" s="5" t="s">
         <v>291</v>
@@ -3884,7 +3884,7 @@
         <v>293</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="J83" s="5" t="s">
         <v>25</v>
@@ -3942,7 +3942,7 @@
         <v>17</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>25</v>
@@ -3972,7 +3972,7 @@
         <v>18</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Updated test cases for Authoring
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="315">
   <si>
     <t>GET</t>
   </si>
@@ -145,18 +145,12 @@
     <t>/posts/count/(SYS_USER1)</t>
   </si>
   <si>
-    <t>{"title":"API Test 8"}</t>
-  </si>
-  <si>
     <t>?status=PUBLISHED</t>
   </si>
   <si>
     <t>?includeContent=false</t>
   </si>
   <si>
-    <t>{"title":"API Test 20","content":"Post content creation from API Automation Script"}</t>
-  </si>
-  <si>
     <t>Verify that prevention of comment flooding by bots with same article as well as different articles works as expected</t>
   </si>
   <si>
@@ -271,15 +265,9 @@
     <t>Verify that user is able to add comments on the posts of others.</t>
   </si>
   <si>
-    <t>{"content":"This is a Edited Post by API Authorized User", "title":"API Test title"}</t>
-  </si>
-  <si>
     <t>Verify that the post shows as updated when the user edits and updates the post</t>
   </si>
   <si>
-    <t>{"content":"This is a Edited Post by API Authorized User - For updated time test", "title":"API Test title"}</t>
-  </si>
-  <si>
     <t>Verify that user is able to view the "comment counts" on posts authored by themselves</t>
   </si>
   <si>
@@ -295,9 +283,6 @@
     <t>Verify that user is able to view the "Appreciation counts" on posts created by others</t>
   </si>
   <si>
-    <t>{"title":"API Edited Title","content":"Edit Post content from API Automation Script"}</t>
-  </si>
-  <si>
     <t>{"adminAction":"REMOVED","adminNote":"Test API from POSTMAN","override":"true"}</t>
   </si>
   <si>
@@ -448,454 +433,433 @@
     <t>OPQA-286_3</t>
   </si>
   <si>
+    <t>OPQA-245</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-245_comments.id)</t>
+  </si>
+  <si>
+    <t>Verify  that user can add allowed html tags while editing the comments</t>
+  </si>
+  <si>
+    <t>OPQA-247</t>
+  </si>
+  <si>
+    <t>Verify that delete a deleted comment works as expected</t>
+  </si>
+  <si>
+    <t>OPQA-337</t>
+  </si>
+  <si>
+    <t>Verify that modify a deleted comment works as expected</t>
+  </si>
+  <si>
+    <t>OPQA-338</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to appreciate a deleted comment</t>
+  </si>
+  <si>
+    <t>OPQA-339</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to un-appreciate a deleted comment</t>
+  </si>
+  <si>
+    <t>OPQA-340</t>
+  </si>
+  <si>
+    <t>Verify that comments count by passing wrong data and testing error status works as expected</t>
+  </si>
+  <si>
+    <t>OPQA-343</t>
+  </si>
+  <si>
+    <t>OPQA-253</t>
+  </si>
+  <si>
+    <t>Verify that comments count by passing wrong userid and testing error status works as expected</t>
+  </si>
+  <si>
+    <t>OPQA-347</t>
+  </si>
+  <si>
+    <t>Verify that comment by passing wrong comment id and testing error status works as expected</t>
+  </si>
+  <si>
+    <t>OPQA-349</t>
+  </si>
+  <si>
+    <t>Verify that comments count by passing wrong user and testing  error status works as expected</t>
+  </si>
+  <si>
+    <t>OPQA-351</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-236_comments.id)(OPQA-331_counterValue)</t>
+  </si>
+  <si>
+    <t>/comments/count/(SYS_USER1)(OPQA-331_counterValue)</t>
+  </si>
+  <si>
+    <t>/comments/comment?id=(OPQA-236_comments.id)(OPQA-331_counterValue)</t>
+  </si>
+  <si>
+    <t>/comments/user/(SYS_USER1)(OPQA-331_counterValue)</t>
+  </si>
+  <si>
+    <t>Verify that get comment by passing comment id works as expected</t>
+  </si>
+  <si>
+    <t>OPQA-352</t>
+  </si>
+  <si>
+    <t>OPQA-236_1</t>
+  </si>
+  <si>
+    <t>/report/Comment/(OPQA-236_1_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=Comment||targetId=(OPQA-236_1_comments.id)||hasReported=UP||reportCount=1</t>
+  </si>
+  <si>
+    <t>/administration/report/Comment/(OPQA-236_1_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=Comment||targetId=(OPQA-236_1_comments.id)||hasSucceeded=true</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-236_1_comments.id)</t>
+  </si>
+  <si>
+    <t>Verify that down a un reported Comment works as expected</t>
+  </si>
+  <si>
+    <t>OPQA-354</t>
+  </si>
+  <si>
+    <t>OPQA-722</t>
+  </si>
+  <si>
+    <t>OPQA-722_1</t>
+  </si>
+  <si>
+    <t>OPQA-723</t>
+  </si>
+  <si>
+    <t>OPQA-723_1</t>
+  </si>
+  <si>
+    <t>OPQA-680</t>
+  </si>
+  <si>
+    <t>OPQA-360</t>
+  </si>
+  <si>
+    <t>status=200||posts[0].id=(OPQA-360_id)||found=true</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-360_id)||found=true</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||id=(OPQA-360_id)||content=This is a Edited Post by API Authorized User</t>
+  </si>
+  <si>
+    <t>status=200||posts[0].id=(OPQA-360_id)||found=true||posts[0].content=""</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-360_id)||found=true||content=''</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>OPQA-360_1</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-360_1_id)</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-360_1_id)</t>
+  </si>
+  <si>
+    <t>OPQA-481</t>
+  </si>
+  <si>
+    <t>OPQA-482</t>
+  </si>
+  <si>
+    <t>OPQA-483</t>
+  </si>
+  <si>
+    <t>OPQA-484</t>
+  </si>
+  <si>
+    <t>OPQA-485</t>
+  </si>
+  <si>
+    <t>OPQA-486</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to edit the title of the post a user authored themselves</t>
+  </si>
+  <si>
+    <t>OPQA-382</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to edit the content of the post a user authored themselves</t>
+  </si>
+  <si>
+    <t>OPQA-388</t>
+  </si>
+  <si>
+    <t>OPQA-406</t>
+  </si>
+  <si>
+    <t>OPQA-377</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/Comment/(OPQA-377_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(OPQA-377_comments.id)</t>
+  </si>
+  <si>
+    <t>/report/Comment/(OPQA-377_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=Comment||targetId=(OPQA-377_comments.id)||hasSucceeded=true</t>
+  </si>
+  <si>
+    <t>status=200||targetType=Comment||targetId=(OPQA-377_comments.id)||hasReported=UP||reportCount=1</t>
+  </si>
+  <si>
+    <t>/administration/report/Comment/(OPQA-377_comments.id)</t>
+  </si>
+  <si>
+    <t>OPQA-385</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/Comment/(OPQA-385_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(OPQA-385_comments.id)</t>
+  </si>
+  <si>
+    <t>OPQA-379</t>
+  </si>
+  <si>
+    <t>OPQA-342</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to appreciate own Comments on the post</t>
+  </si>
+  <si>
+    <t>OPQA-714</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to appreciate the Comments of other users on the post</t>
+  </si>
+  <si>
+    <t>OPQA-364</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to un-appreciate the posts of others</t>
+  </si>
+  <si>
+    <t>OPQA-359</t>
+  </si>
+  <si>
+    <t>OPQA-488</t>
+  </si>
+  <si>
+    <t>OPQA-681</t>
+  </si>
+  <si>
+    <t>OPQA-489</t>
+  </si>
+  <si>
+    <t>OPQA-490</t>
+  </si>
+  <si>
+    <t>OPQA-491</t>
+  </si>
+  <si>
+    <t>OPQA-492</t>
+  </si>
+  <si>
+    <t>OPQA-493</t>
+  </si>
+  <si>
+    <t>OPQA-423</t>
+  </si>
+  <si>
+    <t>OPQA-424</t>
+  </si>
+  <si>
+    <t>OPQA-425</t>
+  </si>
+  <si>
+    <t>OPQA-426</t>
+  </si>
+  <si>
+    <t>OPQA-253_1</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/posts/(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/posts/(OPQA-360_1_id)</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/posts/(OPQA-360_id)a</t>
+  </si>
+  <si>
+    <t>/statistics/posts</t>
+  </si>
+  <si>
+    <t>?id=468387744WOS1</t>
+  </si>
+  <si>
+    <t>/comments/count/468387744WOS1/</t>
+  </si>
+  <si>
+    <t>/comments/count/468387744WOS1/wos</t>
+  </si>
+  <si>
+    <t>/statistics/wos</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"mohana.yalamarthi@thomsonreuters.com        http://thomsonreuters.com/en.html         +91 8197818719"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"FUCK"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=****</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=****</t>
+  </si>
+  <si>
+    <t>status=200||size=(OPQA-331_counterValue)||found=true||comments.targetType=wos||comments.targetId=468387744WOS1</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"233726479WOS1","content":"Testing Error status 500"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"hi"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Edited content"}</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-315_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"HTML content Test:: &lt;br&gt; Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt; &lt;br&gt; "}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=HTML content Test:: &lt;br&gt; Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt; &lt;br&gt;</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-245_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>/comments/468387744WOS1/wos</t>
+  </si>
+  <si>
+    <t>status=200||found=true||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Comment report tesintg"}</t>
+  </si>
+  <si>
+    <t>{"title":"Post Test 333 From API User2","content":"Post content creation from API Automation Script  by User2"}</t>
+  </si>
+  <si>
+    <t>{"title":"Post Test 222 From API User1","content":"Post content creation from API Automation Script by User1"}</t>
+  </si>
+  <si>
+    <t>{"title":"Edited Post Test 222 From API User1","content":"Edit Post content from API Automation Script"}</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-360_id)||found=true||userId=(SYS_USER1)||title=Edited Post Test 222 From API User1</t>
+  </si>
+  <si>
+    <t>{"content":"This is a Edited Post by API Authorized User", "title":"Edited Post Test 222 From API User1"}</t>
+  </si>
+  <si>
+    <t>{"content":"This is a Edited Post by API Authorized User by API User2 - For updated time test", "title":"Post Test 333 From API User2"}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||id=(OPQA-360_1_id)||content=This is a Edited Post by API Authorized User by API User2 - For updated time test</t>
+  </si>
+  <si>
     <t>OPQA-286_4</t>
   </si>
   <si>
-    <t>OPQA-245</t>
-  </si>
-  <si>
-    <t>/comments/comment/(OPQA-245_comments.id)</t>
-  </si>
-  <si>
-    <t>Verify  that user can add allowed html tags while editing the comments</t>
-  </si>
-  <si>
-    <t>OPQA-247</t>
-  </si>
-  <si>
-    <t>Verify that delete a deleted comment works as expected</t>
-  </si>
-  <si>
-    <t>OPQA-337</t>
-  </si>
-  <si>
-    <t>Verify that modify a deleted comment works as expected</t>
-  </si>
-  <si>
-    <t>OPQA-338</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to appreciate a deleted comment</t>
-  </si>
-  <si>
-    <t>OPQA-339</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to un-appreciate a deleted comment</t>
-  </si>
-  <si>
-    <t>OPQA-340</t>
-  </si>
-  <si>
-    <t>Verify that comments count by passing wrong data and testing error status works as expected</t>
-  </si>
-  <si>
-    <t>OPQA-343</t>
-  </si>
-  <si>
-    <t>OPQA-253</t>
-  </si>
-  <si>
-    <t>Verify that comments count by passing wrong userid and testing error status works as expected</t>
-  </si>
-  <si>
-    <t>OPQA-347</t>
-  </si>
-  <si>
-    <t>Verify that comment by passing wrong comment id and testing error status works as expected</t>
-  </si>
-  <si>
-    <t>OPQA-349</t>
-  </si>
-  <si>
-    <t>Verify that comments count by passing wrong user and testing  error status works as expected</t>
-  </si>
-  <si>
-    <t>OPQA-351</t>
-  </si>
-  <si>
-    <t>/comments/comment/(OPQA-236_comments.id)(OPQA-331_counterValue)</t>
-  </si>
-  <si>
-    <t>/comments/count/(SYS_USER1)(OPQA-331_counterValue)</t>
-  </si>
-  <si>
-    <t>/comments/comment?id=(OPQA-236_comments.id)(OPQA-331_counterValue)</t>
-  </si>
-  <si>
-    <t>/comments/user/(SYS_USER1)(OPQA-331_counterValue)</t>
-  </si>
-  <si>
-    <t>Verify that get comment by passing comment id works as expected</t>
-  </si>
-  <si>
-    <t>OPQA-352</t>
-  </si>
-  <si>
-    <t>OPQA-236_1</t>
-  </si>
-  <si>
-    <t>/report/Comment/(OPQA-236_1_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||targetType=Comment||targetId=(OPQA-236_1_comments.id)||hasReported=UP||reportCount=1</t>
-  </si>
-  <si>
-    <t>/administration/report/Comment/(OPQA-236_1_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||targetType=Comment||targetId=(OPQA-236_1_comments.id)||hasSucceeded=true</t>
-  </si>
-  <si>
-    <t>/comments/comment/(OPQA-236_1_comments.id)</t>
-  </si>
-  <si>
-    <t>Verify that down a un reported Comment works as expected</t>
-  </si>
-  <si>
-    <t>OPQA-354</t>
-  </si>
-  <si>
-    <t>OPQA-722</t>
-  </si>
-  <si>
-    <t>OPQA-722_1</t>
-  </si>
-  <si>
-    <t>OPQA-723</t>
-  </si>
-  <si>
-    <t>OPQA-723_1</t>
-  </si>
-  <si>
-    <t>OPQA-680</t>
-  </si>
-  <si>
-    <t>OPQA-360</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=Post||comments.targetId=(OPQA-360_id)||comments.content=Comment Test on Post</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=UP||targetType=Post||appreciateCount=1||targetId=(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>status=200||posts[0].id=(OPQA-360_id)||found=true</t>
-  </si>
-  <si>
-    <t>/posts/post/(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>status=200||id=(OPQA-360_id)||found=true</t>
-  </si>
-  <si>
-    <t>status=200||targetId=(OPQA-360_id)||targetType=Post</t>
-  </si>
-  <si>
-    <t>status=200||id=(OPQA-360_id)||found=true||userId=(SYS_USER1)||title=API Edited Title</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||id=(OPQA-360_id)||content=This is a Edited Post by API Authorized User</t>
-  </si>
-  <si>
-    <t>{"targetType":"Post","targetId":"(OPQA-360_id)","content":"Comment Test on Post"}</t>
-  </si>
-  <si>
-    <t>status=200||posts[0].id=(OPQA-360_id)||found=true||posts[0].content=""</t>
-  </si>
-  <si>
-    <t>/comments/count/(OPQA-360_id)/Post</t>
-  </si>
-  <si>
-    <t>status=200||id=(OPQA-360_id)||type=Post||counterName=commentCountForTarget||counterValue=1</t>
-  </si>
-  <si>
-    <t>status=200||id=(OPQA-360_id)||found=true||content=''</t>
-  </si>
-  <si>
-    <t>?id=(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>status=200||targetId=(OPQA-360_id)||targetType=Post||appreciateCount=1</t>
-  </si>
-  <si>
-    <t>OPQA-360_1</t>
-  </si>
-  <si>
-    <t>/posts/post/(OPQA-360_1_id)</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=Post||comments.targetId=(OPQA-360_1_id)||comments.content=Comment Test by User 2 on Post</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=DOWN||targetType=Post||appreciateCount=0||targetId=(OPQA-360_1_id)</t>
-  </si>
-  <si>
-    <t>/comments/count/(OPQA-360_1_id)/Post</t>
-  </si>
-  <si>
-    <t>status=200||targetId=(OPQA-360_1_id)||targetType=Post||appreciateCount=0</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER2)||id=(OPQA-360_1_id)||content=This is a Edited Post by API Authorized User - For updated time test</t>
-  </si>
-  <si>
-    <t>{"targetType":"Post","targetId":"(OPQA-360_1_id)","content":"Comment Test by User 2 on Post"}</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=UP||targetType=Post||appreciateCount=1||targetId=(OPQA-360_1_id)</t>
-  </si>
-  <si>
-    <t>status=200||id=(OPQA-360_1_id)||type=Post||counterName=commentCountForTarget||counterValue=1</t>
-  </si>
-  <si>
-    <t>?id=(OPQA-360_1_id)</t>
-  </si>
-  <si>
-    <t>OPQA-481</t>
-  </si>
-  <si>
-    <t>OPQA-482</t>
-  </si>
-  <si>
-    <t>OPQA-483</t>
-  </si>
-  <si>
-    <t>OPQA-484</t>
-  </si>
-  <si>
-    <t>OPQA-485</t>
-  </si>
-  <si>
-    <t>OPQA-486</t>
-  </si>
-  <si>
-    <t>Verify that the user is able to edit the title of the post a user authored themselves</t>
-  </si>
-  <si>
-    <t>OPQA-382</t>
-  </si>
-  <si>
-    <t>Verify that the user is able to edit the content of the post a user authored themselves</t>
-  </si>
-  <si>
-    <t>OPQA-388</t>
-  </si>
-  <si>
-    <t>OPQA-406</t>
-  </si>
-  <si>
-    <t>OPQA-377</t>
-  </si>
-  <si>
-    <t>/appreciation/appreciate/Comment/(OPQA-377_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(OPQA-377_comments.id)</t>
-  </si>
-  <si>
-    <t>/report/Comment/(OPQA-377_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||targetType=Comment||targetId=(OPQA-377_comments.id)||hasSucceeded=true</t>
-  </si>
-  <si>
-    <t>status=200||targetType=Comment||targetId=(OPQA-377_comments.id)||hasReported=UP||reportCount=1</t>
-  </si>
-  <si>
-    <t>/administration/report/Comment/(OPQA-377_comments.id)</t>
-  </si>
-  <si>
-    <t>OPQA-385</t>
-  </si>
-  <si>
-    <t>/appreciation/appreciate/Comment/(OPQA-385_comments.id)</t>
-  </si>
-  <si>
-    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(OPQA-385_comments.id)</t>
-  </si>
-  <si>
     <t>/comments/comment/(OPQA-385_comments.id)</t>
   </si>
   <si>
-    <t>OPQA-379</t>
-  </si>
-  <si>
-    <t>OPQA-342</t>
-  </si>
-  <si>
-    <t>Verify that the user is able to appreciate own Comments on the post</t>
-  </si>
-  <si>
-    <t>OPQA-714</t>
-  </si>
-  <si>
-    <t>Verify that the user is able to appreciate the Comments of other users on the post</t>
-  </si>
-  <si>
-    <t>OPQA-364</t>
-  </si>
-  <si>
-    <t>Verify that the user is able to un-appreciate the posts of others</t>
-  </si>
-  <si>
-    <t>OPQA-359</t>
-  </si>
-  <si>
-    <t>OPQA-488</t>
-  </si>
-  <si>
-    <t>OPQA-681</t>
-  </si>
-  <si>
-    <t>OPQA-489</t>
-  </si>
-  <si>
-    <t>OPQA-490</t>
-  </si>
-  <si>
-    <t>OPQA-491</t>
-  </si>
-  <si>
-    <t>OPQA-492</t>
-  </si>
-  <si>
-    <t>OPQA-493</t>
-  </si>
-  <si>
-    <t>OPQA-423</t>
-  </si>
-  <si>
-    <t>OPQA-424</t>
-  </si>
-  <si>
-    <t>OPQA-425</t>
-  </si>
-  <si>
-    <t>OPQA-426</t>
-  </si>
-  <si>
-    <t>OPQA-253_1</t>
-  </si>
-  <si>
-    <t>/appreciation/appreciate/posts/(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>/appreciation/appreciate/posts/(OPQA-360_1_id)</t>
-  </si>
-  <si>
-    <t>/appreciation/appreciate/posts/(OPQA-360_id)a</t>
-  </si>
-  <si>
-    <t>/statistics/posts</t>
+    <t>OPQA-776</t>
+  </si>
+  <si>
+    <t>Verify that the admin can delete any post as a moderator</t>
   </si>
   <si>
     <t>/administration/posts/(OPQA-360_id)</t>
   </si>
   <si>
-    <t>?id=468387744WOS1</t>
-  </si>
-  <si>
-    <t>/comments/count/468387744WOS1/</t>
-  </si>
-  <si>
-    <t>/comments/count/468387744WOS1/wos</t>
-  </si>
-  <si>
-    <t>/statistics/wos</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"hello"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=hello</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"mohana.yalamarthi@thomsonreuters.com        http://thomsonreuters.com/en.html         +91 8197818719"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"&lt;abcd&gt;Hello&lt;abcd&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Hello</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"&lt;abcd&gt;Testing&lt;abcd&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||content= Testing ||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"FUCK"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=****</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=****</t>
-  </si>
-  <si>
-    <t>status=200||size=(OPQA-331_counterValue)||found=true||comments.targetType=wos||comments.targetId=468387744WOS1</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"233726479WOS1","content":"Testing Error status 500"}</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"hi"}</t>
-  </si>
-  <si>
-    <t>status=200||content=hi||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Edited content"}</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-315_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"HTML content Test:: &lt;br&gt; Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt; &lt;br&gt; "}</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=HTML content Test:: &lt;br&gt; Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt; &lt;br&gt;</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-245_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>/comments/468387744WOS1/wos</t>
-  </si>
-  <si>
-    <t>status=200||found=true||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Comment report tesintg"}</t>
-  </si>
-  <si>
     <t>status=200||targetType=posts||targetId=(OPQA-360_id)||hasSucceeded=true</t>
   </si>
   <si>
+    <t>OPQA-777</t>
+  </si>
+  <si>
+    <t>Verify that mixed statistics are returned using API</t>
+  </si>
+  <si>
+    <t>/statistics/getByIds</t>
+  </si>
+  <si>
+    <t>?id=posts::(OPQA-360_id)&amp;id=User::(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-360_id)||id=(SYS_USER1)||type=User</t>
+  </si>
+  <si>
+    <t>OPQA-778</t>
+  </si>
+  <si>
     <t>Verify that user can't delete the deleted post and check the error status using API</t>
   </si>
   <si>
     <t>status=200||targetType=posts||targetId=(OPQA-360_id)||hasSucceeded=false||errorMsg=This post has already been deleted</t>
   </si>
   <si>
+    <t>OPQA-779</t>
+  </si>
+  <si>
     <t>Verify that user can't edit the deleted post and check the error status using API</t>
   </si>
   <si>
-    <t>{"content":"This is a Editing the deleted Post by API Authorized User", "title":"API Test title"}</t>
+    <t>OPQA-780</t>
   </si>
   <si>
     <t>Verify that user can't delete the invalid post and check the error status using API</t>
@@ -907,46 +871,94 @@
     <t>status=200||targetType=posts||targetId=(OPQA-360_id)||hasSucceeded=false||errorMsg=Exception encountered.  Please see the logs for a stack trace.</t>
   </si>
   <si>
+    <t>OPQA-781</t>
+  </si>
+  <si>
     <t>Verify that user can't appreciate the deleted post and check the error status using API</t>
   </si>
   <si>
+    <t>OPQA-782</t>
+  </si>
+  <si>
     <t>Verify that user can't Un-appreciate the deleted post and check the error status using API</t>
   </si>
   <si>
-    <t>Verify that mixed statistics are returned using API</t>
-  </si>
-  <si>
-    <t>?id=posts::(OPQA-360_id)&amp;id=User::(SYS_USER1)</t>
-  </si>
-  <si>
-    <t>status=200||targetType=posts||targetId=(OPQA-360_id)||id=(SYS_USER1)||type=User</t>
-  </si>
-  <si>
-    <t>/statistics/getByIds</t>
-  </si>
-  <si>
-    <t>OPQA-776</t>
-  </si>
-  <si>
-    <t>Verify that the admin can delete any post as a moderator</t>
-  </si>
-  <si>
-    <t>OPQA-777</t>
-  </si>
-  <si>
-    <t>OPQA-778</t>
-  </si>
-  <si>
-    <t>OPQA-779</t>
-  </si>
-  <si>
-    <t>OPQA-780</t>
-  </si>
-  <si>
-    <t>OPQA-781</t>
-  </si>
-  <si>
-    <t>OPQA-782</t>
+    <t>status=200||targetId=(OPQA-360_id)||targetType=posts</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=posts||appreciateCount=1||targetId=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=posts||appreciateCount=1||targetId=(OPQA-360_1_id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=DOWN||targetType=posts||appreciateCount=0||targetId=(OPQA-360_1_id)</t>
+  </si>
+  <si>
+    <t>status=200||targetId=(OPQA-360_id)||targetType=posts||appreciateCount=1</t>
+  </si>
+  <si>
+    <t>status=200||targetId=(OPQA-360_1_id)||targetType=posts||appreciateCount=0</t>
+  </si>
+  <si>
+    <t>/comments/count/(OPQA-360_1_id)/posts</t>
+  </si>
+  <si>
+    <t>/comments/count/(OPQA-360_id)/posts</t>
+  </si>
+  <si>
+    <t>{"title":"Post API Test  title without Content"}</t>
+  </si>
+  <si>
+    <t>{"content":"This is a Editing the deleted Post by API Authorized User1", "title":"API Edited Title222"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Comment test from API by User 1"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Comment test from API by User 1</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Comment test from API by User 1 and Created within 60 sec of previous comment"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Wrong data test : server error expectation"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while creating comment by User 1&lt;abcd&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Tags clean up surround tags like abcd while creating comment by User 1</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while editing comment by User 1&lt;abcd&gt;"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Update own comment"}</t>
+  </si>
+  <si>
+    <t>status=200||content=Update own comment||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||content= Tags clean up surround tags like abcd while editing comment by User 1||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-360_id)","content":"Comment Test on own Post:: Post Test 222 From API User1"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=posts||comments.targetId=(OPQA-360_id)||comments.content=Comment Test on own Post:: Post Test 222 From API User1</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-360_id)","content":"Comment Test by User 2 on others post: Post Test 222 From API User1"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=posts||comments.targetId=(OPQA-360_id)||comments.content=Comment Test by User 2 on others post: Post Test 222 From API User1</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-360_1_id)||type=posts||counterName=commentCountForTarget||counterValue=0</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-360_id)||type=posts||counterName=commentCountForTarget||counterValue=2</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L86"/>
     </sheetView>
   </sheetViews>
@@ -1410,16 +1422,16 @@
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A2" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>0</v>
@@ -1438,38 +1450,38 @@
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A3" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A4" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -1484,12 +1496,12 @@
         <v>21</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="4" t="s">
-        <v>263</v>
+      <c r="H4" s="5" t="s">
+        <v>299</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="5" t="s">
-        <v>264</v>
+        <v>300</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>20</v>
@@ -1498,10 +1510,10 @@
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A5" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -1516,8 +1528,8 @@
         <v>21</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="4" t="s">
-        <v>263</v>
+      <c r="H5" s="5" t="s">
+        <v>301</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="4" t="s">
@@ -1528,10 +1540,10 @@
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A6" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
@@ -1547,11 +1559,11 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="4" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="4" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>20</v>
@@ -1560,10 +1572,10 @@
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A7" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
@@ -1578,8 +1590,8 @@
         <v>28</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="4" t="s">
-        <v>263</v>
+      <c r="H7" s="5" t="s">
+        <v>302</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="4" t="s">
@@ -1588,12 +1600,12 @@
       <c r="K7" s="3"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A8" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
@@ -1608,28 +1620,28 @@
         <v>21</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>267</v>
+      <c r="H8" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="5" t="s">
-        <v>268</v>
+        <v>304</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A9" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>16</v>
@@ -1638,24 +1650,24 @@
         <v>21</v>
       </c>
       <c r="G9" s="8"/>
-      <c r="H9" s="4" t="s">
-        <v>269</v>
+      <c r="H9" s="5" t="s">
+        <v>305</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>270</v>
+        <v>308</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9"/>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A10" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
@@ -1671,27 +1683,27 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="4" t="s">
-        <v>272</v>
+        <v>242</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10"/>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A11" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
@@ -1701,23 +1713,23 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="4" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11"/>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A12" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
@@ -1742,10 +1754,10 @@
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A13" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
@@ -1761,23 +1773,23 @@
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A14" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>16</v>
@@ -1790,7 +1802,7 @@
         <v>18</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>25</v>
@@ -1800,16 +1812,16 @@
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A15" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
@@ -1819,7 +1831,7 @@
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="5" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="3" t="s">
@@ -1830,16 +1842,16 @@
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A16" s="8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>16</v>
@@ -1848,30 +1860,30 @@
         <v>21</v>
       </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="4" t="s">
-        <v>276</v>
+      <c r="H16" s="5" t="s">
+        <v>306</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>277</v>
+        <v>307</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16"/>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A17" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>16</v>
@@ -1881,10 +1893,10 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="4" t="s">
-        <v>278</v>
+        <v>247</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>29</v>
@@ -1894,16 +1906,16 @@
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>16</v>
@@ -1916,26 +1928,26 @@
         <v>17</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K18" s="8"/>
       <c r="L18"/>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A19" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>16</v>
@@ -1948,26 +1960,26 @@
         <v>17</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19"/>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A20" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>16</v>
@@ -1988,16 +2000,16 @@
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A21" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>0</v>
@@ -2009,23 +2021,23 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K21" s="8"/>
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A22" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>16</v>
@@ -2038,26 +2050,26 @@
         <v>18</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K22" s="8"/>
       <c r="L22"/>
     </row>
     <row r="23" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A23" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>16</v>
@@ -2070,26 +2082,26 @@
         <v>18</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="K23" s="8"/>
       <c r="L23"/>
     </row>
     <row r="24" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A24" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>19</v>
@@ -2100,7 +2112,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>29</v>
@@ -2110,16 +2122,16 @@
     </row>
     <row r="25" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A25" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>19</v>
@@ -2130,26 +2142,26 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="K25" s="8"/>
       <c r="L25"/>
     </row>
     <row r="26" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A26" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>19</v>
@@ -2160,20 +2172,20 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26"/>
     </row>
     <row r="27" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A27" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>14</v>
@@ -2189,11 +2201,11 @@
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="5" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="5" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>20</v>
@@ -2202,16 +2214,16 @@
     </row>
     <row r="28" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A28" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>16</v>
@@ -2221,29 +2233,29 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28"/>
     </row>
     <row r="29" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A29" s="8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>19</v>
@@ -2254,26 +2266,26 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="K29" s="8"/>
       <c r="L29"/>
     </row>
     <row r="30" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A30" s="8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>19</v>
@@ -2284,7 +2296,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>25</v>
@@ -2294,16 +2306,16 @@
     </row>
     <row r="31" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A31" s="8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>16</v>
@@ -2312,11 +2324,11 @@
         <v>21</v>
       </c>
       <c r="G31" s="8"/>
-      <c r="H31" s="4" t="s">
-        <v>276</v>
+      <c r="H31" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>25</v>
@@ -2326,16 +2338,16 @@
     </row>
     <row r="32" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A32" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>16</v>
@@ -2348,7 +2360,7 @@
         <v>17</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>25</v>
@@ -2358,16 +2370,16 @@
     </row>
     <row r="33" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A33" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>16</v>
@@ -2380,7 +2392,7 @@
         <v>18</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>25</v>
@@ -2390,16 +2402,16 @@
     </row>
     <row r="34" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A34" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>0</v>
@@ -2416,16 +2428,16 @@
     </row>
     <row r="35" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A35" s="8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
@@ -2442,16 +2454,16 @@
     </row>
     <row r="36" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A36" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>0</v>
@@ -2460,7 +2472,7 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>29</v>
@@ -2470,16 +2482,16 @@
     </row>
     <row r="37" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A37" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>0</v>
@@ -2490,7 +2502,7 @@
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>29</v>
@@ -2500,16 +2512,16 @@
     </row>
     <row r="38" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A38" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>0</v>
@@ -2518,7 +2530,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>29</v>
@@ -2528,16 +2540,16 @@
     </row>
     <row r="39" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A39" s="8" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>0</v>
@@ -2554,16 +2566,16 @@
     </row>
     <row r="40" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A40" s="8" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>0</v>
@@ -2572,20 +2584,20 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="K40" s="8"/>
       <c r="L40"/>
     </row>
     <row r="41" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A41" s="8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>14</v>
@@ -2601,7 +2613,7 @@
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="4" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="4" t="s">
@@ -2614,16 +2626,16 @@
     </row>
     <row r="42" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A42" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>16</v>
@@ -2636,7 +2648,7 @@
         <v>32</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>25</v>
@@ -2646,16 +2658,16 @@
     </row>
     <row r="43" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A43" s="8" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>16</v>
@@ -2668,26 +2680,26 @@
         <v>33</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K43" s="8"/>
       <c r="L43"/>
     </row>
     <row r="44" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A44" s="8" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>16</v>
@@ -2700,26 +2712,26 @@
         <v>34</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44"/>
     </row>
     <row r="45" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A45" s="8" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>19</v>
@@ -2730,7 +2742,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>11</v>
@@ -2740,16 +2752,16 @@
     </row>
     <row r="46" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A46" s="8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>16</v>
@@ -2762,7 +2774,7 @@
         <v>35</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>25</v>
@@ -2772,16 +2784,16 @@
     </row>
     <row r="47" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A47" s="8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>0</v>
@@ -2800,10 +2812,10 @@
     </row>
     <row r="48" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A48" s="8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>14</v>
@@ -2818,8 +2830,8 @@
         <v>21</v>
       </c>
       <c r="G48" s="8"/>
-      <c r="H48" s="4" t="s">
-        <v>46</v>
+      <c r="H48" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="4" t="s">
@@ -2832,10 +2844,10 @@
     </row>
     <row r="49" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A49" s="8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>14</v>
@@ -2851,11 +2863,11 @@
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="5" t="s">
-        <v>46</v>
+        <v>258</v>
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>38</v>
@@ -2864,10 +2876,10 @@
     </row>
     <row r="50" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A50" s="8" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>14</v>
@@ -2886,7 +2898,7 @@
         <v>39</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>26</v>
@@ -2896,16 +2908,16 @@
     </row>
     <row r="51" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A51" s="8" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>0</v>
@@ -2914,20 +2926,20 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="K51" s="8"/>
       <c r="L51"/>
     </row>
     <row r="52" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A52" s="8" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>14</v>
@@ -2940,24 +2952,24 @@
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="K52" s="8"/>
       <c r="L52"/>
     </row>
     <row r="53" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A53" s="8" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>14</v>
@@ -2972,50 +2984,50 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="K53" s="8"/>
       <c r="L53"/>
     </row>
     <row r="54" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A54" s="8" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>191</v>
+        <v>289</v>
       </c>
       <c r="K54" s="8"/>
       <c r="L54"/>
     </row>
     <row r="55" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A55" s="8" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>14</v>
@@ -3030,7 +3042,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>11</v>
@@ -3042,16 +3054,16 @@
     </row>
     <row r="56" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A56" s="8" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>16</v>
@@ -3061,29 +3073,29 @@
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="5" t="s">
-        <v>93</v>
+        <v>260</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>192</v>
+        <v>261</v>
       </c>
       <c r="K56" s="8"/>
       <c r="L56"/>
     </row>
     <row r="57" spans="1:12" ht="30">
       <c r="A57" s="8" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>16</v>
@@ -3093,28 +3105,28 @@
       </c>
       <c r="G57" s="8"/>
       <c r="H57" s="5" t="s">
-        <v>85</v>
+        <v>262</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="K57" s="8"/>
     </row>
     <row r="58" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A58" s="8" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>16</v>
@@ -3124,23 +3136,23 @@
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="5" t="s">
-        <v>87</v>
+        <v>263</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>207</v>
+        <v>264</v>
       </c>
       <c r="K58" s="8"/>
       <c r="L58"/>
     </row>
     <row r="59" spans="1:12" ht="30">
       <c r="A59" s="8" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>14</v>
@@ -3156,13 +3168,13 @@
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="5" t="s">
-        <v>194</v>
+        <v>309</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>186</v>
+        <v>310</v>
       </c>
       <c r="K59" s="3" t="s">
         <v>20</v>
@@ -3170,10 +3182,10 @@
     </row>
     <row r="60" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A60" s="8" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>14</v>
@@ -3189,13 +3201,13 @@
       </c>
       <c r="G60" s="8"/>
       <c r="H60" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="I60" s="8" t="s">
-        <v>201</v>
+        <v>311</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>203</v>
+        <v>312</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>20</v>
@@ -3204,16 +3216,16 @@
     </row>
     <row r="61" spans="1:12" ht="30">
       <c r="A61" s="8" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>16</v>
@@ -3226,25 +3238,25 @@
         <v>17</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>187</v>
+        <v>290</v>
       </c>
       <c r="K61" s="8"/>
     </row>
     <row r="62" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A62" s="8" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>16</v>
@@ -3257,26 +3269,26 @@
         <v>17</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J62" s="8" t="s">
-        <v>209</v>
+        <v>291</v>
       </c>
       <c r="K62" s="8"/>
       <c r="L62"/>
     </row>
     <row r="63" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A63" s="8" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>16</v>
@@ -3289,26 +3301,26 @@
         <v>17</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="J63" s="8" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
       <c r="K63" s="8"/>
       <c r="L63"/>
     </row>
     <row r="64" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A64" s="8" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>16</v>
@@ -3321,26 +3333,26 @@
         <v>17</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="J64" s="8" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="K64" s="8"/>
       <c r="L64"/>
     </row>
     <row r="65" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A65" s="8" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>16</v>
@@ -3353,20 +3365,20 @@
         <v>18</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J65" s="8" t="s">
-        <v>204</v>
+        <v>292</v>
       </c>
       <c r="K65" s="8"/>
       <c r="L65"/>
     </row>
     <row r="66" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A66" s="8" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>14</v>
@@ -3381,8 +3393,8 @@
         <v>21</v>
       </c>
       <c r="G66" s="8"/>
-      <c r="H66" s="4" t="s">
-        <v>43</v>
+      <c r="H66" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="I66" s="8"/>
       <c r="J66" s="4" t="s">
@@ -3393,10 +3405,10 @@
     </row>
     <row r="67" spans="1:12" ht="30">
       <c r="A67" s="8" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>14</v>
@@ -3409,29 +3421,29 @@
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H67" s="8"/>
       <c r="I67" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="K67" s="8"/>
     </row>
     <row r="68" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A68" s="8" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>16</v>
@@ -3444,7 +3456,7 @@
         <v>18</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>29</v>
@@ -3454,16 +3466,16 @@
     </row>
     <row r="69" spans="1:12" ht="30">
       <c r="A69" s="8" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>16</v>
@@ -3476,7 +3488,7 @@
         <v>17</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>25</v>
@@ -3485,16 +3497,16 @@
     </row>
     <row r="70" spans="1:12" ht="45">
       <c r="A70" s="8" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>16</v>
@@ -3507,7 +3519,7 @@
         <v>18</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J70" s="3" t="s">
         <v>25</v>
@@ -3516,10 +3528,10 @@
     </row>
     <row r="71" spans="1:12" ht="30">
       <c r="A71" s="8" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>14</v>
@@ -3532,58 +3544,58 @@
       </c>
       <c r="F71" s="8"/>
       <c r="G71" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H71" s="8"/>
       <c r="I71" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="K71" s="8"/>
     </row>
     <row r="72" spans="1:12" ht="30">
       <c r="A72" s="8" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F72" s="8"/>
       <c r="G72" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H72" s="8"/>
       <c r="I72" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="J72" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="K72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="30">
       <c r="A73" s="8" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>196</v>
+        <v>296</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>0</v>
@@ -3592,25 +3604,25 @@
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
       <c r="I73" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J73" s="8" t="s">
-        <v>197</v>
+        <v>314</v>
       </c>
       <c r="K73" s="8"/>
     </row>
     <row r="74" spans="1:12" ht="30">
       <c r="A74" s="8" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>205</v>
+        <v>295</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>0</v>
@@ -3619,83 +3631,83 @@
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J74" s="8" t="s">
-        <v>210</v>
+        <v>313</v>
       </c>
       <c r="K74" s="8"/>
     </row>
     <row r="75" spans="1:12" ht="45">
       <c r="A75" s="8" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F75" s="8"/>
       <c r="G75" s="8" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="H75" s="8"/>
       <c r="I75" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>200</v>
+        <v>293</v>
       </c>
       <c r="K75" s="8"/>
     </row>
     <row r="76" spans="1:12" ht="45">
       <c r="A76" s="8" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="8" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="H76" s="8"/>
       <c r="I76" s="8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>206</v>
+        <v>294</v>
       </c>
       <c r="K76" s="8"/>
     </row>
     <row r="77" spans="1:12" ht="30">
       <c r="A77" s="8" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>16</v>
@@ -3708,25 +3720,25 @@
         <v>33</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="K77" s="8"/>
     </row>
     <row r="78" spans="1:12" ht="30">
       <c r="A78" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>16</v>
@@ -3736,28 +3748,28 @@
       </c>
       <c r="G78" s="8"/>
       <c r="H78" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="K78" s="8"/>
     </row>
     <row r="79" spans="1:12" ht="45">
       <c r="A79" s="8" t="s">
-        <v>144</v>
+        <v>265</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>19</v>
@@ -3768,7 +3780,7 @@
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>11</v>
@@ -3777,16 +3789,16 @@
     </row>
     <row r="80" spans="1:12" ht="30">
       <c r="A80" s="13" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>19</v>
@@ -3797,53 +3809,53 @@
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
       <c r="I80" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="K80" s="8"/>
     </row>
     <row r="81" spans="1:10" ht="30">
       <c r="A81" t="s">
-        <v>305</v>
+        <v>271</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D81" t="s">
-        <v>302</v>
+        <v>273</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="H81"/>
       <c r="I81" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30">
       <c r="A82" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>19</v>
@@ -3854,24 +3866,24 @@
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="3" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30">
       <c r="A83" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>16</v>
@@ -3881,10 +3893,10 @@
       </c>
       <c r="G83" s="8"/>
       <c r="H83" s="5" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="J83" s="5" t="s">
         <v>25</v>
@@ -3892,16 +3904,16 @@
     </row>
     <row r="84" spans="1:10" ht="30">
       <c r="A84" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>19</v>
@@ -3912,24 +3924,24 @@
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30">
       <c r="A85" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>16</v>
@@ -3942,7 +3954,7 @@
         <v>17</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>25</v>
@@ -3950,16 +3962,16 @@
     </row>
     <row r="86" spans="1:10" ht="45">
       <c r="A86" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>16</v>
@@ -3972,7 +3984,7 @@
         <v>18</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Updated test cases for Authoring module
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="315">
   <si>
     <t>GET</t>
   </si>
@@ -496,15 +496,9 @@
     <t>OPQA-351</t>
   </si>
   <si>
-    <t>/comments/comment/(OPQA-236_comments.id)(OPQA-331_counterValue)</t>
-  </si>
-  <si>
     <t>/comments/count/(SYS_USER1)(OPQA-331_counterValue)</t>
   </si>
   <si>
-    <t>/comments/comment?id=(OPQA-236_comments.id)(OPQA-331_counterValue)</t>
-  </si>
-  <si>
     <t>/comments/user/(SYS_USER1)(OPQA-331_counterValue)</t>
   </si>
   <si>
@@ -959,6 +953,12 @@
   </si>
   <si>
     <t>status=200||id=(OPQA-360_id)||type=posts||counterName=commentCountForTarget||counterValue=2</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-236_comments.id)a</t>
+  </si>
+  <si>
+    <t>/comments/comment?id=(OPQA-236_comments.id)a</t>
   </si>
 </sst>
 </file>
@@ -1362,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L86"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1431,7 +1431,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>0</v>
@@ -1459,14 +1459,14 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -1497,11 +1497,11 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>20</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="4" t="s">
@@ -1559,11 +1559,11 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>20</v>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="4" t="s">
@@ -1621,11 +1621,11 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8"/>
@@ -1651,13 +1651,13 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9"/>
@@ -1683,11 +1683,11 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10"/>
@@ -1713,13 +1713,13 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11"/>
@@ -1773,7 +1773,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13"/>
@@ -1821,7 +1821,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>160</v>
+        <v>313</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
@@ -1831,9 +1831,11 @@
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="I15" s="8"/>
+        <v>243</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="J15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1861,13 +1863,13 @@
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16"/>
@@ -1893,7 +1895,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>96</v>
@@ -1991,7 +1993,9 @@
       <c r="H20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="8"/>
+      <c r="I20" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="J20" s="3" t="s">
         <v>29</v>
       </c>
@@ -2019,7 +2023,9 @@
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="I21" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="J21" s="8" t="s">
         <v>101</v>
       </c>
@@ -2145,7 +2151,7 @@
         <v>96</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K25" s="8"/>
       <c r="L25"/>
@@ -2175,7 +2181,7 @@
         <v>106</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26"/>
@@ -2201,11 +2207,11 @@
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>20</v>
@@ -2233,13 +2239,13 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>139</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28"/>
@@ -2269,7 +2275,7 @@
         <v>139</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K29" s="8"/>
       <c r="L29"/>
@@ -2325,7 +2331,7 @@
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>135</v>
@@ -2411,7 +2417,7 @@
         <v>14</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>0</v>
@@ -2437,7 +2443,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
@@ -2463,7 +2469,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>0</v>
@@ -2491,7 +2497,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>162</v>
+        <v>314</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>0</v>
@@ -2521,7 +2527,7 @@
         <v>14</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>0</v>
@@ -2540,7 +2546,7 @@
     </row>
     <row r="39" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A39" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>68</v>
@@ -2549,7 +2555,7 @@
         <v>14</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>0</v>
@@ -2566,10 +2572,10 @@
     </row>
     <row r="40" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A40" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>14</v>
@@ -2587,14 +2593,14 @@
         <v>96</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K40" s="8"/>
       <c r="L40"/>
     </row>
     <row r="41" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A41" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>72</v>
@@ -2613,7 +2619,7 @@
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="4" t="s">
@@ -2626,16 +2632,16 @@
     </row>
     <row r="42" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A42" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>16</v>
@@ -2648,7 +2654,7 @@
         <v>32</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>25</v>
@@ -2658,7 +2664,7 @@
     </row>
     <row r="43" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A43" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>50</v>
@@ -2667,7 +2673,7 @@
         <v>14</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>16</v>
@@ -2680,17 +2686,17 @@
         <v>33</v>
       </c>
       <c r="I43" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J43" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="K43" s="8"/>
       <c r="L43"/>
     </row>
     <row r="44" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A44" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>51</v>
@@ -2699,7 +2705,7 @@
         <v>14</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>16</v>
@@ -2712,10 +2718,10 @@
         <v>34</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44"/>
@@ -2731,7 +2737,7 @@
         <v>14</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>19</v>
@@ -2742,7 +2748,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>11</v>
@@ -2752,7 +2758,7 @@
     </row>
     <row r="46" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A46" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>78</v>
@@ -2761,7 +2767,7 @@
         <v>14</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>16</v>
@@ -2774,7 +2780,7 @@
         <v>35</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>25</v>
@@ -2793,7 +2799,7 @@
         <v>14</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>0</v>
@@ -2812,7 +2818,7 @@
     </row>
     <row r="48" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A48" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>52</v>
@@ -2831,7 +2837,7 @@
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="4" t="s">
@@ -2844,7 +2850,7 @@
     </row>
     <row r="49" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A49" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>52</v>
@@ -2863,7 +2869,7 @@
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="5" t="s">
@@ -2876,7 +2882,7 @@
     </row>
     <row r="50" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A50" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>55</v>
@@ -2898,7 +2904,7 @@
         <v>39</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>26</v>
@@ -2908,7 +2914,7 @@
     </row>
     <row r="51" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A51" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>54</v>
@@ -2917,7 +2923,7 @@
         <v>14</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>0</v>
@@ -2926,17 +2932,17 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K51" s="8"/>
       <c r="L51"/>
     </row>
     <row r="52" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A52" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>53</v>
@@ -2952,21 +2958,21 @@
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K52" s="8"/>
       <c r="L52"/>
     </row>
     <row r="53" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A53" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>56</v>
@@ -2984,17 +2990,17 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K53" s="8"/>
       <c r="L53"/>
     </row>
     <row r="54" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A54" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>57</v>
@@ -3003,28 +3009,28 @@
         <v>14</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K54" s="8"/>
       <c r="L54"/>
     </row>
     <row r="55" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A55" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>58</v>
@@ -3042,7 +3048,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>11</v>
@@ -3054,16 +3060,16 @@
     </row>
     <row r="56" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A56" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>16</v>
@@ -3073,29 +3079,29 @@
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K56" s="8"/>
       <c r="L56"/>
     </row>
     <row r="57" spans="1:12" ht="30">
       <c r="A57" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>16</v>
@@ -3105,19 +3111,19 @@
       </c>
       <c r="G57" s="8"/>
       <c r="H57" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K57" s="8"/>
     </row>
     <row r="58" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A58" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>83</v>
@@ -3126,7 +3132,7 @@
         <v>14</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>16</v>
@@ -3136,20 +3142,20 @@
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K58" s="8"/>
       <c r="L58"/>
     </row>
     <row r="59" spans="1:12" ht="30">
       <c r="A59" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>80</v>
@@ -3168,13 +3174,13 @@
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K59" s="3" t="s">
         <v>20</v>
@@ -3182,7 +3188,7 @@
     </row>
     <row r="60" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A60" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>82</v>
@@ -3201,13 +3207,13 @@
       </c>
       <c r="G60" s="8"/>
       <c r="H60" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>20</v>
@@ -3216,7 +3222,7 @@
     </row>
     <row r="61" spans="1:12" ht="30">
       <c r="A61" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>81</v>
@@ -3225,7 +3231,7 @@
         <v>14</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>16</v>
@@ -3238,16 +3244,16 @@
         <v>17</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="K61" s="8"/>
     </row>
     <row r="62" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A62" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>60</v>
@@ -3256,7 +3262,7 @@
         <v>14</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>16</v>
@@ -3269,26 +3275,26 @@
         <v>17</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J62" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K62" s="8"/>
       <c r="L62"/>
     </row>
     <row r="63" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A63" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>16</v>
@@ -3301,26 +3307,26 @@
         <v>17</v>
       </c>
       <c r="I63" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J63" s="8" t="s">
         <v>201</v>
-      </c>
-      <c r="J63" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="K63" s="8"/>
       <c r="L63"/>
     </row>
     <row r="64" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A64" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>16</v>
@@ -3333,26 +3339,26 @@
         <v>17</v>
       </c>
       <c r="I64" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J64" s="8" t="s">
         <v>208</v>
-      </c>
-      <c r="J64" s="8" t="s">
-        <v>210</v>
       </c>
       <c r="K64" s="8"/>
       <c r="L64"/>
     </row>
     <row r="65" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A65" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>16</v>
@@ -3365,17 +3371,17 @@
         <v>18</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J65" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K65" s="8"/>
       <c r="L65"/>
     </row>
     <row r="66" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A66" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>59</v>
@@ -3394,7 +3400,7 @@
       </c>
       <c r="G66" s="8"/>
       <c r="H66" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I66" s="8"/>
       <c r="J66" s="4" t="s">
@@ -3405,7 +3411,7 @@
     </row>
     <row r="67" spans="1:12" ht="30">
       <c r="A67" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>67</v>
@@ -3425,16 +3431,16 @@
       </c>
       <c r="H67" s="8"/>
       <c r="I67" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K67" s="8"/>
     </row>
     <row r="68" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A68" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>61</v>
@@ -3443,7 +3449,7 @@
         <v>14</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>16</v>
@@ -3456,7 +3462,7 @@
         <v>18</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>29</v>
@@ -3466,7 +3472,7 @@
     </row>
     <row r="69" spans="1:12" ht="30">
       <c r="A69" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>62</v>
@@ -3475,7 +3481,7 @@
         <v>14</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>16</v>
@@ -3488,7 +3494,7 @@
         <v>17</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>25</v>
@@ -3497,7 +3503,7 @@
     </row>
     <row r="70" spans="1:12" ht="45">
       <c r="A70" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>65</v>
@@ -3506,7 +3512,7 @@
         <v>14</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>16</v>
@@ -3519,7 +3525,7 @@
         <v>18</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J70" s="3" t="s">
         <v>25</v>
@@ -3528,7 +3534,7 @@
     </row>
     <row r="71" spans="1:12" ht="30">
       <c r="A71" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>63</v>
@@ -3548,16 +3554,16 @@
       </c>
       <c r="H71" s="8"/>
       <c r="I71" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K71" s="8"/>
     </row>
     <row r="72" spans="1:12" ht="30">
       <c r="A72" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>66</v>
@@ -3566,7 +3572,7 @@
         <v>14</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>0</v>
@@ -3577,16 +3583,16 @@
       </c>
       <c r="H72" s="8"/>
       <c r="I72" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="30">
       <c r="A73" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>84</v>
@@ -3595,7 +3601,7 @@
         <v>14</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>0</v>
@@ -3604,16 +3610,16 @@
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
       <c r="I73" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J73" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K73" s="8"/>
     </row>
     <row r="74" spans="1:12" ht="30">
       <c r="A74" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>85</v>
@@ -3622,7 +3628,7 @@
         <v>14</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>0</v>
@@ -3631,16 +3637,16 @@
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J74" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K74" s="8"/>
     </row>
     <row r="75" spans="1:12" ht="45">
       <c r="A75" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B75" s="9" t="s">
         <v>87</v>
@@ -3649,27 +3655,27 @@
         <v>14</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F75" s="8"/>
       <c r="G75" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H75" s="8"/>
       <c r="I75" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K75" s="8"/>
     </row>
     <row r="76" spans="1:12" ht="45">
       <c r="A76" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>88</v>
@@ -3678,27 +3684,27 @@
         <v>14</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H76" s="8"/>
       <c r="I76" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K76" s="8"/>
     </row>
     <row r="77" spans="1:12" ht="30">
       <c r="A77" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>50</v>
@@ -3707,7 +3713,7 @@
         <v>14</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>16</v>
@@ -3720,16 +3726,16 @@
         <v>33</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K77" s="8"/>
     </row>
     <row r="78" spans="1:12" ht="30">
       <c r="A78" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>51</v>
@@ -3738,7 +3744,7 @@
         <v>14</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>16</v>
@@ -3751,16 +3757,16 @@
         <v>89</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K78" s="8"/>
     </row>
     <row r="79" spans="1:12" ht="45">
       <c r="A79" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>75</v>
@@ -3769,7 +3775,7 @@
         <v>14</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>19</v>
@@ -3780,7 +3786,7 @@
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>11</v>
@@ -3789,16 +3795,16 @@
     </row>
     <row r="80" spans="1:12" ht="30">
       <c r="A80" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>269</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>19</v>
@@ -3809,53 +3815,53 @@
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
       <c r="I80" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K80" s="8"/>
     </row>
     <row r="81" spans="1:10" ht="30">
       <c r="A81" t="s">
+        <v>269</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" t="s">
         <v>271</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D81" t="s">
-        <v>273</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H81"/>
       <c r="I81" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30">
       <c r="A82" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>19</v>
@@ -3866,24 +3872,24 @@
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30">
       <c r="A83" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>16</v>
@@ -3893,10 +3899,10 @@
       </c>
       <c r="G83" s="8"/>
       <c r="H83" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J83" s="5" t="s">
         <v>25</v>
@@ -3904,16 +3910,16 @@
     </row>
     <row r="84" spans="1:10" ht="30">
       <c r="A84" t="s">
+        <v>279</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>283</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>19</v>
@@ -3924,24 +3930,24 @@
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30">
       <c r="A85" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>16</v>
@@ -3954,7 +3960,7 @@
         <v>17</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>25</v>
@@ -3962,16 +3968,16 @@
     </row>
     <row r="86" spans="1:10" ht="45">
       <c r="A86" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>16</v>
@@ -3984,7 +3990,7 @@
         <v>18</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Fixed failed test cases in Authoring
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -934,9 +934,6 @@
     <t>status=200||content=Update own comment||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
   </si>
   <si>
-    <t>status=200||content= Tags clean up surround tags like abcd while editing comment by User 1||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
     <t>{"targetType":"posts","targetId":"(OPQA-360_id)","content":"Comment Test on own Post:: Post Test 222 From API User1"}</t>
   </si>
   <si>
@@ -959,6 +956,9 @@
   </si>
   <si>
     <t>/comments/comment?id=(OPQA-236_comments.id)a</t>
+  </si>
+  <si>
+    <t>status=200||content=Tags clean up surround tags like abcd while editing comment by User 1||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
   </si>
 </sst>
 </file>
@@ -1362,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1657,7 +1657,7 @@
         <v>96</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9"/>
@@ -1821,7 +1821,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
@@ -2497,7 +2497,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>0</v>
@@ -3174,13 +3174,13 @@
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K59" s="3" t="s">
         <v>20</v>
@@ -3207,13 +3207,13 @@
       </c>
       <c r="G60" s="8"/>
       <c r="H60" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>20</v>
@@ -3613,7 +3613,7 @@
         <v>177</v>
       </c>
       <c r="J73" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K73" s="8"/>
     </row>
@@ -3640,7 +3640,7 @@
         <v>185</v>
       </c>
       <c r="J74" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K74" s="8"/>
     </row>

</xml_diff>

<commit_message>
Fixed testcases for Authoring
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -766,12 +766,6 @@
     <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
   </si>
   <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"HTML content Test:: &lt;br&gt; Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt; &lt;br&gt; "}</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=HTML content Test:: &lt;br&gt; Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt; &lt;br&gt;</t>
-  </si>
-  <si>
     <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-245_comments.id)||content=""</t>
   </si>
   <si>
@@ -959,6 +953,12 @@
   </si>
   <si>
     <t>status=200||content=Tags clean up surround tags like abcd while editing comment by User 1||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
   </si>
 </sst>
 </file>
@@ -1497,11 +1497,11 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>20</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="4" t="s">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="4" t="s">
@@ -1621,11 +1621,11 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8"/>
@@ -1651,13 +1651,13 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9"/>
@@ -1821,7 +1821,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
@@ -1863,13 +1863,13 @@
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16"/>
@@ -2218,8 +2218,8 @@
       </c>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" s="2" customFormat="1" ht="45">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A28" s="13" t="s">
         <v>142</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -2239,13 +2239,13 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5" t="s">
-        <v>250</v>
+        <v>313</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>139</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>251</v>
+        <v>314</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28"/>
@@ -2275,7 +2275,7 @@
         <v>139</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K29" s="8"/>
       <c r="L29"/>
@@ -2443,7 +2443,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
@@ -2497,7 +2497,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>0</v>
@@ -2555,7 +2555,7 @@
         <v>14</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>0</v>
@@ -2593,7 +2593,7 @@
         <v>96</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K40" s="8"/>
       <c r="L40"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="4" t="s">
@@ -2837,7 +2837,7 @@
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="4" t="s">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="5" t="s">
@@ -3023,7 +3023,7 @@
         <v>177</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K54" s="8"/>
       <c r="L54"/>
@@ -3079,13 +3079,13 @@
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K56" s="8"/>
       <c r="L56"/>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="G57" s="8"/>
       <c r="H57" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>177</v>
@@ -3142,13 +3142,13 @@
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I58" s="8" t="s">
         <v>185</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K58" s="8"/>
       <c r="L58"/>
@@ -3174,13 +3174,13 @@
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K59" s="3" t="s">
         <v>20</v>
@@ -3207,13 +3207,13 @@
       </c>
       <c r="G60" s="8"/>
       <c r="H60" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>20</v>
@@ -3247,7 +3247,7 @@
         <v>177</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K61" s="8"/>
     </row>
@@ -3278,7 +3278,7 @@
         <v>185</v>
       </c>
       <c r="J62" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K62" s="8"/>
       <c r="L62"/>
@@ -3374,7 +3374,7 @@
         <v>185</v>
       </c>
       <c r="J65" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="K65" s="8"/>
       <c r="L65"/>
@@ -3400,7 +3400,7 @@
       </c>
       <c r="G66" s="8"/>
       <c r="H66" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I66" s="8"/>
       <c r="J66" s="4" t="s">
@@ -3601,7 +3601,7 @@
         <v>14</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>0</v>
@@ -3613,7 +3613,7 @@
         <v>177</v>
       </c>
       <c r="J73" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K73" s="8"/>
     </row>
@@ -3628,7 +3628,7 @@
         <v>14</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>0</v>
@@ -3640,7 +3640,7 @@
         <v>185</v>
       </c>
       <c r="J74" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K74" s="8"/>
     </row>
@@ -3669,7 +3669,7 @@
         <v>177</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K75" s="8"/>
     </row>
@@ -3698,7 +3698,7 @@
         <v>185</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K76" s="8"/>
     </row>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="79" spans="1:12" ht="45">
       <c r="A79" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>75</v>
@@ -3775,7 +3775,7 @@
         <v>14</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>19</v>
@@ -3795,16 +3795,16 @@
     </row>
     <row r="80" spans="1:12" ht="30">
       <c r="A80" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>267</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>19</v>
@@ -3818,50 +3818,50 @@
         <v>177</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K80" s="8"/>
     </row>
     <row r="81" spans="1:10" ht="30">
       <c r="A81" t="s">
+        <v>267</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" t="s">
         <v>269</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D81" t="s">
-        <v>271</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H81"/>
       <c r="I81" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30">
       <c r="A82" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>19</v>
@@ -3872,18 +3872,18 @@
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30">
       <c r="A83" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>14</v>
@@ -3899,10 +3899,10 @@
       </c>
       <c r="G83" s="8"/>
       <c r="H83" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J83" s="5" t="s">
         <v>25</v>
@@ -3910,16 +3910,16 @@
     </row>
     <row r="84" spans="1:10" ht="30">
       <c r="A84" t="s">
+        <v>277</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="8" t="s">
         <v>279</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>281</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>19</v>
@@ -3933,15 +3933,15 @@
         <v>177</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30">
       <c r="A85" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>14</v>
@@ -3960,7 +3960,7 @@
         <v>17</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>25</v>
@@ -3968,10 +3968,10 @@
     </row>
     <row r="86" spans="1:10" ht="45">
       <c r="A86" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>14</v>
@@ -3990,7 +3990,7 @@
         <v>18</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Added new test cases for draft posts under Authoring.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="393">
   <si>
     <t>GET</t>
   </si>
@@ -959,6 +959,240 @@
   </si>
   <si>
     <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>/drafts</t>
+  </si>
+  <si>
+    <t>{"content":"Draft Post 1 creation by Neon User1 creds. Later it might be published", "title":"Draft Post 1 by Neon User1", "topics":[]}</t>
+  </si>
+  <si>
+    <t>{"content":"Draft Post 1_1 creation by Neon User1 creds. This draft should not be created as last draft created just now.", "title":"Draft Post 1_1 by Neon User1", "topics":[]}</t>
+  </si>
+  <si>
+    <t>Verify that spam check and unsupported tag validations are not done on draft post</t>
+  </si>
+  <si>
+    <t>Verify that spam check and unsupported tag validations are done when user publishes the draft post</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to access and edit the draft posts from their profile</t>
+  </si>
+  <si>
+    <t>Verfiy that the Drafts Post tab displays the count of the saved posts correctly</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to delete the draft post from the list in their profile</t>
+  </si>
+  <si>
+    <t>{"content":"Edited Draft Post 1 by Neon User1. &lt;br&gt; And this draft might be published as a Post using Post API", "title":"Draft Post 1 From API Edited", "topics":[]}</t>
+  </si>
+  <si>
+    <t>/drafts/count/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>/drafts/draft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verfify that user is able to publish the draft post using API </t>
+  </si>
+  <si>
+    <t>/posts</t>
+  </si>
+  <si>
+    <t>{"content":"Draft Post 2 creation by Neon User1 creds. Later it might be published. This draft doesn't check spam and profanity example is bitch and fuck words allowed. Also allowed unsupported html tags like &lt;abcd&gt;Tags not clean up surround tags like abcd while creating draft by Neon User 2&lt;abcd&gt;", "title":"Draft Post 2 by Neon User2", "topics":[]}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||title=Draft Post 2 by Neon User2||content=""||found=true</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>Verfiy that un authorized user is not able to delete the draft post using API and check the error status</t>
+  </si>
+  <si>
+    <t>Verift that deleted drafts not able to delete using API and check the error status</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to add external links to the comment</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to add links other NEON content [ex -Posts, articles, patents, profiles] to the comment</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to flag a Post of others</t>
+  </si>
+  <si>
+    <t>Verify that user is able to un flag the Post of others that they have flagged</t>
+  </si>
+  <si>
+    <t>Verify that moderator is able to take appropriate action on flagged post.</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to delete their post</t>
+  </si>
+  <si>
+    <t>/report/posts/(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>{"report":"UP","reason":"RRP001"}</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-360_id)||hasReported=UP||reportCount=1</t>
+  </si>
+  <si>
+    <t>{"report":"DOWN","reason":"RRP102"}</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-360_id)||hasReported=DOWN||reportCount=0</t>
+  </si>
+  <si>
+    <t>OPQA-286_5</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||id=(OPQA-360_1_id)</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||title=Draft Post 1 by Neon User1||content=""||found=true</t>
+  </si>
+  <si>
+    <t>status=200||id=(SYS_USER1)||type=User||counterName=draftCountForUser||counterValue=2</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||title=Draft Post 2 From API||content=Draft Post 2 creation by API. it shouldn't be published. This draft must check spam and profanity example is ***** and **** words shouldn't be allowed. Also should not allow unsupported html tags like Tags clean up surround tags like abcd while creating draft ||found=true||wasCleanedUp=3</t>
+  </si>
+  <si>
+    <t>OPQA-1074</t>
+  </si>
+  <si>
+    <t>OPQA-1075</t>
+  </si>
+  <si>
+    <t>OPQA-1076</t>
+  </si>
+  <si>
+    <t>Verify that user able to create a draft post using API</t>
+  </si>
+  <si>
+    <t>OPQA-1078</t>
+  </si>
+  <si>
+    <t>/drafts/draft/(OPQA-1078_id)</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||title=Draft Post 1 by Neon User1||content=Draft Post 1 creation by Neon User1 creds. Later it might be published||found=true||id=(OPQA-1078_id)</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-1078_id)||userId=(SYS_USER1)||title=Draft Post 1 From API Edited||content=""||found=true</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-1078_id)&amp;includeContent=true</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-1078_id)||userId=(SYS_USER1)||title=Draft Post 1 From API Edited||content=Edited Draft Post 1 by Neon User1. &lt;br&gt; And this draft might be published as a Post using Post API||found=true</t>
+  </si>
+  <si>
+    <t>{"content":"Draft Post 1 by Neon User1. &lt;br&gt; And this draft should be published as a Post using Post API", "title":"Draft Post 1 From API", "topics":[], "id":"(OPQA-1078_id)"}</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-1078_id)||userId=(SYS_USER1)||title=Draft Post 1 From API||content=Draft Post 1 by Neon User1. &lt;br&gt; And this draft should be published as a Post using Post API||found=true</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-1078_id)||found=false||keydateModified=0||keydate=0</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=posts||comments.targetId=(OPQA-1078_id)||comments.content=Testing for adding external link from API:: &lt;br&gt; &lt;a href=\"www.flipkart.com\"&gt;Flipkart here&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=posts||comments.targetId=(OPQA-1078_id)||comments.content=Testing for adding neon external links from API:: &lt;br&gt; Patent link: &lt;a href=\"#/patents/US5272057A_19931221\"&gt;click here&lt;/a&gt;&lt;br&gt; Neon User1 Profile link: &lt;a href=\"#/profile/fd983517-2c2d-4151-9c1a-6b3c3d6b6fb0\"&gt;click here&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to create a draft within less than 60 seconds of last created draft using API</t>
+  </si>
+  <si>
+    <t>OPQA-1079</t>
+  </si>
+  <si>
+    <t>OPQA-1080</t>
+  </si>
+  <si>
+    <t>{"content":"Draft Post 2 creation by API. it shouldn't be published. This draft must check spam and profanity example is bitch and fuck words shouldn't be allowed. Also should not allow unsupported html tags like &lt;abcd&gt;Tags clean up surround tags like abcd while creating draft &lt;abcd&gt;", "title":"Draft Post 2 From API", "topics":[], "id":"(OPQA-1080_id)"}</t>
+  </si>
+  <si>
+    <t>/drafts/draft/(OPQA-1080_id)</t>
+  </si>
+  <si>
+    <t>Verify that user able to view draft by draft ID using API</t>
+  </si>
+  <si>
+    <t>OPQA-1081</t>
+  </si>
+  <si>
+    <t>OPQA-1083</t>
+  </si>
+  <si>
+    <t>OPQA-1084</t>
+  </si>
+  <si>
+    <t>OPQA-1085</t>
+  </si>
+  <si>
+    <t>Verify that user able to view draft posts based on list of ids specified in query string using API</t>
+  </si>
+  <si>
+    <t>OPQA-1086</t>
+  </si>
+  <si>
+    <t>OPQA-1087</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-1087_id)","content":"Testing for adding external link from API:: &lt;br&gt; &lt;a href=\"www.flipkart.com\"&gt;Flipkart here&lt;/a&gt;"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-1087_id)","content":"Testing for adding neon external links from API:: &lt;br&gt; Patent link: &lt;a href=\"#/patents/US5272057A_19931221\"&gt;click here&lt;/a&gt;&lt;br&gt; Neon User1 Profile link: &lt;a href=\"#/profile/(SYS_USER1)\"&gt;click here&lt;/a&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-1087_id)||hasReported=UP||reportCount=1</t>
+  </si>
+  <si>
+    <t>/report/posts/(OPQA-1087_id)</t>
+  </si>
+  <si>
+    <t>/administration/posts/(OPQA-1087_id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-1087_id)||hasSucceeded=true||errorMsg=""</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to access the draft once it is published using API</t>
+  </si>
+  <si>
+    <t>OPQA-1088</t>
+  </si>
+  <si>
+    <t>OPQA-1089</t>
+  </si>
+  <si>
+    <t>OPQA-1090</t>
+  </si>
+  <si>
+    <t>OPQA-1091</t>
+  </si>
+  <si>
+    <t>OPQA-1092</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-1092_comments.id)</t>
+  </si>
+  <si>
+    <t>OPQA-1093</t>
+  </si>
+  <si>
+    <t>OPQA-1074_1</t>
+  </si>
+  <si>
+    <t>OPQA-1094</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1244,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1031,11 +1265,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1066,6 +1315,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1360,15 +1619,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L86"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="43.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3542,7 +3801,7 @@
       <c r="C71" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E71" s="3" t="s">
@@ -3795,205 +4054,810 @@
     </row>
     <row r="80" spans="1:12" ht="30">
       <c r="A80" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>264</v>
+        <v>349</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>335</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>265</v>
+        <v>339</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
+      <c r="H80" s="8" t="s">
+        <v>340</v>
+      </c>
       <c r="I80" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>266</v>
+        <v>341</v>
       </c>
       <c r="K80" s="8"/>
     </row>
-    <row r="81" spans="1:10" ht="30">
-      <c r="A81" t="s">
-        <v>267</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>268</v>
+    <row r="81" spans="1:11" ht="30">
+      <c r="A81" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>336</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D81" t="s">
-        <v>269</v>
+      <c r="D81" s="8" t="s">
+        <v>339</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F81"/>
-      <c r="G81" t="s">
-        <v>270</v>
-      </c>
-      <c r="H81"/>
-      <c r="I81" s="3" t="s">
-        <v>177</v>
+        <v>16</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>349</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="30">
-      <c r="A82" t="s">
-        <v>272</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>273</v>
+        <v>343</v>
+      </c>
+      <c r="K81" s="8"/>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>338</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>265</v>
+        <v>186</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>27</v>
+        <v>330</v>
       </c>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
-      <c r="I82" s="3" t="s">
+      <c r="I82" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="K82" s="8"/>
+    </row>
+    <row r="83" spans="1:11" ht="30">
+      <c r="A83" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="J82" s="5" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="30">
-      <c r="A83" t="s">
-        <v>275</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>276</v>
+      <c r="B83" s="9" t="s">
+        <v>264</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>179</v>
+        <v>265</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="G83" s="8"/>
-      <c r="H83" s="5" t="s">
-        <v>294</v>
-      </c>
+      <c r="H83" s="8"/>
       <c r="I83" s="3" t="s">
-        <v>263</v>
+        <v>177</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="30">
+        <v>266</v>
+      </c>
+      <c r="K83" s="8"/>
+    </row>
+    <row r="84" spans="1:11" ht="30">
       <c r="A84" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="8" t="s">
-        <v>279</v>
+      <c r="D84" t="s">
+        <v>269</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="F84"/>
+      <c r="G84" t="s">
+        <v>270</v>
+      </c>
+      <c r="H84"/>
       <c r="I84" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="30">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="30">
       <c r="A85" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="G85" s="8"/>
-      <c r="H85" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="H85" s="8"/>
       <c r="I85" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="J85" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="45">
+      <c r="J85" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="30">
       <c r="A86" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>229</v>
+        <v>179</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="F86" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G86" s="8"/>
-      <c r="H86" s="4" t="s">
-        <v>18</v>
+      <c r="H86" s="5" t="s">
+        <v>294</v>
       </c>
       <c r="I86" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="J86" s="3" t="s">
+      <c r="J86" s="5" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="30">
+      <c r="A87" t="s">
+        <v>277</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="30">
+      <c r="A88" t="s">
+        <v>281</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G88" s="8"/>
+      <c r="H88" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="45">
+      <c r="A89" t="s">
+        <v>283</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G89" s="8"/>
+      <c r="H89" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="30">
+      <c r="A90" t="s">
+        <v>353</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" t="s">
+        <v>315</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="K90" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="45">
+      <c r="A91" t="s">
+        <v>365</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" t="s">
+        <v>315</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="75">
+      <c r="A92" t="s">
+        <v>366</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" t="s">
+        <v>315</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="K92" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="30">
+      <c r="A93" t="s">
+        <v>370</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" t="s">
+        <v>354</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F93"/>
+      <c r="H93"/>
+      <c r="I93" t="s">
+        <v>353</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="75">
+      <c r="A94" t="s">
+        <v>371</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" t="s">
+        <v>327</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H94" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="I94" t="s">
+        <v>366</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="45">
+      <c r="A95" t="s">
+        <v>372</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" t="s">
+        <v>354</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="I95" t="s">
+        <v>353</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="30">
+      <c r="A96" t="s">
+        <v>373</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" t="s">
+        <v>324</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H96"/>
+      <c r="I96" t="s">
+        <v>353</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="30">
+      <c r="A97" t="s">
+        <v>375</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" t="s">
+        <v>325</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F97"/>
+      <c r="G97" t="s">
+        <v>357</v>
+      </c>
+      <c r="H97"/>
+      <c r="I97" t="s">
+        <v>353</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="45">
+      <c r="A98" t="s">
+        <v>376</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" t="s">
+        <v>327</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="I98" t="s">
+        <v>353</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="K98" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="30">
+      <c r="A99" t="s">
+        <v>384</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" t="s">
+        <v>354</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F99"/>
+      <c r="H99"/>
+      <c r="I99" t="s">
+        <v>376</v>
+      </c>
+      <c r="J99" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="45">
+      <c r="A100" t="s">
+        <v>385</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s">
+        <v>368</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H100"/>
+      <c r="I100" t="s">
+        <v>366</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="30">
+      <c r="A101" t="s">
+        <v>386</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" t="s">
+        <v>368</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="H101"/>
+      <c r="I101" t="s">
+        <v>366</v>
+      </c>
+      <c r="J101" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="30">
+      <c r="A102" t="s">
+        <v>387</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" t="s">
+        <v>368</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="H102"/>
+      <c r="I102" t="s">
+        <v>366</v>
+      </c>
+      <c r="J102" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="45">
+      <c r="A103" t="s">
+        <v>388</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="I103" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="J103" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="45">
+      <c r="A104" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="J104" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K104" s="8"/>
+    </row>
+    <row r="105" spans="1:11" ht="60">
+      <c r="A105" t="s">
+        <v>390</v>
+      </c>
+      <c r="B105" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H105" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="I105" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="K105" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="30">
+      <c r="A106" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="I106" t="s">
+        <v>376</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="K106" s="8"/>
+    </row>
+    <row r="107" spans="1:11" ht="30">
+      <c r="A107" t="s">
+        <v>392</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="G107" s="8"/>
+      <c r="H107" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I107" t="s">
+        <v>376</v>
+      </c>
+      <c r="J107" s="5" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testcases for WatchlistRA and Authoring module.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -7,14 +7,16 @@
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
-    <sheet name="Authoring" sheetId="1" r:id="rId1"/>
+    <sheet name="Authoring-wos and patents" sheetId="1" r:id="rId1"/>
+    <sheet name="Authoring-Posts" sheetId="2" r:id="rId2"/>
+    <sheet name="Authoring-Drafts" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="408">
   <si>
     <t>GET</t>
   </si>
@@ -808,9 +810,6 @@
     <t>OPQA-776</t>
   </si>
   <si>
-    <t>Verify that the admin can delete any post as a moderator</t>
-  </si>
-  <si>
     <t>/administration/posts/(OPQA-360_id)</t>
   </si>
   <si>
@@ -1159,9 +1158,6 @@
     <t>/report/posts/(OPQA-1087_id)</t>
   </si>
   <si>
-    <t>/administration/posts/(OPQA-1087_id)</t>
-  </si>
-  <si>
     <t>status=200||targetType=posts||targetId=(OPQA-1087_id)||hasSucceeded=true||errorMsg=""</t>
   </si>
   <si>
@@ -1193,6 +1189,57 @@
   </si>
   <si>
     <t>OPQA-1094</t>
+  </si>
+  <si>
+    <t>Verify that the admin can delete any post using backend admin API</t>
+  </si>
+  <si>
+    <t>Verify that moderator is not able to process the unreported post and check the error status using API</t>
+  </si>
+  <si>
+    <t>/administration/report/posts/(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER3)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>{"adminAction":"REMOVED","adminNote":"Test API from POSTMAN","override":"false"}</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-360_id)||hasSucceeded=false||errorMsg=Authored item not found with id: (OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>OPQA-360_2</t>
+  </si>
+  <si>
+    <t>{"title":"Post Test 1  From API User1","content":"Post content creation from API Automation Script  by User1. &lt;br&gt; This post might be flagged and deleted by moderator"}</t>
+  </si>
+  <si>
+    <t>/report/posts/(OPQA-360_2_id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-360_2_id)||hasReported=UP||reportCount=1</t>
+  </si>
+  <si>
+    <t>OPQA-1074_2</t>
+  </si>
+  <si>
+    <t>OPQA-1094_1</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-360_2_id)||hasSucceeded=true||errorMsg=""</t>
+  </si>
+  <si>
+    <t>OPQA-360_2||OPQA-1074</t>
+  </si>
+  <si>
+    <t>/administration/report/posts/(OPQA-360_2_id)</t>
+  </si>
+  <si>
+    <t>/administration/report/posts/(OPQA-1087_id)</t>
+  </si>
+  <si>
+    <t>OPQA-1258</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1315,9 +1362,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1619,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1756,11 +1800,11 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>20</v>
@@ -1788,7 +1832,7 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="4" t="s">
@@ -1850,7 +1894,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="4" t="s">
@@ -1880,11 +1924,11 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8"/>
@@ -1910,13 +1954,13 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9"/>
@@ -2080,7 +2124,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
@@ -2122,13 +2166,13 @@
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16"/>
@@ -2498,13 +2542,13 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>139</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28"/>
@@ -2756,7 +2800,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>0</v>
@@ -3075,1793 +3119,2040 @@
       </c>
       <c r="L47"/>
     </row>
-    <row r="48" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A48" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" s="8"/>
-      <c r="H48" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="I48" s="8"/>
-      <c r="J48" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L48"/>
-    </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A49" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G49" s="8"/>
-      <c r="H49" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="I49" s="8"/>
-      <c r="J49" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L49"/>
-    </row>
-    <row r="50" spans="1:12" s="2" customFormat="1" ht="45">
-      <c r="A50" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G50" s="3"/>
-      <c r="H50" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K50" s="3"/>
-      <c r="L50"/>
-    </row>
-    <row r="51" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A51" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="K51" s="8"/>
-      <c r="L51"/>
-    </row>
-    <row r="52" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A52" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="H52" s="8"/>
-      <c r="I52" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="K52" s="8"/>
-      <c r="L52"/>
-    </row>
-    <row r="53" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A53" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="K53" s="8"/>
-      <c r="L53"/>
-    </row>
-    <row r="54" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A54" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="H54" s="8"/>
-      <c r="I54" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="K54" s="8"/>
-      <c r="L54"/>
-    </row>
-    <row r="55" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A55" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L55"/>
-    </row>
-    <row r="56" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A56" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="K56" s="8"/>
-      <c r="L56"/>
-    </row>
-    <row r="57" spans="1:12" ht="30">
-      <c r="A57" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G57" s="8"/>
-      <c r="H57" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J57" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="K57" s="8"/>
-    </row>
-    <row r="58" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A58" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="I58" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J58" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="K58" s="8"/>
-      <c r="L58"/>
-    </row>
-    <row r="59" spans="1:12" ht="30">
-      <c r="A59" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G59" s="8"/>
-      <c r="H59" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="K59" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A60" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G60" s="8"/>
-      <c r="H60" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J60" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="K60" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L60"/>
-    </row>
-    <row r="61" spans="1:12" ht="30">
-      <c r="A61" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G61" s="8"/>
-      <c r="H61" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J61" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="K61" s="8"/>
-    </row>
-    <row r="62" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A62" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G62" s="8"/>
-      <c r="H62" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I62" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J62" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="K62" s="8"/>
-      <c r="L62"/>
-    </row>
-    <row r="63" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A63" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G63" s="8"/>
-      <c r="H63" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I63" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J63" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="K63" s="8"/>
-      <c r="L63"/>
-    </row>
-    <row r="64" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A64" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G64" s="8"/>
-      <c r="H64" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I64" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="J64" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="K64" s="8"/>
-      <c r="L64"/>
-    </row>
-    <row r="65" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A65" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G65" s="8"/>
-      <c r="H65" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I65" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J65" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="K65" s="8"/>
-      <c r="L65"/>
-    </row>
-    <row r="66" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A66" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G66" s="8"/>
-      <c r="H66" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="I66" s="8"/>
-      <c r="J66" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K66" s="8"/>
-      <c r="L66"/>
-    </row>
-    <row r="67" spans="1:12" ht="30">
-      <c r="A67" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F67" s="8"/>
-      <c r="G67" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H67" s="8"/>
-      <c r="I67" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="K67" s="8"/>
-    </row>
-    <row r="68" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A68" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G68" s="8"/>
-      <c r="H68" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K68" s="8"/>
-      <c r="L68"/>
-    </row>
-    <row r="69" spans="1:12" ht="30">
-      <c r="A69" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G69" s="8"/>
-      <c r="H69" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K69" s="8"/>
-    </row>
-    <row r="70" spans="1:12" ht="45">
-      <c r="A70" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G70" s="8"/>
-      <c r="H70" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I70" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K70" s="8"/>
-    </row>
-    <row r="71" spans="1:12" ht="30">
-      <c r="A71" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F71" s="8"/>
-      <c r="G71" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H71" s="8"/>
-      <c r="I71" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="K71" s="8"/>
-    </row>
-    <row r="72" spans="1:12" ht="30">
-      <c r="A72" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F72" s="8"/>
-      <c r="G72" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H72" s="8"/>
-      <c r="I72" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="K72" s="8"/>
-    </row>
-    <row r="73" spans="1:12" ht="30">
-      <c r="A73" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J73" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="K73" s="8"/>
-    </row>
-    <row r="74" spans="1:12" ht="30">
-      <c r="A74" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J74" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="K74" s="8"/>
-    </row>
-    <row r="75" spans="1:12" ht="45">
-      <c r="A75" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="H75" s="8"/>
-      <c r="I75" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="K75" s="8"/>
-    </row>
-    <row r="76" spans="1:12" ht="45">
-      <c r="A76" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="K76" s="8"/>
-    </row>
-    <row r="77" spans="1:12" ht="30">
-      <c r="A77" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G77" s="8"/>
-      <c r="H77" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I77" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="K77" s="8"/>
-    </row>
-    <row r="78" spans="1:12" ht="30">
-      <c r="A78" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J78" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="K78" s="8"/>
-    </row>
-    <row r="79" spans="1:12" ht="45">
-      <c r="A79" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="J79" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K79" s="8"/>
-    </row>
-    <row r="80" spans="1:12" ht="30">
-      <c r="A80" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="B80" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J80" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="K80" s="8"/>
-    </row>
-    <row r="81" spans="1:11" ht="30">
-      <c r="A81" s="13" t="s">
-        <v>350</v>
-      </c>
-      <c r="B81" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="I81" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="J81" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="K81" s="8"/>
-    </row>
-    <row r="82" spans="1:11">
-      <c r="A82" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J82" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="K82" s="8"/>
-    </row>
-    <row r="83" spans="1:11" ht="30">
-      <c r="A83" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
-      <c r="I83" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J83" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="K83" s="8"/>
-    </row>
-    <row r="84" spans="1:11" ht="30">
-      <c r="A84" t="s">
-        <v>267</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D84" t="s">
-        <v>269</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F84"/>
-      <c r="G84" t="s">
-        <v>270</v>
-      </c>
-      <c r="H84"/>
-      <c r="I84" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J84" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="30">
-      <c r="A85" t="s">
-        <v>272</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="30">
-      <c r="A86" t="s">
-        <v>275</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G86" s="8"/>
-      <c r="H86" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="J86" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="30">
-      <c r="A87" t="s">
-        <v>277</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
-      <c r="I87" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" ht="30">
-      <c r="A88" t="s">
-        <v>281</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D88" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G88" s="8"/>
-      <c r="H88" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" ht="45">
-      <c r="A89" t="s">
-        <v>283</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G89" s="8"/>
-      <c r="H89" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="30">
-      <c r="A90" t="s">
-        <v>353</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" t="s">
-        <v>315</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="K90" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="45">
-      <c r="A91" t="s">
-        <v>365</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" t="s">
-        <v>315</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="75">
-      <c r="A92" t="s">
-        <v>366</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D92" t="s">
-        <v>315</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="J92" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="K92" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" ht="30">
-      <c r="A93" t="s">
-        <v>370</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D93" t="s">
-        <v>354</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F93"/>
-      <c r="H93"/>
-      <c r="I93" t="s">
-        <v>353</v>
-      </c>
-      <c r="J93" s="5" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="75">
-      <c r="A94" t="s">
-        <v>371</v>
-      </c>
-      <c r="B94" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D94" t="s">
-        <v>327</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H94" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="I94" t="s">
-        <v>366</v>
-      </c>
-      <c r="J94" s="5" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="45">
-      <c r="A95" t="s">
-        <v>372</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D95" t="s">
-        <v>354</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="I95" t="s">
-        <v>353</v>
-      </c>
-      <c r="J95" s="5" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" ht="30">
-      <c r="A96" t="s">
-        <v>373</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D96" t="s">
-        <v>324</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H96"/>
-      <c r="I96" t="s">
-        <v>353</v>
-      </c>
-      <c r="J96" s="5" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" ht="30">
-      <c r="A97" t="s">
-        <v>375</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D97" t="s">
-        <v>325</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F97"/>
-      <c r="G97" t="s">
-        <v>357</v>
-      </c>
-      <c r="H97"/>
-      <c r="I97" t="s">
-        <v>353</v>
-      </c>
-      <c r="J97" s="5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="45">
-      <c r="A98" t="s">
-        <v>376</v>
-      </c>
-      <c r="B98" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D98" t="s">
-        <v>327</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="I98" t="s">
-        <v>353</v>
-      </c>
-      <c r="J98" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="K98" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" ht="30">
-      <c r="A99" t="s">
-        <v>384</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D99" t="s">
-        <v>354</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F99"/>
-      <c r="H99"/>
-      <c r="I99" t="s">
-        <v>376</v>
-      </c>
-      <c r="J99" s="5" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" ht="45">
-      <c r="A100" t="s">
-        <v>385</v>
-      </c>
-      <c r="B100" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D100" t="s">
-        <v>368</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H100"/>
-      <c r="I100" t="s">
-        <v>366</v>
-      </c>
-      <c r="J100" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="30">
-      <c r="A101" t="s">
-        <v>386</v>
-      </c>
-      <c r="B101" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D101" t="s">
-        <v>368</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="H101"/>
-      <c r="I101" t="s">
-        <v>366</v>
-      </c>
-      <c r="J101" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" ht="30">
-      <c r="A102" t="s">
-        <v>387</v>
-      </c>
-      <c r="B102" s="15" t="s">
-        <v>332</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" t="s">
-        <v>368</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="H102"/>
-      <c r="I102" t="s">
-        <v>366</v>
-      </c>
-      <c r="J102" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" ht="45">
-      <c r="A103" t="s">
-        <v>388</v>
-      </c>
-      <c r="B103" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D103" t="s">
-        <v>15</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H103" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="I103" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="J103" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="K103" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" ht="45">
-      <c r="A104" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D104" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G104" s="8"/>
-      <c r="H104" s="8"/>
-      <c r="I104" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="J104" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K104" s="8"/>
-    </row>
-    <row r="105" spans="1:11" ht="60">
-      <c r="A105" t="s">
-        <v>390</v>
-      </c>
-      <c r="B105" s="15" t="s">
-        <v>334</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D105" t="s">
-        <v>15</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H105" s="16" t="s">
-        <v>378</v>
-      </c>
-      <c r="I105" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="J105" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="K105" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" ht="30">
-      <c r="A106" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="B106" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="I106" t="s">
-        <v>376</v>
-      </c>
-      <c r="J106" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="K106" s="8"/>
-    </row>
-    <row r="107" spans="1:11" ht="30">
-      <c r="A107" t="s">
-        <v>392</v>
-      </c>
-      <c r="B107" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E107" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F107" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="G107" s="8"/>
-      <c r="H107" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I107" t="s">
-        <v>376</v>
-      </c>
-      <c r="J107" s="5" t="s">
-        <v>382</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="58.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="45" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="133.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A2" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2"/>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A3" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A4" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4"/>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A5" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5"/>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A6" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A7" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A8" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A9" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A10" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A12" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A14" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A16" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A17" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A18" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A19" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="K19" s="8"/>
+      <c r="L19"/>
+    </row>
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A20" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="1:12" ht="30">
+      <c r="A21" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A22" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22"/>
+    </row>
+    <row r="23" spans="1:12" ht="30">
+      <c r="A23" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" ht="45">
+      <c r="A24" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:12" ht="30">
+      <c r="A25" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:12" ht="30">
+      <c r="A26" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" ht="30">
+      <c r="A27" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" ht="30">
+      <c r="A28" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" ht="45">
+      <c r="A29" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" ht="45">
+      <c r="A30" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" ht="30">
+      <c r="A31" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" ht="30">
+      <c r="A32" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="K32" s="8"/>
+    </row>
+    <row r="33" spans="1:12" ht="45">
+      <c r="A33" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="8"/>
+    </row>
+    <row r="34" spans="1:12" ht="45">
+      <c r="A34" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:12" ht="30">
+      <c r="A35" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="K35" s="8"/>
+    </row>
+    <row r="36" spans="1:12" ht="30">
+      <c r="A36" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="K36" s="8"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:12" ht="30">
+      <c r="A38" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="K38" s="8"/>
+    </row>
+    <row r="39" spans="1:12" ht="30">
+      <c r="A39" t="s">
+        <v>266</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>269</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="30">
+      <c r="A40" t="s">
+        <v>271</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="30">
+      <c r="A41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="30">
+      <c r="A42" t="s">
+        <v>276</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="30">
+      <c r="A43" t="s">
+        <v>280</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="45">
+      <c r="A44" t="s">
+        <v>282</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="H44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A45" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="8"/>
+      <c r="H45" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L45"/>
+    </row>
+    <row r="46" spans="1:12" ht="30">
+      <c r="A46" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="K46" s="8"/>
+    </row>
+    <row r="47" spans="1:12" ht="30">
+      <c r="A47" t="s">
+        <v>390</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="98.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="A2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45">
+      <c r="A3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="75">
+      <c r="A4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>314</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>353</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>352</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="75">
+      <c r="A6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="I6" t="s">
+        <v>365</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>353</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="I7" t="s">
+        <v>352</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" t="s">
+        <v>372</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>323</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>352</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>324</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>356</v>
+      </c>
+      <c r="I9" t="s">
+        <v>352</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>326</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="I10" t="s">
+        <v>352</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>353</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>375</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45">
+      <c r="A12" t="s">
+        <v>383</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>367</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>365</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>384</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>367</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="I13" t="s">
+        <v>365</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" t="s">
+        <v>385</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>367</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="I14" t="s">
+        <v>365</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" t="s">
+        <v>386</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45">
+      <c r="A16" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:11" ht="60">
+      <c r="A17" t="s">
+        <v>388</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30">
+      <c r="A18" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="I18" t="s">
+        <v>375</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" t="s">
+        <v>402</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="I19" t="s">
+        <v>401</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating new testcases for Authoring.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Authoring-wos and patents" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="423">
   <si>
     <t>GET</t>
   </si>
@@ -1240,6 +1240,51 @@
   </si>
   <si>
     <t>OPQA-1258</t>
+  </si>
+  <si>
+    <t>OPQA-367</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to add external links to the post and publish it.</t>
+  </si>
+  <si>
+    <t>OPQA-1076_1</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-367_id)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER3)||id=(OPQA-367_id)</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to add links to other neon articles or profile to the post and publish it.</t>
+  </si>
+  <si>
+    <t>OPQA-369</t>
+  </si>
+  <si>
+    <t>OPQA-1076_2</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-369_id)</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER3)||id=(OPQA-369_id)</t>
+  </si>
+  <si>
+    <t>{"title":"Post Test 3 From API by Neon User3","content":"Testing for adding neon external links from API:: &lt;br&gt; Patent link: &lt;a href=\"#/patents/US5272057A_19931221\"&gt;click here&lt;/a&gt;&lt;br&gt; Neon User1 Profile link: &lt;a href=\"#/profile/(SYS_USER1)\"&gt;click here&lt;/a&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER3)||content=Testing for adding neon external links from API:: &lt;br&gt; Patent link: &lt;a href=\"#/patents/US5272057A_19931221\"&gt;click here&lt;/a&gt;&lt;br&gt; Neon User1 Profile link: &lt;a href=\"#/profile/(SYS_USER1)\"&gt;click here&lt;/a&gt;||title=Post Test 3 From API by Neon User3||found=true</t>
+  </si>
+  <si>
+    <t>{"title":"Post Test From API by Neon User3","content":"Testing for adding external link to the post from API:: &lt;br&gt; &lt;a href=\"www.flipkart.com\"&gt;Flipkart here&lt;/a&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER3)||content=Testing for adding external link to the post from API:: &lt;br&gt; &lt;a href=\"www.flipkart.com\"&gt;Flipkart here&lt;/a&gt;title=Post Test From API by Neon User3||found=true</t>
   </si>
 </sst>
 </file>
@@ -1665,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="I39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L47" sqref="L2:L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3127,10 +3172,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="I44" workbookViewId="0">
+      <selection activeCell="L51" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4582,6 +4627,128 @@
         <v>403</v>
       </c>
     </row>
+    <row r="48" spans="1:12" ht="30">
+      <c r="A48" t="s">
+        <v>408</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="I48" s="8"/>
+      <c r="J48" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" t="s">
+        <v>408</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="K49" s="8"/>
+    </row>
+    <row r="50" spans="1:11" ht="60">
+      <c r="A50" t="s">
+        <v>415</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="G50" s="8"/>
+      <c r="H50" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" t="s">
+        <v>415</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="K51" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4591,8 +4758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated pending test cases for Profile and Authoring.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Authoring-wos and patents" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="432">
   <si>
     <t>GET</t>
   </si>
@@ -999,9 +999,6 @@
     <t>/posts</t>
   </si>
   <si>
-    <t>{"content":"Draft Post 2 creation by Neon User1 creds. Later it might be published. This draft doesn't check spam and profanity example is bitch and fuck words allowed. Also allowed unsupported html tags like &lt;abcd&gt;Tags not clean up surround tags like abcd while creating draft by Neon User 2&lt;abcd&gt;", "title":"Draft Post 2 by Neon User2", "topics":[]}</t>
-  </si>
-  <si>
     <t>status=200||userId=(SYS_USER2)||title=Draft Post 2 by Neon User2||content=""||found=true</t>
   </si>
   <si>
@@ -1285,6 +1282,36 @@
   </si>
   <si>
     <t>status=200||userId=(SYS_USER3)||content=Testing for adding external link to the post from API:: &lt;br&gt; &lt;a href=\"www.flipkart.com\"&gt;Flipkart here&lt;/a&gt;title=Post Test From API by Neon User3||found=true</t>
+  </si>
+  <si>
+    <t>status=403</t>
+  </si>
+  <si>
+    <t>/drafts/user/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>Verify that API returns 403 for the mismatched truids while getting draft posts for the user.</t>
+  </si>
+  <si>
+    <t>{"content":"Draft Post 2 creation by Neon User2 creds. Later it might be published. This draft doesn't check spam and profanity example is bitch and fuck words allowed. Also allowed unsupported html tags like &lt;abcd&gt;Tags not clean up surround tags like abcd while creating draft by Neon User 2&lt;abcd&gt;", "title":"Draft Post 2 by Neon User2", "topics":[]}</t>
+  </si>
+  <si>
+    <t>Verify that API returns 403 for the mismatched truids while getting count of draft posts for the user.</t>
+  </si>
+  <si>
+    <t>Verify that for the given truid, API is able to get all the draft posts.</t>
+  </si>
+  <si>
+    <t>status=200||size=2||found=true||drafts[0].userId=(SYS_USER1)||drafts[0].id=(OPQA-1078_id)</t>
+  </si>
+  <si>
+    <t>OPQA-1363</t>
+  </si>
+  <si>
+    <t>OPQA-1364</t>
+  </si>
+  <si>
+    <t>OPQA-1365</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1406,14 +1433,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1710,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView topLeftCell="I39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L47" sqref="L2:L47"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2567,7 +2593,7 @@
       <c r="L27"/>
     </row>
     <row r="28" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="8" t="s">
         <v>142</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -3174,8 +3200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="I44" workbookViewId="0">
-      <selection activeCell="L51" sqref="L2:L51"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4211,47 +4237,47 @@
     </row>
     <row r="34" spans="1:12" ht="45">
       <c r="A34" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>393</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>394</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:12" ht="30">
       <c r="A35" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>334</v>
+        <v>347</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>333</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>16</v>
@@ -4261,28 +4287,28 @@
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:12" ht="30">
       <c r="A36" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>335</v>
+        <v>348</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>334</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>16</v>
@@ -4292,22 +4318,22 @@
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>341</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>342</v>
       </c>
       <c r="K36" s="8"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>337</v>
+        <v>349</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>336</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>14</v>
@@ -4319,7 +4345,7 @@
         <v>19</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
@@ -4327,7 +4353,7 @@
         <v>185</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K37" s="8"/>
     </row>
@@ -4336,7 +4362,7 @@
         <v>263</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>14</v>
@@ -4534,7 +4560,7 @@
     </row>
     <row r="45" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A45" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>52</v>
@@ -4553,7 +4579,7 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>263</v>
@@ -4568,16 +4594,16 @@
     </row>
     <row r="46" spans="1:12" ht="30">
       <c r="A46" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>334</v>
+        <v>388</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>333</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>16</v>
@@ -4587,52 +4613,52 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K46" s="8"/>
     </row>
     <row r="47" spans="1:12" ht="30">
       <c r="A47" t="s">
-        <v>390</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>336</v>
+        <v>389</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>335</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="30">
       <c r="A48" t="s">
+        <v>407</v>
+      </c>
+      <c r="B48" s="13" t="s">
         <v>408</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>409</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>14</v>
@@ -4644,15 +4670,15 @@
         <v>16</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>38</v>
@@ -4660,39 +4686,39 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>410</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>411</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K49" s="8"/>
     </row>
     <row r="50" spans="1:11" ht="60">
       <c r="A50" t="s">
-        <v>415</v>
-      </c>
-      <c r="B50" s="14" t="s">
         <v>414</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>413</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>14</v>
@@ -4704,17 +4730,17 @@
         <v>16</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="J50" s="5" t="s">
         <v>419</v>
-      </c>
-      <c r="I50" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>420</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>38</v>
@@ -4722,30 +4748,30 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>416</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>417</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K51" s="8"/>
     </row>
@@ -4756,10 +4782,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L2:L19"/>
+    <sheetView topLeftCell="I15" workbookViewId="0">
+      <selection activeCell="L22" sqref="L2:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4817,10 +4843,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
@@ -4838,7 +4864,7 @@
         <v>315</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K2" t="s">
         <v>38</v>
@@ -4846,10 +4872,10 @@
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -4872,7 +4898,7 @@
     </row>
     <row r="4" spans="1:12" ht="75">
       <c r="A4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>317</v>
@@ -4890,10 +4916,10 @@
         <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>327</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>328</v>
       </c>
       <c r="K4" t="s">
         <v>38</v>
@@ -4901,30 +4927,30 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="75">
       <c r="A6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>318</v>
@@ -4941,28 +4967,28 @@
       <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>366</v>
+      <c r="H6" s="14" t="s">
+        <v>365</v>
       </c>
       <c r="I6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>371</v>
-      </c>
-      <c r="B7" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>319</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
@@ -4974,17 +5000,17 @@
         <v>322</v>
       </c>
       <c r="I7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>372</v>
-      </c>
-      <c r="B8" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>320</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -5000,276 +5026,270 @@
         <v>27</v>
       </c>
       <c r="I8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
-      <c r="A9" t="s">
-        <v>374</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>373</v>
+      <c r="A9" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>427</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>324</v>
+        <v>423</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G9" t="s">
-        <v>356</v>
+      <c r="F9" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>357</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>375</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>325</v>
+        <v>373</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>372</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>358</v>
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>355</v>
       </c>
       <c r="I10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="K10" t="s">
-        <v>38</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
+        <v>374</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="I11" t="s">
+        <v>351</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" t="s">
+        <v>381</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>352</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>374</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45">
+      <c r="A13" t="s">
         <v>382</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>353</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>375</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="45">
-      <c r="A12" t="s">
-        <v>383</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>367</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" t="s">
-        <v>365</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30">
-      <c r="A13" t="s">
-        <v>384</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>321</v>
+      <c r="B13" s="13" t="s">
+        <v>329</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>329</v>
+        <v>27</v>
       </c>
       <c r="I13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>385</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>331</v>
+        <v>383</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>321</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J14" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>366</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="I15" t="s">
+        <v>364</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45">
-      <c r="A15" t="s">
-        <v>386</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="16" spans="1:12" ht="45">
+      <c r="A16" t="s">
+        <v>385</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="45">
-      <c r="A16" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>387</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="16" t="s">
+      <c r="H16" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="45">
+      <c r="A17" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" ht="60">
-      <c r="A17" t="s">
-        <v>388</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="30">
-      <c r="A18" s="13" t="s">
-        <v>401</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>334</v>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:11" ht="60">
+      <c r="A18" t="s">
+        <v>387</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>332</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>379</v>
+      <c r="D18" t="s">
+        <v>15</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>16</v>
@@ -5277,46 +5297,124 @@
       <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="I18" t="s">
-        <v>375</v>
+      <c r="H18" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>374</v>
       </c>
       <c r="J18" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" ht="30">
-      <c r="A19" t="s">
-        <v>402</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>394</v>
+        <v>23</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>395</v>
+        <v>338</v>
       </c>
       <c r="I19" t="s">
+        <v>374</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="30">
+      <c r="A20" t="s">
         <v>401</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>380</v>
+      <c r="B20" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="I20" t="s">
+        <v>400</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" t="s">
+        <v>430</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>423</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45">
+      <c r="A22" t="s">
+        <v>431</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>323</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Authoring: Removed hard coding article ids with searched result article ids.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="438">
   <si>
     <t>GET</t>
   </si>
@@ -717,69 +717,12 @@
     <t>/statistics/posts</t>
   </si>
   <si>
-    <t>?id=468387744WOS1</t>
-  </si>
-  <si>
-    <t>/comments/count/468387744WOS1/</t>
-  </si>
-  <si>
-    <t>/comments/count/468387744WOS1/wos</t>
-  </si>
-  <si>
     <t>/statistics/wos</t>
   </si>
   <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"mohana.yalamarthi@thomsonreuters.com        http://thomsonreuters.com/en.html         +91 8197818719"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"FUCK"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=****</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=****</t>
-  </si>
-  <si>
-    <t>status=200||size=(OPQA-331_counterValue)||found=true||comments.targetType=wos||comments.targetId=468387744WOS1</t>
-  </si>
-  <si>
     <t>{"targetType":"wos","targetId":"233726479WOS1","content":"Testing Error status 500"}</t>
   </si>
   <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"hi"}</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Edited content"}</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-315_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=468387744WOS1||id=(OPQA-245_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>/comments/468387744WOS1/wos</t>
-  </si>
-  <si>
-    <t>status=200||found=true||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Comment report tesintg"}</t>
-  </si>
-  <si>
     <t>{"title":"Post Test 333 From API User2","content":"Post content creation from API Automation Script  by User2"}</t>
   </si>
   <si>
@@ -900,33 +843,6 @@
     <t>{"content":"This is a Editing the deleted Post by API Authorized User1", "title":"API Edited Title222"}</t>
   </si>
   <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Comment test from API by User 1"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Comment test from API by User 1</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Comment test from API by User 1 and Created within 60 sec of previous comment"}</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Wrong data test : server error expectation"}</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while creating comment by User 1&lt;abcd&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=468387744WOS1||comments.content=Tags clean up surround tags like abcd while creating comment by User 1</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while editing comment by User 1&lt;abcd&gt;"}</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"Update own comment"}</t>
-  </si>
-  <si>
-    <t>status=200||content=Update own comment||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
     <t>{"targetType":"posts","targetId":"(OPQA-360_id)","content":"Comment Test on own Post:: Post Test 222 From API User1"}</t>
   </si>
   <si>
@@ -951,15 +867,6 @@
     <t>/comments/comment?id=(OPQA-236_comments.id)a</t>
   </si>
   <si>
-    <t>status=200||content=Tags clean up surround tags like abcd while editing comment by User 1||targetType=wos||targetId=468387744WOS1||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"468387744WOS1","content":"HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=468387744WOS1||content=HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>/drafts</t>
   </si>
   <si>
@@ -1312,13 +1219,124 @@
   </si>
   <si>
     <t>OPQA-1365</t>
+  </si>
+  <si>
+    <t>Verify that to get articles for query</t>
+  </si>
+  <si>
+    <t>1PSEARCHV3</t>
+  </si>
+  <si>
+    <t>/wos/search</t>
+  </si>
+  <si>
+    <t>?query=biology</t>
+  </si>
+  <si>
+    <t>hits.hits[0]._id||hits.hits[1]._id</t>
+  </si>
+  <si>
+    <t>OPQA-896_1</t>
+  </si>
+  <si>
+    <t>/comments/count/(OPQA-896_1_hits.hits[0]._id)/wos</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-896_1_hits.hits[0]._id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment test from API by User 1"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=Comment test from API by User 1</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment test from API by User 1 and Created within 60 sec of previous comment"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"mohana.yalamarthi@thomsonreuters.com        http://thomsonreuters.com/en.html         +91 8197818719"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Wrong data test : server error expectation"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while creating comment by User 1&lt;abcd&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=Tags clean up surround tags like abcd while creating comment by User 1</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while editing comment by User 1&lt;abcd&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||content=Tags clean up surround tags like abcd while editing comment by User 1||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"FUCK"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=****</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||content=****</t>
+  </si>
+  <si>
+    <t>status=200||size=(OPQA-331_counterValue)||found=true||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Update own comment"}</t>
+  </si>
+  <si>
+    <t>status=200||content=Update own comment||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Edited content"}</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-236_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-315_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||content=HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-245_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"hi"}</t>
+  </si>
+  <si>
+    <t>/comments/count/(OPQA-896_1_hits.hits[0]._id)/</t>
+  </si>
+  <si>
+    <t>/comments/(OPQA-896_1_hits.hits[0]._id)/wos</t>
+  </si>
+  <si>
+    <t>status=200||found=true||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment report tesintg"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1347,6 +1365,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1400,10 +1425,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1440,8 +1469,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1734,10 +1769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1794,100 +1829,102 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="2" spans="1:12" s="17" customFormat="1" ht="45">
       <c r="A2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="3" t="s">
+      <c r="F2"/>
+      <c r="G2" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="H2" s="16"/>
+      <c r="I2"/>
+      <c r="J2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>24</v>
+      <c r="K2" s="16" t="s">
+        <v>405</v>
       </c>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A3" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>236</v>
+      <c r="D3" s="8" t="s">
+        <v>407</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A4" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
+      <c r="E4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3"/>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="45">
-      <c r="A4" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="K4" s="8"/>
       <c r="L4"/>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A5" s="8" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -1903,21 +1940,25 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="3"/>
+        <v>409</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="L5"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A6" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
@@ -1929,27 +1970,27 @@
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="I6" s="3"/>
+      <c r="H6" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>406</v>
+      </c>
       <c r="J6" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="K6" s="3"/>
       <c r="L6"/>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A7" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
@@ -1961,25 +2002,29 @@
         <v>16</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="I7" s="3"/>
+      <c r="H7" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>406</v>
+      </c>
       <c r="J7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="3"/>
+        <v>413</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A8" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>47</v>
+        <v>112</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
@@ -1991,31 +2036,33 @@
         <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="5" t="s">
-        <v>299</v>
+        <v>414</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A9" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>97</v>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>16</v>
@@ -2023,31 +2070,31 @@
       <c r="F9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="K9" s="8"/>
+        <v>415</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="K9" s="3"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A10" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
+      <c r="D10" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>16</v>
@@ -2055,29 +2102,31 @@
       <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="K10" s="3"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="K10" s="8"/>
       <c r="L10"/>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A11" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>97</v>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
@@ -2087,57 +2136,61 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>96</v>
+        <v>419</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>406</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>241</v>
+        <v>420</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11"/>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A12" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>31</v>
+      <c r="D12" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="K12" s="3"/>
       <c r="L12"/>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A13" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>0</v>
@@ -2146,56 +2199,54 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="K13" s="8"/>
+      <c r="J13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A14" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>98</v>
+      <c r="D14" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>25</v>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>422</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" ht="45">
+    <row r="15" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A15" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>69</v>
+        <v>122</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>309</v>
+        <v>98</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
@@ -2204,30 +2255,30 @@
         <v>21</v>
       </c>
       <c r="G15" s="8"/>
-      <c r="H15" s="5" t="s">
-        <v>243</v>
+      <c r="H15" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K15" s="8"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="16" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A16" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>48</v>
+        <v>123</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>97</v>
+        <v>281</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>16</v>
@@ -2237,23 +2288,23 @@
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="5" t="s">
-        <v>301</v>
+        <v>234</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>302</v>
+      <c r="J16" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16"/>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A17" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -2265,65 +2316,65 @@
         <v>16</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="4" t="s">
-        <v>245</v>
+        <v>21</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="5" t="s">
+        <v>423</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="3"/>
+      <c r="J17" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="K17" s="8"/>
       <c r="L17"/>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="4" t="s">
-        <v>17</v>
+        <v>425</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J18" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="K18" s="8"/>
+      <c r="J18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="3"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" ht="45">
+    <row r="19" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>16</v>
@@ -2336,120 +2387,120 @@
         <v>17</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19"/>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A20" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>29</v>
+        <v>106</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="21" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A21" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="H21" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I21" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>101</v>
+      <c r="J21" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="K21" s="8"/>
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A22" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>76</v>
+        <v>131</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="H22" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="H22" s="8"/>
       <c r="I22" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K22" s="8"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" s="2" customFormat="1" ht="45">
+    <row r="23" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A23" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>16</v>
@@ -2462,50 +2513,52 @@
         <v>18</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K23" s="8"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="24" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A24" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="H24" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I24" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>29</v>
+        <v>106</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="K24" s="8"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" ht="45">
+    <row r="25" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A25" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>14</v>
@@ -2517,22 +2570,22 @@
         <v>19</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>246</v>
+      <c r="J25" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="K25" s="8"/>
       <c r="L25"/>
     </row>
     <row r="26" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A26" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>75</v>
@@ -2541,69 +2594,67 @@
         <v>14</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>247</v>
+        <v>426</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="27" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A27" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="K27" s="8"/>
+      <c r="L27"/>
+    </row>
+    <row r="28" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A28" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="C28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A28" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>16</v>
@@ -2613,23 +2664,25 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>139</v>
+        <v>428</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>406</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="K28" s="3"/>
+        <v>429</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="L28"/>
     </row>
     <row r="29" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A29" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>75</v>
+        <v>142</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>14</v>
@@ -2638,34 +2691,36 @@
         <v>140</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="5" t="s">
+        <v>430</v>
+      </c>
       <c r="I29" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J29" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="K29" s="8"/>
+      <c r="J29" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="K29" s="3"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="30" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A30" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>19</v>
@@ -2675,21 +2730,21 @@
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>25</v>
+      <c r="I30" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>432</v>
       </c>
       <c r="K30" s="8"/>
       <c r="L30"/>
     </row>
     <row r="31" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A31" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
@@ -2698,15 +2753,13 @@
         <v>97</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G31" s="8"/>
-      <c r="H31" s="5" t="s">
-        <v>244</v>
-      </c>
+      <c r="H31" s="8"/>
       <c r="I31" s="8" t="s">
         <v>135</v>
       </c>
@@ -2718,16 +2771,16 @@
     </row>
     <row r="32" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A32" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>16</v>
@@ -2736,8 +2789,8 @@
         <v>21</v>
       </c>
       <c r="G32" s="8"/>
-      <c r="H32" s="4" t="s">
-        <v>17</v>
+      <c r="H32" s="5" t="s">
+        <v>433</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>135</v>
@@ -2750,10 +2803,10 @@
     </row>
     <row r="33" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A33" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>14</v>
@@ -2769,55 +2822,61 @@
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J33" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K33" s="8"/>
       <c r="L33"/>
     </row>
-    <row r="34" spans="1:12" s="2" customFormat="1" ht="45">
+    <row r="34" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A34" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="8"/>
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A35" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K34" s="3"/>
-      <c r="L34"/>
-    </row>
-    <row r="35" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A35" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="C35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>251</v>
+        <v>434</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
@@ -2825,25 +2884,27 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="I35" s="8" t="s">
+        <v>406</v>
+      </c>
       <c r="J35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K35" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="K35" s="3"/>
       <c r="L35"/>
     </row>
-    <row r="36" spans="1:12" s="2" customFormat="1" ht="45">
+    <row r="36" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A36" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>160</v>
+      <c r="D36" s="3" t="s">
+        <v>435</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>0</v>
@@ -2851,38 +2912,36 @@
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="3" t="s">
-        <v>118</v>
+      <c r="I36" s="8" t="s">
+        <v>406</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K36" s="8"/>
       <c r="L36"/>
     </row>
     <row r="37" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A37" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>310</v>
+        <v>160</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F37" s="8"/>
-      <c r="G37" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="3" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>29</v>
@@ -2892,25 +2951,27 @@
     </row>
     <row r="38" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A38" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>161</v>
+        <v>282</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
+      <c r="G38" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H38" s="8"/>
       <c r="I38" s="3" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>29</v>
@@ -2918,18 +2979,18 @@
       <c r="K38" s="8"/>
       <c r="L38"/>
     </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="39" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A39" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>68</v>
+        <v>159</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>251</v>
+      <c r="D39" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>0</v>
@@ -2937,111 +2998,111 @@
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
+      <c r="I39" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="J39" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="K39" s="8"/>
       <c r="L39"/>
     </row>
     <row r="40" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A40" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>162</v>
+        <v>228</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>103</v>
+      <c r="D40" s="3" t="s">
+        <v>435</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>252</v>
+      <c r="I40" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="K40" s="8"/>
       <c r="L40"/>
     </row>
-    <row r="41" spans="1:12" s="2" customFormat="1" ht="45">
+    <row r="41" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A41" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="K41" s="8"/>
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A42" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B42" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="C42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="4" t="s">
+      <c r="E42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="I41" s="8"/>
-      <c r="J41" s="4" t="s">
+      <c r="G42" s="3"/>
+      <c r="H42" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K41" s="3" t="s">
+      <c r="K42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L41"/>
-    </row>
-    <row r="42" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A42" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K42" s="8"/>
       <c r="L42"/>
     </row>
     <row r="43" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A43" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>50</v>
+        <v>171</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
@@ -3057,29 +3118,29 @@
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J43" s="5" t="s">
-        <v>166</v>
+      <c r="J43" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="K43" s="8"/>
       <c r="L43"/>
     </row>
     <row r="44" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A44" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>16</v>
@@ -3088,107 +3149,141 @@
         <v>23</v>
       </c>
       <c r="G44" s="8"/>
-      <c r="H44" s="12" t="s">
-        <v>34</v>
+      <c r="H44" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>164</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44"/>
     </row>
-    <row r="45" spans="1:12" s="2" customFormat="1" ht="45">
+    <row r="45" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A45" s="8" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
+      <c r="H45" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="I45" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J45" s="4" t="s">
-        <v>11</v>
+      <c r="J45" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="K45" s="8"/>
       <c r="L45"/>
     </row>
-    <row r="46" spans="1:12" s="2" customFormat="1" ht="30">
+    <row r="46" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A46" s="8" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G46" s="8"/>
-      <c r="H46" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="H46" s="8"/>
       <c r="I46" s="3" t="s">
         <v>164</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="K46" s="8"/>
       <c r="L46"/>
     </row>
     <row r="47" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A47" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="8"/>
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="1:12" s="2" customFormat="1" ht="30">
+      <c r="A48" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B48" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="C48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="3" t="s">
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="K48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L47"/>
+      <c r="L48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3200,7 +3295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
@@ -3279,7 +3374,7 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="5" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="4" t="s">
@@ -3311,7 +3406,7 @@
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="5" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="5" t="s">
@@ -3465,7 +3560,7 @@
         <v>177</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="K8" s="8"/>
       <c r="L8"/>
@@ -3521,13 +3616,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="5" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="K10" s="8"/>
       <c r="L10"/>
@@ -3553,7 +3648,7 @@
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="5" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>177</v>
@@ -3584,13 +3679,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="5" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>185</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12"/>
@@ -3616,13 +3711,13 @@
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="5" t="s">
-        <v>303</v>
+        <v>275</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>304</v>
+        <v>276</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>20</v>
@@ -3649,13 +3744,13 @@
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="5" t="s">
-        <v>305</v>
+        <v>277</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>20</v>
@@ -3689,7 +3784,7 @@
         <v>177</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="K15" s="8"/>
     </row>
@@ -3720,7 +3815,7 @@
         <v>185</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16"/>
@@ -3816,7 +3911,7 @@
         <v>185</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19"/>
@@ -3842,7 +3937,7 @@
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="5" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="4" t="s">
@@ -4043,7 +4138,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>0</v>
@@ -4055,7 +4150,7 @@
         <v>177</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="K27" s="8"/>
     </row>
@@ -4070,7 +4165,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>0</v>
@@ -4082,7 +4177,7 @@
         <v>185</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="K28" s="8"/>
     </row>
@@ -4111,7 +4206,7 @@
         <v>177</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="K29" s="8"/>
     </row>
@@ -4140,7 +4235,7 @@
         <v>185</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="K30" s="8"/>
     </row>
@@ -4208,7 +4303,7 @@
     </row>
     <row r="33" spans="1:12" ht="45">
       <c r="A33" s="8" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>75</v>
@@ -4217,7 +4312,7 @@
         <v>14</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>19</v>
@@ -4237,47 +4332,47 @@
     </row>
     <row r="34" spans="1:12" ht="45">
       <c r="A34" s="8" t="s">
-        <v>406</v>
+        <v>375</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>391</v>
+        <v>360</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>392</v>
+        <v>361</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:12" ht="30">
       <c r="A35" s="8" t="s">
-        <v>347</v>
+        <v>316</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>333</v>
+        <v>302</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>337</v>
+        <v>306</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>16</v>
@@ -4287,28 +4382,28 @@
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>338</v>
+        <v>307</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>339</v>
+        <v>308</v>
       </c>
       <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:12" ht="30">
       <c r="A36" s="8" t="s">
-        <v>348</v>
+        <v>317</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>337</v>
+        <v>306</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>16</v>
@@ -4318,22 +4413,22 @@
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
-        <v>340</v>
+        <v>309</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>347</v>
+        <v>316</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>341</v>
+        <v>310</v>
       </c>
       <c r="K36" s="8"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="8" t="s">
-        <v>349</v>
+        <v>318</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>336</v>
+        <v>305</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>14</v>
@@ -4345,7 +4440,7 @@
         <v>19</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>328</v>
+        <v>297</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
@@ -4353,22 +4448,22 @@
         <v>185</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>343</v>
+        <v>312</v>
       </c>
       <c r="K37" s="8"/>
     </row>
     <row r="38" spans="1:12" ht="30">
       <c r="A38" s="8" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>390</v>
+        <v>359</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>19</v>
@@ -4382,48 +4477,48 @@
         <v>177</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="K38" s="8"/>
     </row>
     <row r="39" spans="1:12" ht="30">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30">
       <c r="A40" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>19</v>
@@ -4434,18 +4529,18 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="3" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>14</v>
@@ -4461,10 +4556,10 @@
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="5" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>25</v>
@@ -4472,16 +4567,16 @@
     </row>
     <row r="42" spans="1:12" ht="30">
       <c r="A42" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>19</v>
@@ -4495,15 +4590,15 @@
         <v>177</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
@@ -4522,7 +4617,7 @@
         <v>17</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>25</v>
@@ -4530,10 +4625,10 @@
     </row>
     <row r="44" spans="1:12" ht="45">
       <c r="A44" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>14</v>
@@ -4552,7 +4647,7 @@
         <v>18</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>25</v>
@@ -4560,7 +4655,7 @@
     </row>
     <row r="45" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A45" s="8" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>52</v>
@@ -4579,10 +4674,10 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="5" t="s">
-        <v>397</v>
+        <v>366</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>37</v>
@@ -4594,16 +4689,16 @@
     </row>
     <row r="46" spans="1:12" ht="30">
       <c r="A46" s="8" t="s">
-        <v>388</v>
+        <v>357</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>333</v>
+        <v>302</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>398</v>
+        <v>367</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>16</v>
@@ -4613,52 +4708,52 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
-        <v>338</v>
+        <v>307</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>403</v>
+        <v>372</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>399</v>
+        <v>368</v>
       </c>
       <c r="K46" s="8"/>
     </row>
     <row r="47" spans="1:12" ht="30">
       <c r="A47" t="s">
-        <v>389</v>
+        <v>358</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>335</v>
+        <v>304</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>404</v>
+        <v>373</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>388</v>
+        <v>357</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="30">
       <c r="A48" t="s">
-        <v>407</v>
+        <v>376</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>408</v>
+        <v>377</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>14</v>
@@ -4670,15 +4765,15 @@
         <v>16</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="5" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="5" t="s">
-        <v>421</v>
+        <v>390</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>38</v>
@@ -4686,39 +4781,39 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="8" t="s">
-        <v>409</v>
+        <v>378</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>336</v>
+        <v>305</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>410</v>
+        <v>379</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>411</v>
+        <v>380</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" t="s">
-        <v>407</v>
+        <v>376</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>412</v>
+        <v>381</v>
       </c>
       <c r="K49" s="8"/>
     </row>
     <row r="50" spans="1:11" ht="60">
       <c r="A50" t="s">
-        <v>414</v>
+        <v>383</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>413</v>
+        <v>382</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>14</v>
@@ -4730,17 +4825,17 @@
         <v>16</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="5" t="s">
-        <v>418</v>
+        <v>387</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>409</v>
+        <v>378</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>419</v>
+        <v>388</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>38</v>
@@ -4748,30 +4843,30 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="8" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>336</v>
+        <v>305</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>416</v>
+        <v>385</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>411</v>
+        <v>380</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" t="s">
-        <v>414</v>
+        <v>383</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>417</v>
+        <v>386</v>
       </c>
       <c r="K51" s="8"/>
     </row>
@@ -4784,8 +4879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="I15" workbookViewId="0">
-      <selection activeCell="L22" sqref="L2:L22"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4843,16 +4938,16 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>350</v>
+        <v>319</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>16</v>
@@ -4861,10 +4956,10 @@
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>315</v>
+        <v>284</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>344</v>
+        <v>313</v>
       </c>
       <c r="K2" t="s">
         <v>38</v>
@@ -4872,16 +4967,16 @@
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>363</v>
+        <v>332</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>362</v>
+        <v>331</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
@@ -4890,7 +4985,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>316</v>
+        <v>285</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>26</v>
@@ -4898,16 +4993,16 @@
     </row>
     <row r="4" spans="1:12" ht="75">
       <c r="A4" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>286</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>16</v>
@@ -4916,10 +5011,10 @@
         <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>425</v>
+        <v>394</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>327</v>
+        <v>296</v>
       </c>
       <c r="K4" t="s">
         <v>38</v>
@@ -4927,39 +5022,39 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>368</v>
+        <v>337</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>367</v>
+        <v>336</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>353</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="75">
       <c r="A6" t="s">
-        <v>369</v>
+        <v>338</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>318</v>
+        <v>287</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>326</v>
+        <v>295</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
@@ -4968,27 +5063,27 @@
         <v>23</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>365</v>
+        <v>334</v>
       </c>
       <c r="I6" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>346</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>370</v>
+        <v>339</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>319</v>
+        <v>288</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
@@ -4997,27 +5092,27 @@
         <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>322</v>
+        <v>291</v>
       </c>
       <c r="I7" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>354</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>371</v>
+        <v>340</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>323</v>
+        <v>292</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>0</v>
@@ -5026,24 +5121,24 @@
         <v>27</v>
       </c>
       <c r="I8" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>345</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="15" t="s">
-        <v>429</v>
+        <v>398</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>427</v>
+        <v>396</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>423</v>
+        <v>392</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>0</v>
@@ -5052,50 +5147,50 @@
         <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>428</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>373</v>
+        <v>342</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>372</v>
+        <v>341</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>324</v>
+        <v>293</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>355</v>
+        <v>324</v>
       </c>
       <c r="I10" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>356</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>374</v>
+        <v>343</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>325</v>
+        <v>294</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>326</v>
+        <v>295</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
@@ -5104,13 +5199,13 @@
         <v>21</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>357</v>
+        <v>326</v>
       </c>
       <c r="I11" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>358</v>
+        <v>327</v>
       </c>
       <c r="K11" t="s">
         <v>38</v>
@@ -5118,39 +5213,39 @@
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>381</v>
+        <v>350</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>380</v>
+        <v>349</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>374</v>
+        <v>343</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>359</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45">
       <c r="A13" t="s">
-        <v>382</v>
+        <v>351</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>329</v>
+        <v>298</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>366</v>
+        <v>335</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>19</v>
@@ -5159,7 +5254,7 @@
         <v>27</v>
       </c>
       <c r="I13" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>29</v>
@@ -5167,25 +5262,25 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>383</v>
+        <v>352</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>321</v>
+        <v>290</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>366</v>
+        <v>335</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>328</v>
+        <v>297</v>
       </c>
       <c r="I14" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>11</v>
@@ -5193,25 +5288,25 @@
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" t="s">
-        <v>384</v>
+        <v>353</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>330</v>
+        <v>299</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>366</v>
+        <v>335</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>328</v>
+        <v>297</v>
       </c>
       <c r="I15" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>25</v>
@@ -5219,10 +5314,10 @@
     </row>
     <row r="16" spans="1:12" ht="45">
       <c r="A16" t="s">
-        <v>385</v>
+        <v>354</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>331</v>
+        <v>300</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
@@ -5237,13 +5332,13 @@
         <v>23</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>375</v>
+        <v>344</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>374</v>
+        <v>343</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>360</v>
+        <v>329</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>20</v>
@@ -5251,7 +5346,7 @@
     </row>
     <row r="17" spans="1:11" ht="45">
       <c r="A17" s="8" t="s">
-        <v>342</v>
+        <v>311</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>75</v>
@@ -5260,7 +5355,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>386</v>
+        <v>355</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>19</v>
@@ -5271,7 +5366,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="15" t="s">
-        <v>385</v>
+        <v>354</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>11</v>
@@ -5280,10 +5375,10 @@
     </row>
     <row r="18" spans="1:11" ht="60">
       <c r="A18" t="s">
-        <v>387</v>
+        <v>356</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>332</v>
+        <v>301</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
@@ -5298,13 +5393,13 @@
         <v>23</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>376</v>
+        <v>345</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>374</v>
+        <v>343</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>361</v>
+        <v>330</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>20</v>
@@ -5312,16 +5407,16 @@
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" s="8" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>333</v>
+        <v>302</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>378</v>
+        <v>347</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>16</v>
@@ -5331,90 +5426,90 @@
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>338</v>
+        <v>307</v>
       </c>
       <c r="I19" t="s">
-        <v>374</v>
+        <v>343</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>377</v>
+        <v>346</v>
       </c>
       <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="30">
       <c r="A20" t="s">
-        <v>401</v>
+        <v>370</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>335</v>
+        <v>304</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>405</v>
+        <v>374</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="I20" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>379</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>424</v>
+        <v>393</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>423</v>
+        <v>392</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>328</v>
+        <v>297</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>422</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45">
       <c r="A22" t="s">
-        <v>431</v>
+        <v>400</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>426</v>
+        <v>395</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>323</v>
+        <v>292</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>328</v>
+        <v>297</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>422</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed authoring test cases and added STeAM pending test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="456">
   <si>
     <t>GET</t>
   </si>
@@ -885,9 +885,6 @@
     <t>Verfiy that user is able to access and edit the draft posts from their profile</t>
   </si>
   <si>
-    <t>Verfiy that the Drafts Post tab displays the count of the saved posts correctly</t>
-  </si>
-  <si>
     <t>Verfiy that user is able to delete the draft post from the list in their profile</t>
   </si>
   <si>
@@ -960,9 +957,6 @@
     <t>status=200||userId=(SYS_USER1)||title=Draft Post 1 by Neon User1||content=""||found=true</t>
   </si>
   <si>
-    <t>status=200||id=(SYS_USER1)||type=User||counterName=draftCountForUser||counterValue=2</t>
-  </si>
-  <si>
     <t>status=200||userId=(SYS_USER2)||title=Draft Post 2 From API||content=Draft Post 2 creation by API. it shouldn't be published. This draft must check spam and profanity example is ***** and **** words shouldn't be allowed. Also should not allow unsupported html tags like Tags clean up surround tags like abcd while creating draft ||found=true||wasCleanedUp=3</t>
   </si>
   <si>
@@ -1209,9 +1203,6 @@
     <t>Verify that for the given truid, API is able to get all the draft posts.</t>
   </si>
   <si>
-    <t>status=200||size=2||found=true||drafts[0].userId=(SYS_USER1)||drafts[0].id=(OPQA-1078_id)</t>
-  </si>
-  <si>
     <t>OPQA-1363</t>
   </si>
   <si>
@@ -1330,6 +1321,69 @@
   </si>
   <si>
     <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment report tesintg"}</t>
+  </si>
+  <si>
+    <t>Verfiy that the Drafts Post tab displays the count of the saved drafts correctly</t>
+  </si>
+  <si>
+    <t>status=200||id=(SYS_USER1)||type=User||counterName=draftCountForUser</t>
+  </si>
+  <si>
+    <t>OPQA-1085_1</t>
+  </si>
+  <si>
+    <t>OPQA-1078||OPQA-1085</t>
+  </si>
+  <si>
+    <t>status=200||id=(SYS_USER1)||type=User||counterName=draftCountForUser||counterValue=eval$(OPQA-1085_counterValue)+1</t>
+  </si>
+  <si>
+    <t>status=200||size=eval$(OPQA-1085_counterValue)+1||found=true||drafts[0].userId=(SYS_USER1)||drafts[0].id=(OPQA-1078_id)</t>
+  </si>
+  <si>
+    <t>OPQA-682</t>
+  </si>
+  <si>
+    <t>Verify that API truncated the comment length to 2500 characters while creating/Editing the comment</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment Max Length Test: As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher,&gt;1500I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge...! &gt;2500"}</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-682_comments.id)</t>
+  </si>
+  <si>
+    <t>OPQA-286_6</t>
+  </si>
+  <si>
+    <t>OPQA-360||OPQA-286_4</t>
+  </si>
+  <si>
+    <t>OPQA-344_1||OPQA-286_3</t>
+  </si>
+  <si>
+    <t>OPQA-896_1||OPQA-286</t>
+  </si>
+  <si>
+    <t>OPQA-896_1||OPQA-286_2</t>
+  </si>
+  <si>
+    <t>OPQA-360||OPQA-286_1</t>
+  </si>
+  <si>
+    <t>OPQA-1087||OPQA-286_5</t>
+  </si>
+  <si>
+    <t>OPQA-286_7</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-1093_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||size=eval$(OPQA-344_1_counterValue)+1||comments.userId=(SYS_USER1)||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.targetType=wos||comments.content=Comment Max Length Test: As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher,&gt;1500I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge...!||comments.wasTruncated=true</t>
+  </si>
+  <si>
+    <t>OPQA-1087||OPQA-286_6</t>
   </si>
 </sst>
 </file>
@@ -1769,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L48"/>
+    <sheetView tabSelected="1" topLeftCell="J48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L50" sqref="L2:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1785,8 +1839,8 @@
     <col min="6" max="6" width="47.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="68.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="119.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="119.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -1816,10 +1870,10 @@
       <c r="H1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="10" t="s">
@@ -1831,31 +1885,31 @@
     </row>
     <row r="2" spans="1:12" s="17" customFormat="1" ht="45">
       <c r="A2" s="8" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="16" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="H2" s="16"/>
-      <c r="I2"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="L2"/>
     </row>
@@ -1870,7 +1924,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
@@ -1878,10 +1932,10 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -1907,13 +1961,13 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H4" s="8"/>
-      <c r="I4" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>93</v>
       </c>
       <c r="K4" s="8"/>
@@ -1940,13 +1994,13 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="I5" s="8" t="s">
         <v>406</v>
       </c>
+      <c r="I5" s="5" t="s">
+        <v>403</v>
+      </c>
       <c r="J5" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>20</v>
@@ -1974,10 +2028,10 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>406</v>
+        <v>408</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>403</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>26</v>
@@ -2006,13 +2060,13 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>406</v>
+        <v>409</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>403</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>20</v>
@@ -2040,10 +2094,10 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>406</v>
+        <v>411</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>403</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>29</v>
@@ -2072,13 +2126,13 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>406</v>
+        <v>412</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>403</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9"/>
@@ -2104,13 +2158,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="I10" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>418</v>
+      <c r="J10" s="5" t="s">
+        <v>415</v>
       </c>
       <c r="K10" s="8"/>
       <c r="L10"/>
@@ -2136,13 +2190,13 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>406</v>
+        <v>416</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>403</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11"/>
@@ -2168,13 +2222,13 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="I12" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>96</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12"/>
@@ -2198,8 +2252,8 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="3" t="s">
+      <c r="I13" s="5"/>
+      <c r="J13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="3" t="s">
@@ -2226,11 +2280,11 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>422</v>
+      <c r="I14" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>419</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14"/>
@@ -2258,10 +2312,10 @@
       <c r="H15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K15" s="8"/>
@@ -2290,10 +2344,10 @@
       <c r="H16" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K16" s="8"/>
@@ -2320,13 +2374,13 @@
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="I17" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>424</v>
+      <c r="J17" s="5" t="s">
+        <v>421</v>
       </c>
       <c r="K17" s="8"/>
       <c r="L17"/>
@@ -2352,9 +2406,9 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="I18" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>96</v>
       </c>
       <c r="J18" s="4" t="s">
@@ -2386,10 +2440,10 @@
       <c r="H19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="5" t="s">
         <v>99</v>
       </c>
       <c r="K19" s="8"/>
@@ -2418,10 +2472,10 @@
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="5" t="s">
         <v>108</v>
       </c>
       <c r="K20" s="8"/>
@@ -2450,10 +2504,10 @@
       <c r="H21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K21" s="8"/>
@@ -2480,10 +2534,10 @@
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="5" t="s">
         <v>101</v>
       </c>
       <c r="K22" s="8"/>
@@ -2512,10 +2566,10 @@
       <c r="H23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="5" t="s">
         <v>102</v>
       </c>
       <c r="K23" s="8"/>
@@ -2544,10 +2598,10 @@
       <c r="H24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="5" t="s">
         <v>109</v>
       </c>
       <c r="K24" s="8"/>
@@ -2574,10 +2628,10 @@
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K25" s="8"/>
@@ -2604,11 +2658,11 @@
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J26" s="8" t="s">
-        <v>426</v>
+      <c r="J26" s="5" t="s">
+        <v>423</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26"/>
@@ -2634,11 +2688,11 @@
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>427</v>
+      <c r="J27" s="5" t="s">
+        <v>424</v>
       </c>
       <c r="K27" s="8"/>
       <c r="L27"/>
@@ -2664,13 +2718,13 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>406</v>
+        <v>425</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>448</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>20</v>
@@ -2698,13 +2752,13 @@
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="I29" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>139</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29"/>
@@ -2730,11 +2784,11 @@
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="J30" s="8" t="s">
-        <v>432</v>
+      <c r="J30" s="5" t="s">
+        <v>429</v>
       </c>
       <c r="K30" s="8"/>
       <c r="L30"/>
@@ -2760,7 +2814,7 @@
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
-      <c r="I31" s="8" t="s">
+      <c r="I31" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J31" s="4" t="s">
@@ -2790,9 +2844,9 @@
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="I32" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J32" s="4" t="s">
@@ -2824,7 +2878,7 @@
       <c r="H33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J33" s="4" t="s">
@@ -2856,10 +2910,10 @@
       <c r="H34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="J34" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K34" s="8"/>
@@ -2876,7 +2930,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
@@ -2884,10 +2938,10 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="J35" s="3" t="s">
+      <c r="I35" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K35" s="3"/>
@@ -2904,7 +2958,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>0</v>
@@ -2912,10 +2966,10 @@
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="J36" s="3" t="s">
+      <c r="I36" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K36" s="8"/>
@@ -2940,10 +2994,10 @@
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="3" t="s">
+      <c r="I37" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="J37" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K37" s="8"/>
@@ -2970,10 +3024,10 @@
         <v>30</v>
       </c>
       <c r="H38" s="8"/>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J38" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K38" s="8"/>
@@ -2998,10 +3052,10 @@
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
-      <c r="I39" s="3" t="s">
+      <c r="I39" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="J39" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K39" s="8"/>
@@ -3018,7 +3072,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>0</v>
@@ -3026,10 +3080,10 @@
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="J40" s="3" t="s">
+      <c r="I40" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K40" s="8"/>
@@ -3054,11 +3108,11 @@
       <c r="F41" s="4"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
-      <c r="I41" s="3" t="s">
+      <c r="I41" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J41" s="8" t="s">
-        <v>436</v>
+      <c r="J41" s="5" t="s">
+        <v>433</v>
       </c>
       <c r="K41" s="8"/>
       <c r="L41"/>
@@ -3084,10 +3138,10 @@
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="I42" s="8" t="s">
-        <v>406</v>
+        <v>434</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>449</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>11</v>
@@ -3120,7 +3174,7 @@
       <c r="H43" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="4" t="s">
         <v>164</v>
       </c>
       <c r="J43" s="4" t="s">
@@ -3152,7 +3206,7 @@
       <c r="H44" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="I44" s="4" t="s">
         <v>164</v>
       </c>
       <c r="J44" s="5" t="s">
@@ -3184,7 +3238,7 @@
       <c r="H45" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="I45" s="4" t="s">
         <v>164</v>
       </c>
       <c r="J45" s="5" t="s">
@@ -3214,7 +3268,7 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
-      <c r="I46" s="3" t="s">
+      <c r="I46" s="4" t="s">
         <v>164</v>
       </c>
       <c r="J46" s="4" t="s">
@@ -3246,7 +3300,7 @@
       <c r="H47" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="4" t="s">
         <v>164</v>
       </c>
       <c r="J47" s="4" t="s">
@@ -3266,7 +3320,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>0</v>
@@ -3274,16 +3328,78 @@
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
-      <c r="I48" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="J48" s="3" t="s">
+      <c r="I48" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J48" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>24</v>
       </c>
       <c r="L48"/>
+    </row>
+    <row r="49" spans="1:12" ht="240">
+      <c r="A49" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A50" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K50" s="8"/>
+      <c r="L50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3295,7 +3411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
@@ -3713,8 +3829,8 @@
       <c r="H13" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>177</v>
+      <c r="I13" s="8" t="s">
+        <v>446</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>276</v>
@@ -3746,8 +3862,8 @@
       <c r="H14" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>177</v>
+      <c r="I14" s="8" t="s">
+        <v>450</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>278</v>
@@ -4303,7 +4419,7 @@
     </row>
     <row r="33" spans="1:12" ht="45">
       <c r="A33" s="8" t="s">
-        <v>242</v>
+        <v>310</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>75</v>
@@ -4332,47 +4448,47 @@
     </row>
     <row r="34" spans="1:12" ht="45">
       <c r="A34" s="8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>360</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>362</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:12" ht="30">
       <c r="A35" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>16</v>
@@ -4382,28 +4498,28 @@
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:12" ht="30">
       <c r="A36" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>16</v>
@@ -4413,22 +4529,22 @@
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>310</v>
       </c>
       <c r="K36" s="8"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>14</v>
@@ -4440,7 +4556,7 @@
         <v>19</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
@@ -4448,7 +4564,7 @@
         <v>185</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K37" s="8"/>
     </row>
@@ -4457,7 +4573,7 @@
         <v>244</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>14</v>
@@ -4655,7 +4771,7 @@
     </row>
     <row r="45" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A45" s="8" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>52</v>
@@ -4674,7 +4790,7 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>244</v>
@@ -4689,16 +4805,16 @@
     </row>
     <row r="46" spans="1:12" ht="30">
       <c r="A46" s="8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>16</v>
@@ -4708,52 +4824,52 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K46" s="8"/>
     </row>
     <row r="47" spans="1:12" ht="30">
       <c r="A47" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="30">
       <c r="A48" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>14</v>
@@ -4765,15 +4881,15 @@
         <v>16</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>38</v>
@@ -4781,39 +4897,39 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K49" s="8"/>
     </row>
     <row r="50" spans="1:11" ht="60">
       <c r="A50" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>14</v>
@@ -4825,17 +4941,17 @@
         <v>16</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>38</v>
@@ -4843,30 +4959,30 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K51" s="8"/>
     </row>
@@ -4877,10 +4993,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L22"/>
+    <sheetView topLeftCell="I18" workbookViewId="0">
+      <selection activeCell="L24" sqref="L2:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4938,39 +5054,36 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>320</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>319</v>
+        <v>338</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>435</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>284</v>
+        <v>27</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>313</v>
+        <v>436</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -4985,18 +5098,21 @@
         <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="75">
+        <v>284</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>286</v>
+        <v>329</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -5008,137 +5124,137 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="75">
+      <c r="A5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="H5" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="K5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30">
-      <c r="A5" t="s">
-        <v>337</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:12" ht="30">
+      <c r="A6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>318</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75">
+      <c r="A7" t="s">
         <v>336</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>321</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>320</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="75">
-      <c r="A6" t="s">
-        <v>338</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>295</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="I6" t="s">
-        <v>333</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30">
-      <c r="A7" t="s">
-        <v>339</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>321</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>291</v>
+      <c r="H7" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="I7" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>292</v>
+        <v>319</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="I8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
-      <c r="A9" s="15" t="s">
-        <v>398</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>396</v>
+      <c r="A9" t="s">
+        <v>437</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>435</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>392</v>
+        <v>291</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>0</v>
@@ -5147,276 +5263,270 @@
         <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>320</v>
+        <v>438</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>397</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
-      <c r="A10" t="s">
-        <v>342</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>341</v>
+      <c r="A10" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>394</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>293</v>
+        <v>390</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
-        <v>324</v>
+      <c r="F10" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>320</v>
+        <v>438</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>325</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>343</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>294</v>
+        <v>340</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>326</v>
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>322</v>
       </c>
       <c r="I11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="K11" t="s">
-        <v>38</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>350</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>294</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I12" t="s">
+        <v>318</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>319</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>341</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45">
+      <c r="A14" t="s">
         <v>349</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>321</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>343</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="45">
-      <c r="A13" t="s">
-        <v>351</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>335</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="B14" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
         <v>333</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30">
-      <c r="A14" t="s">
-        <v>352</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>335</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>297</v>
+        <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I15" t="s">
+        <v>331</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30">
+      <c r="A16" t="s">
+        <v>351</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
         <v>333</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="E16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="I16" t="s">
+        <v>331</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45">
-      <c r="A16" t="s">
-        <v>354</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
+    <row r="17" spans="1:11" ht="45">
+      <c r="A17" t="s">
+        <v>352</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="45">
-      <c r="A17" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>355</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="H17" s="1" t="s">
+        <v>342</v>
+      </c>
       <c r="I17" s="15" t="s">
-        <v>354</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="60">
-      <c r="A18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>301</v>
+        <v>451</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45">
+      <c r="A18" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
-        <v>15</v>
+      <c r="D18" s="8" t="s">
+        <v>353</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>345</v>
-      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="30">
-      <c r="A19" s="8" t="s">
-        <v>369</v>
+        <v>352</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" ht="60">
+      <c r="A19" t="s">
+        <v>354</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>347</v>
+      <c r="D19" t="s">
+        <v>15</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>16</v>
@@ -5424,93 +5534,154 @@
       <c r="F19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="H19" s="14" t="s">
         <v>343</v>
       </c>
+      <c r="I19" s="15" t="s">
+        <v>455</v>
+      </c>
       <c r="J19" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="K19" s="8"/>
+        <v>328</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="30">
-      <c r="A20" t="s">
-        <v>370</v>
+      <c r="A20" s="8" t="s">
+        <v>367</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="E20" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>362</v>
+        <v>23</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8" t="s">
-        <v>363</v>
+        <v>306</v>
       </c>
       <c r="I20" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>348</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" t="s">
-        <v>399</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>393</v>
+        <v>368</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>303</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D21" t="s">
-        <v>392</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>0</v>
+      <c r="D21" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>297</v>
+        <v>360</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="I21" t="s">
+        <v>367</v>
       </c>
       <c r="J21" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30">
+      <c r="A22" t="s">
+        <v>396</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="45">
-      <c r="A22" t="s">
-        <v>400</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>395</v>
-      </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>292</v>
+        <v>390</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>391</v>
-      </c>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="45">
+      <c r="A23" t="s">
+        <v>397</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>291</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45">
+      <c r="A24" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" t="s">
+        <v>354</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed Authoring failed test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -1825,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L50" sqref="L2:L50"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2055,7 +2055,7 @@
       <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="3"/>
@@ -2099,8 +2099,8 @@
       <c r="I8" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>29</v>
+      <c r="J8" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8"/>
@@ -2347,8 +2347,8 @@
       <c r="I16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>29</v>
+      <c r="J16" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16"/>
@@ -2507,8 +2507,8 @@
       <c r="I21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>29</v>
+      <c r="J21" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="K21" s="8"/>
       <c r="L21"/>
@@ -3411,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L51"/>
+    <sheetView topLeftCell="I35" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4117,8 +4117,8 @@
       <c r="I22" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>29</v>
+      <c r="J22" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="K22" s="8"/>
       <c r="L22"/>
@@ -4995,8 +4995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="I18" workbookViewId="0">
-      <selection activeCell="L24" sqref="L2:L24"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fixed authoring test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="451">
   <si>
     <t>GET</t>
   </si>
@@ -1356,24 +1356,9 @@
     <t>OPQA-286_6</t>
   </si>
   <si>
-    <t>OPQA-360||OPQA-286_4</t>
-  </si>
-  <si>
-    <t>OPQA-344_1||OPQA-286_3</t>
-  </si>
-  <si>
     <t>OPQA-896_1||OPQA-286</t>
   </si>
   <si>
-    <t>OPQA-896_1||OPQA-286_2</t>
-  </si>
-  <si>
-    <t>OPQA-360||OPQA-286_1</t>
-  </si>
-  <si>
-    <t>OPQA-1087||OPQA-286_5</t>
-  </si>
-  <si>
     <t>OPQA-286_7</t>
   </si>
   <si>
@@ -1383,7 +1368,7 @@
     <t>status=200||size=eval$(OPQA-344_1_counterValue)+1||comments.userId=(SYS_USER1)||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.targetType=wos||comments.content=Comment Max Length Test: As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher,&gt;1500I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge...!||comments.wasTruncated=true</t>
   </si>
   <si>
-    <t>OPQA-1087||OPQA-286_6</t>
+    <t>OPQA-377||OPQA-385</t>
   </si>
 </sst>
 </file>
@@ -1825,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L50"/>
+    <sheetView tabSelected="1" topLeftCell="I48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L50" sqref="L2:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2721,7 +2706,7 @@
         <v>425</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>426</v>
@@ -3141,7 +3126,7 @@
         <v>434</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>449</v>
+        <v>403</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>11</v>
@@ -3362,10 +3347,10 @@
         <v>443</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>447</v>
+        <v>94</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="K49" s="8" t="s">
         <v>20</v>
@@ -3411,8 +3396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="I35" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView topLeftCell="J44" workbookViewId="0">
+      <selection activeCell="L51" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3425,7 +3410,7 @@
     <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="45" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="133.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3830,7 +3815,7 @@
         <v>275</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>446</v>
+        <v>177</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>276</v>
@@ -3863,7 +3848,7 @@
         <v>277</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>450</v>
+        <v>177</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>278</v>
@@ -4262,8 +4247,8 @@
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
-      <c r="I27" s="3" t="s">
-        <v>177</v>
+      <c r="I27" s="8" t="s">
+        <v>450</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>280</v>
@@ -4995,8 +4980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="I18" workbookViewId="0">
+      <selection activeCell="L24" sqref="L2:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5477,7 +5462,7 @@
         <v>342</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>451</v>
+        <v>341</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>327</v>
@@ -5538,7 +5523,7 @@
         <v>343</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>455</v>
+        <v>341</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>328</v>
@@ -5656,7 +5641,7 @@
     </row>
     <row r="24" spans="1:11" ht="45">
       <c r="A24" s="8" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>75</v>
@@ -5665,7 +5650,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added new test cases to the Authoring, Groups and added jira ids to project container
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="499">
   <si>
     <t>GET</t>
   </si>
@@ -879,9 +879,6 @@
     <t>Verify that spam check and unsupported tag validations are not done on draft post</t>
   </si>
   <si>
-    <t>Verify that spam check and unsupported tag validations are done when user publishes the draft post</t>
-  </si>
-  <si>
     <t>Verfiy that user is able to access and edit the draft posts from their profile</t>
   </si>
   <si>
@@ -1369,6 +1366,153 @@
   </si>
   <si>
     <t>OPQA-377||OPQA-385</t>
+  </si>
+  <si>
+    <t>OPQA-1078_1</t>
+  </si>
+  <si>
+    <t>{"content":"Draft Post 3 creation by Neon User3 creds using API. Later it might be deleted", "title":"Draft Post 3 by Neon User3", "topics":[]}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER3)||title=Draft Post 3 by Neon User3||content=""||found=true</t>
+  </si>
+  <si>
+    <t>/drafts/draft/(OPQA-1078_1_id)</t>
+  </si>
+  <si>
+    <t>Verify that spam check and unsupported tag validations are done, auto removed upsupported tags and published when user publishes the draft post</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to add supported tags like emphasis, strikethrough, strong tags to the post and publish it.</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to add supported tags like emphasis, strikethrough, strong tags while editing the post.</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add supported tags like emphasis, strong tags to the comment and publish it under any post.</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add supported tags like emphasis, strong tags while editing the comment and publish it.</t>
+  </si>
+  <si>
+    <t>OPQA-1076_3</t>
+  </si>
+  <si>
+    <t>OPQA-286_8</t>
+  </si>
+  <si>
+    <t>OPQA-1076_4</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-1083_id)</t>
+  </si>
+  <si>
+    <t>?size=10</t>
+  </si>
+  <si>
+    <t>/appreciation/posts/(OPQA-360_1_id)/appreciations</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-360_1_id)||userId=(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>Verify that for the given comment id, appreciation details like user ids, time created are returned properly by using API</t>
+  </si>
+  <si>
+    <t>Verify that for the given post id, appreciation details like user ids, time created are returned properly by using API</t>
+  </si>
+  <si>
+    <t>/appreciation/Comment/(OPQA-385_comments.id)/appreciations</t>
+  </si>
+  <si>
+    <t>status=200||targetType=Comment||targetId=(OPQA-385_comments.id)||userId=(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>Verify that API truncated the post length to 27000 characters while creating/Editing the post</t>
+  </si>
+  <si>
+    <t>{ "title":"Supported tags test from API - Post", "content":"Testing adding supported tags like strikethrough, emphasis, strong to the post from API:: &lt;br&gt; Example on strikethrough tag: &lt;s&gt;This is strikethrough tag &lt;/s&gt; &lt;br&gt; Example on emphasis tag: &lt;em&gt;This is emphasis tag &lt;/em&gt; &lt;br&gt;  Example on strong tag: &lt;strong&gt;This is strong tag &lt;/strong&gt;" }</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-1083_id)||userId=(SYS_USER2)||title=Draft Post 2 From API||content=''||wasCleanedUp=0||wasTruncated=false||found=true</t>
+  </si>
+  <si>
+    <t>OPQA-1076_5</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||content=Testing adding supported tags like strikethrough, emphasis, strong to the post from API:: &lt;br&gt; Example on strikethrough tag: &lt;s&gt;This is strikethrough tag &lt;/s&gt; &lt;br&gt; Example on emphasis tag: &lt;em&gt;This is emphasis tag &lt;/em&gt; &lt;br&gt;  Example on strong tag: &lt;strong&gt;This is strong tag &lt;/strong&gt;||title=Supported tags test from API - Post||found=true</t>
+  </si>
+  <si>
+    <t>OPQA-1080||OPQA-1076_4</t>
+  </si>
+  <si>
+    <t>{ "title":"Supported tags test from API - Edited Post", "content":"Testing adding supported tags like strikethrough, emphasis, strong in the Edit post from API:: Example on strikethrough tag: &lt;s&gt;This is edited strikethrough tag &lt;/s&gt; Example on emphasis tag: &lt;em&gt;This is edite4d emphasis tag &lt;/em&gt;  Example on strong tag: &lt;strong&gt;This is edited strong tag &lt;/strong&gt;" }</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||title=Supported tags test from API - Edited Post||content=Testing adding supported tags like strikethrough, emphasis, strong in the Edit post from API:: Example on strikethrough tag: &lt;s&gt;This is edited strikethrough tag &lt;/s&gt; Example on emphasis tag: &lt;em&gt;This is edite4d emphasis tag &lt;/em&gt;  Example on strong tag: &lt;strong&gt;This is edited strong tag &lt;/strong&gt;||wasCleanedUp=0||wasTruncated=false||found=true</t>
+  </si>
+  <si>
+    <t>{ "title":"Large Content 27,350 chars test from API - About Cancer from Wikipedia", "content":"Cancer is a group of diseases involving abnormal cell growth with the potential to invade or spread to other parts of the body.[1][2] Not all tumors are cancerous; benign tumors do not spread to other parts of the body.[2] Possible signs and symptoms include a lump, abnormal bleeding, prolonged cough, unexplained weight loss and a change in bowel movements.[3] While these symptoms may indicate cancer, they may have other causes.[3] Over 100 cancers affect humans.[2]Tobacco use is the cause of about 22% of cancer deaths.[1] Another 10% is due to obesity, poor diet, lack of physical activity and drinking alcohol.[1][4] Other factors include certain infections, exposure to ionizing radiation and environmental pollutants.[5] In the developing world nearly 20% of cancers are due to infections such as hepatitis B, hepatitis C and human papillomavirus HPV.[1] These factors act, at least partly, by changing the genes of a cell.[6] Typically many genetic changes are required before cancer develops.[6] Approximately 5-10% of cancers are due to inherited genetic defects from a person's parents.[7] Cancer can be detected by certain signs and symptoms or screening tests.[1] It is then typically further investigated by medical imaging and confirmed by biopsy.[8]Many cancers can be prevented by not smoking, maintaining a healthy weight, not drinking too much alcohol, eating plenty of vegetables, fruits and whole grains, vaccination against certain infectious diseases, not eating too much processed and red meat, and avoiding too much sunlight exposure.[9][10] Early detection through screening is useful for cervical and colorectal cancer.[11] The benefits of screening in breast cancer are controversial.[11][12] Cancer is often treated with some combination of radiation therapy, surgery, chemotherapy, and targeted therapy.[1][13] Pain and symptom management are an important part of care. Palliative care is particularly important in people with advanced disease.[1] The chance of survival depends on the type of cancer and extent of disease at the start of treatment.[6] In children under 15 at diagnosis the five-year survival rate in the developed world is on average 80%.[14] For cancer in the United States the average five-year survival rate is 66%.[15]In 2012 about 14.1 million new cases of cancer occurred globally not including skin cancer other than melanoma.[6] It caused about 8.2 million deaths or 14.6% of human deaths.[6][16] The most common types of cancer in males are lung cancer, prostate cancer, colorectal cancer and stomach cancer. In females, the most common types are breast cancer, colorectal cancer, lung cancer and cervical cancer.[6] If skin cancer other than melanoma were included in total new cancers each year it would account for around 40% of cases.[17][18] In children, acute lymphoblastic leukaemia and brain tumors are most common except in Africa where non-Hodgkin lymphoma occurs more often.[14] In 2012, about 165,000 children under 15 years of age were diagnosed with cancer. The risk of cancer increases significantly with age and many cancers occur more commonly in developed countries.[6] Rates are increasing as more people live to an old age and as lifestyle changes occur in the developing world.[19] The financial costs of cancer were estimated at $1.16 trillion US dollars per year as of 2010.[20]Cancers are a large family of diseases that involve abnormal cell growth with the potential to invade or spread to other parts of the body.[1][2] They form a subset of neoplasms. A neoplasm or tumor is a group of cells that have undergone unregulated growth and will often form a mass or lump, but may be distributed diffusely.[21][22]All tumor cells show the six hallmarks of cancer. These characteristics are required to produce a malignant tumor. They include:23]Cell growth and division absent the proper signalsContinuous growth and division even given contrary signalsAvoidance of programmed cell deathLimitless number of cell divisionsPromoting blood vessel constructionInvasion of tissue and formation of metastases[24]The progression from normal cells to cells that can form a detectable mass to outright cancer involves multiple steps known as malignant progression.[24][25]Signs and symptomsMain article: Cancer signs and symptomsSymptoms of cancer metastasis depend on the location of the tumor.When cancer begins, it produces no symptoms. Signs and symptoms appear as the mass grows or ulcerates. The findings that result depend on the cancer's type and location. Few symptoms are specific. Many frequently occur in individuals who have other conditions. Cancer is a great imitator. Thus, it is common for people diagnosed with cancer to have been treated for other diseases, which were hypothesized to be causing their symptoms.[26]Local symptomsLocal symptoms may occur due to the mass of the tumor or its ulceration. For example, mass effects from lung cancer can block the bronchus resulting in cough or pneumonia; esophageal cancer can cause narrowing of the esophagus, making it difficult or painful to swallow; and colorectal cancer may lead to narrowing or blockages in the bowel, affecting bowel habits. Masses in breasts or ********* may produce observable lumps. Ulceration can cause bleeding that, if it occurs in the lung, will lead to coughing up blood, in the bowels to anemia or rectal bleeding, in the bladder to blood in the urine and in the uterus to ******* bleeding. Although localized pain may occur in advanced cancer, the initial swelling is usually painless. Some cancers can cause a buildup of fluid within the chest or abdomen.[26]Systemic symptomsGeneral symptoms occur due to effects that are not related to direct or metastatic spread. These may include: unintentional weight loss, fever, excessive fatigue and changes to the skin.[27] Hodgkin disease, leukemias and cancers of the liver or kidney can cause a persistent fever.[26]Some cancers may cause specific groups of systemic symptoms, termed paraneoplastic phenomena. Examples include the appearance of myasthenia gravis in thymoma and clubbing in lung cancer.[26]MetastasisMain article: MetastasisCancer can spread from its original site by local spread, lymphatic spread to regional lymph nodes or by haematogenous spread via the blood to distant sites, known as metastasis. When cancer spreads by a haematogenous route, it usually spreads all over the body. However, cancer 'seeds' grow in certain selected site only 'soil' as hypothesized in the soil and seed hypothesis of cancer metastasis. The symptoms of metastatic cancers depend on the tumor location and can include enlarged lymph nodes which can be felt or sometimes seen under the skin and are typically hard, enlarged liver or enlarged spleen, which can be felt in the abdomen, pain or fracture of affected bones and neurological symptoms.[26]CausesMain article: Causes of cancerThe majority of cancers, some 90-95% of cases, are due to environmental factors. The remaining 5-10% are due to inherited genetics.[5] Environmental, as used by cancer researchers, means any cause that is not inherited genetically, such as lifestyle, economic and behavioral factors and not merely pollution.[28] Common environmental factors that contribute to cancer death include tobacco 25-30%, diet and obesity 30-35%, infections 15-20%, radiation both ionizing and non-ionizing, up to 10%, stress, lack of physical activity and environmental pollutants.[5]It is not generally possible to prove what caused a particular cancer, because the various causes do not have specific fingerprints. For example, if a person who uses tobacco heavily develops lung cancer, then it was probably caused by the tobacco use, but since everyone has a small chance of developing lung cancer as a result of air pollution or radiation, the cancer may have developed for one of those reasons. Excepting the rare transmissions that occur with pregnancies and occasional organ donors, cancer is generally not a transmissible disease.[29]ChemicalsFurther information: Alcohol and cancer and Smoking and cancerThe incidence of lung cancer is highly correlated with smoking.Exposure to particular substances have been linked to specific types of cancer. These substances are called carcinogens.Tobacco smoke, for example, causes 90% of lung cancer.[30] It also causes cancer in the larynx, head, neck, stomach, bladder, kidney, esophagus and pancreas.[31] Tobacco smoke contains over fifty known carcinogens, including nitrosamines and polycyclic aromatic hydrocarbons.[32]Tobacco is responsible about one in five cancer deaths worldwide[32] and about one in three in the developed world[33] Lung cancer death rates in the United States have mirrored smoking patterns, with increases in smoking followed by dramatic increases in lung cancer death rates and, more recently, decreases in smoking rates since the 1950s followed by decreases in lung cancer death rates in men since 1990.[34][35]In Western Europe, 10% of cancers in males and 3% of cancers in females are attributed to alcohol exposure, especially liver and digestive tract cancers.[36] Cancer from work-related substance exposures may cause between 2-20% of cases,37] causing at least 200,000 deaths.[38] Cancers such as lung cancer and mesothelioma can come from inhaling tobacco smoke or asbestos fibers, or leukemia from exposure to benzene.[38]Diet and exerciseMain article: Diet and cancerDiet, physical inactivity and obesity are related to up to 30-35% of cancer deaths.[5][39] In the United States excess body weight is associated with the development of many types of cancer and is a factor in 14-20% of cancer deaths.[39] A UK study including data on over 5 million people showed higher body mass index to be related to at least 10 types of cancer and responsible for around 12,000 cases each year in that country.[40] Physical inactivity is believed to contribute to cancer risk, not only through its effect on body weight but also through negative effects on the immune system and endocrine system.[39] More than half of the effect from diet is due to overnutrition eating too much, rather than from eating too few vegetables or other healthful foods.Some specific foods are linked to specific cancers. A high-salt diet is linked to gastric cancer.[41] Aflatoxin B1, a frequent food contaminant, causes liver cancer.[41] Betel nut chewing can cause oral cancer.[41] National differences in dietary practices may partly explain differences in cancer incidence. For example, gastric cancer is more common in Japan due to its high-salt diet[42] while colon cancer is more common in the United States. Immigrant cancer profiles develop mirror that of their new country, often within one generation.[43]InfectionMain article: Infectious causes of cancerWorldwide approximately 18% of cancer deaths are related to infectious diseases.[5] This proportion ranges from a high of 25% in Africa to less than 10% in the developed world.[5] Viruses are the usual infectious agents that cause cancer but cancer bacteria and parasites may also play a role.Oncoviruses viruses that can cause cancer include human papillomavirus cervical cancer, Epstein-Barr virus B-cell lymphoproliferative disease and nasopharyngeal carcinoma, Kaposi's sarcoma herpesvirus Kaposi's sarcoma and primary effusion lymphomas, hepatitis B and hepatitis C viruses hepatocellular carcinoma and human T-cell leukemia virus-1 T-cell leukemias. Bacterial infection may also increase the risk of cancer, as seen in Helicobacter pylori-induced gastric carcinoma.[44][45] Parasitic infections associated with cancer include Schistosoma haematobium squamous cell carcinoma of the bladder and the liver flukes, Opisthorchis viverrini and Clonorchis sinensis cholangiocarcinoma.[46]RadiationMain article: Radiation-induced cancerUp to 10% of invasive cancers are related to radiation exposure, including both ionizing radiation and non-ionizing ultraviolet radiation.[5] Additionally, the majority of non-invasive cancers are non-melanoma skin cancers caused by non-ionizing ultraviolet radiation, mostly from sunlight. Sources of ionizing radiation include medical imaging and radon gas.Ionizing radiation is not a particularly strong mutagen.[47] Residential exposure to radon gas, for example, has similar cancer risks as passive smoking.[47] Radiation is a more potent source of cancer when combined with other cancer-causing agents, such as radon plus tobacco smoke.[47] Radiation can cause cancer in most parts of the body, in all animals and at any age. Children and adolescents are twice as likely to develop radiation-induced leukemia as adults; radiation exposure before birth has ten times the effect.[47]Medical use of ionizing radiation is a small but growing source of radiation-induced cancers. Ionizing radiation may be used to treat other cancers, but this may, in some cases, induce a second form of cancer.[47] It is also used in some kinds of medical imaging.[48]Prolonged exposure to ultraviolet radiation from the sun can lead to melanoma and other skin malignancies.[49] Clear evidence establishes ultraviolet radiation, especially the non-ionizing medium wave UVB, as the cause of most non-melanoma skin cancers, which are the most common forms of cancer in the world.[49]Non-ionizing radio frequency radiation from mobile phones, electric power transmission and other similar sources have been described as a possible carcinogen by the World Health Organization's International Agency for Research on Cancer.[50] However, studies have not found a consistent link between mobile phone radiation and cancer risk.[51]HeredityMain article: Cancer syndromeThe vast majority of cancers are non-hereditary sporadic. Hereditary cancers are primarily caused by an inherited genetic defect. Less than 0.3% of the population are carriers of a genetic mutation that has a large effect on cancer risk and these cause less than 3-10% of cancer.[52] Some of these syndromes include: certain inherited mutations in the genes BRCA1 and BRCA2 with a more than 75% risk of breast cancer and ovarian cancer,52] and hereditary nonpolyposis colorectal cancer HNPCC or Lynch syndrome, which is present in about 3% of people with colorectal cancer,53] among others.Physical agentsSome substances cause cancer primarily through their physical, rather than chemical, effects.[54] A prominent example of this is prolonged exposure to asbestos, naturally occurring mineral fibers that are a major cause of mesothelioma cancer of the serous membrane usually the serous membrane surrounding the lungs.[54] Other substances in this category, including both naturally occurring and synthetic asbestos-like fibers, such as wollastonite, attapulgite, glass wool and rock wool, are believed to have similar effects.[54] Non-fibrous particulate materials that cause cancer include powdered metallic cobalt and nickel and crystalline silica quartz, cristobalite and tridymite.[54] Usually, physical carcinogens must get inside the body such as through inhalation and require years of exposure to produce cancer.[54]Physical trauma resulting in cancer is relatively rare.[55] Claims that breaking bones resulted in bone cancer, for example, have not been proven.[55] Similarly, physical trauma is not accepted as a cause for cervical cancer, breast cancer or brain cancer.[55] One accepted source is frequent, long-term application of hot objects to the body. It is possible that repeated burns on the same part of the body, such as those produced by kanger and kairo heaters charcoal hand warmers, may produce skin cancer, especially if carcinogenic chemicals are also present.[55] Frequent consumption of scalding hot tea may produce esophageal cancer.[55] Generally, it is believed that the cancer arises, or a pre-existing cancer is encouraged, during the process of healing, rather than directly by the trauma.[55] However, repeated injuries to the same tissues might promote excessive cell proliferation, which could then increase the odds of a cancerous mutation.Chronic inflammation has been hypothesized to directly cause mutation.[55][56] Inflammation can contribute to proliferation, survival, angiogenesis and migration of cancer cells by influencing the tumor microenvironment.[57][58] Oncogenes build up an inflammatory pro-tumorigenic microenvironment.[59]HormonesSome hormones play a role in the development of cancer by promoting cell proliferation.[60] Insulin-like growth factors and their binding proteins play a key role in cancer cell proliferation, differentiation and apoptosis, suggesting possible involvement in carcinogenesis.[61]Hormones are important agents in sex-related cancers, such as cancer of the breast, endometrium, prostate, ovary and testis and also of thyroid cancer and bone cancer.[60] For example, the daughters of women who have breast cancer have significantly higher levels of estrogen and progesterone than the daughters of women without breast cancer. These higher hormone levels may explain their higher risk of breast cancer, even in the absence of a breast-cancer gene.[60] Similarly, men of African ancestry have significantly higher levels of testosterone than men of European ancestry and have a correspondingly higher level of prostate cancer.[60] Men of Asian ancestry, with the lowest levels of testosterone-activating androstanediol glucuronide, have the lowest levels of prostate cancer.[60]Other factors are relevant: obese people have higher levels of some hormones associated with cancer and a higher rate of those cancers.[60] Women who take hormone replacement therapy have a higher risk of developing cancers associated with those hormones.[60] On the other hand, people who exercise far more than average have lower levels of these hormones and lower risk of cancer.[60] Osteosarcoma may be promoted by growth hormones.[60] Some treatments and prevention approaches leH16H16H30H48H65H96H127H158H189H220H251H282H313H344H375H406H437H468H499H530H499H468H437H406H375H344H313H282H251H220H189H158H127H96H69verage this cause by artificially reducing hormone levels and thus discouraging hormone-sensitive cancers.[60]Autoimmune diseasesThere is an association between celiac disease and an increased risk of all cancers. People with untreated celiac disease have a higher risk, but this risk decreases with time after diagnosis and strict treatment, probably due to the adoption of a gluten-free diet, which seems to have a protective role against development of malignancy in people with celiac disease. However, the delay in diagnosis and initiation of a gluten-free diet seems to increase the risk of malignancies.[62] Rates of gastrointestinal cancers are increased in people with Crohn's disease and ulcerative colitis, due to chronic inflammation. Also, immunomodulators and biologic agents used to treat these diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur through..these diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur through..these diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur through.. these diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur throughthese diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur throughthese diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur throughthese diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur throughthese diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. &lt;b&gt;&lt;i&gt;This is FINAL..... 27,350 &lt;/b&gt;&lt;/i&gt;" }</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||content=Cancer is a group of diseases involving abnormal cell growth with the potential to invade or spread to other parts of the body.[1][2] Not all tumors are cancerous; benign tumors do not spread to other parts of the body.[2] Possible signs and symptoms include a lump, abnormal bleeding, prolonged cough, unexplained weight loss and a change in bowel movements.[3] While these symptoms may indicate cancer, they may have other causes.[3] Over 100 cancers affect humans.[2]Tobacco use is the cause of about 22% of cancer deaths.[1] Another 10% is due to obesity, poor diet, lack of physical activity and drinking alcohol.[1][4] Other factors include certain infections, exposure to ionizing radiation and environmental pollutants.[5] In the developing world nearly 20% of cancers are due to infections such as hepatitis B, hepatitis C and human papillomavirus HPV.[1] These factors act, at least partly, by changing the genes of a cell.[6] Typically many genetic changes are required before cancer develops.[6] Approximately 5-10% of cancers are due to inherited genetic defects from a person's parents.[7] Cancer can be detected by certain signs and symptoms or screening tests.[1] It is then typically further investigated by medical imaging and confirmed by biopsy.[8]Many cancers can be prevented by not smoking, maintaining a healthy weight, not drinking too much alcohol, eating plenty of vegetables, fruits and whole grains, vaccination against certain infectious diseases, not eating too much processed and red meat, and avoiding too much sunlight exposure.[9][10] Early detection through screening is useful for cervical and colorectal cancer.[11] The benefits of screening in breast cancer are controversial.[11][12] Cancer is often treated with some combination of radiation therapy, surgery, chemotherapy, and targeted therapy.[1][13] Pain and symptom management are an important part of care. Palliative care is particularly important in people with advanced disease.[1] The chance of survival depends on the type of cancer and extent of disease at the start of treatment.[6] In children under 15 at diagnosis the five-year survival rate in the developed world is on average 80%.[14] For cancer in the United States the average five-year survival rate is 66%.[15]In 2012 about 14.1 million new cases of cancer occurred globally not including skin cancer other than melanoma.[6] It caused about 8.2 million deaths or 14.6% of human deaths.[6][16] The most common types of cancer in males are lung cancer, prostate cancer, colorectal cancer and stomach cancer. In females, the most common types are breast cancer, colorectal cancer, lung cancer and cervical cancer.[6] If skin cancer other than melanoma were included in total new cancers each year it would account for around 40% of cases.[17][18] In children, acute lymphoblastic leukaemia and brain tumors are most common except in Africa where non-Hodgkin lymphoma occurs more often.[14] In 2012, about 165,000 children under 15 years of age were diagnosed with cancer. The risk of cancer increases significantly with age and many cancers occur more commonly in developed countries.[6] Rates are increasing as more people live to an old age and as lifestyle changes occur in the developing world.[19] The financial costs of cancer were estimated at $1.16 trillion US dollars per year as of 2010.[20]Cancers are a large family of diseases that involve abnormal cell growth with the potential to invade or spread to other parts of the body.[1][2] They form a subset of neoplasms. A neoplasm or tumor is a group of cells that have undergone unregulated growth and will often form a mass or lump, but may be distributed diffusely.[21][22]All tumor cells show the six hallmarks of cancer. These characteristics are required to produce a malignant tumor. They include:23]Cell growth and division absent the proper signalsContinuous growth and division even given contrary signalsAvoidance of programmed cell deathLimitless number of cell divisionsPromoting blood vessel constructionInvasion of tissue and formation of metastases[24]The progression from normal cells to cells that can form a detectable mass to outright cancer involves multiple steps known as malignant progression.[24][25]Signs and symptomsMain article: Cancer signs and symptomsSymptoms of cancer metastasis depend on the location of the tumor.When cancer begins, it produces no symptoms. Signs and symptoms appear as the mass grows or ulcerates. The findings that result depend on the cancer's type and location. Few symptoms are specific. Many frequently occur in individuals who have other conditions. Cancer is a great imitator. Thus, it is common for people diagnosed with cancer to have been treated for other diseases, which were hypothesized to be causing their symptoms.[26]Local symptomsLocal symptoms may occur due to the mass of the tumor or its ulceration. For example, mass effects from lung cancer can block the bronchus resulting in cough or pneumonia; esophageal cancer can cause narrowing of the esophagus, making it difficult or painful to swallow; and colorectal cancer may lead to narrowing or blockages in the bowel, affecting bowel habits. Masses in breasts or ********* may produce observable lumps. Ulceration can cause bleeding that, if it occurs in the lung, will lead to coughing up blood, in the bowels to anemia or rectal bleeding, in the bladder to blood in the urine and in the uterus to ******* bleeding. Although localized pain may occur in advanced cancer, the initial swelling is usually painless. Some cancers can cause a buildup of fluid within the chest or abdomen.[26]Systemic symptomsGeneral symptoms occur due to effects that are not related to direct or metastatic spread. These may include: unintentional weight loss, fever, excessive fatigue and changes to the skin.[27] Hodgkin disease, leukemias and cancers of the liver or kidney can cause a persistent fever.[26]Some cancers may cause specific groups of systemic symptoms, termed paraneoplastic phenomena. Examples include the appearance of myasthenia gravis in thymoma and clubbing in lung cancer.[26]MetastasisMain article: MetastasisCancer can spread from its original site by local spread, lymphatic spread to regional lymph nodes or by haematogenous spread via the blood to distant sites, known as metastasis. When cancer spreads by a haematogenous route, it usually spreads all over the body. However, cancer 'seeds' grow in certain selected site only 'soil' as hypothesized in the soil and seed hypothesis of cancer metastasis. The symptoms of metastatic cancers depend on the tumor location and can include enlarged lymph nodes which can be felt or sometimes seen under the skin and are typically hard, enlarged liver or enlarged spleen, which can be felt in the abdomen, pain or fracture of affected bones and neurological symptoms.[26]CausesMain article: Causes of cancerThe majority of cancers, some 90-95% of cases, are due to environmental factors. The remaining 5-10% are due to inherited genetics.[5] Environmental, as used by cancer researchers, means any cause that is not inherited genetically, such as lifestyle, economic and behavioral factors and not merely pollution.[28] Common environmental factors that contribute to cancer death include tobacco 25-30%, diet and obesity 30-35%, infections 15-20%, radiation both ionizing and non-ionizing, up to 10%, stress, lack of physical activity and environmental pollutants.[5]It is not generally possible to prove what caused a particular cancer, because the various causes do not have specific fingerprints. For example, if a person who uses tobacco heavily develops lung cancer, then it was probably caused by the tobacco use, but since everyone has a small chance of developing lung cancer as a result of air pollution or radiation, the cancer may have developed for one of those reasons. Excepting the rare transmissions that occur with pregnancies and occasional organ donors, cancer is generally not a transmissible disease.[29]ChemicalsFurther information: Alcohol and cancer and Smoking and cancerThe incidence of lung cancer is highly correlated with smoking.Exposure to particular substances have been linked to specific types of cancer. These substances are called carcinogens.Tobacco smoke, for example, causes 90% of lung cancer.[30] It also causes cancer in the larynx, head, neck, stomach, bladder, kidney, esophagus and pancreas.[31] Tobacco smoke contains over fifty known carcinogens, including nitrosamines and polycyclic aromatic hydrocarbons.[32]Tobacco is responsible about one in five cancer deaths worldwide[32] and about one in three in the developed world[33] Lung cancer death rates in the United States have mirrored smoking patterns, with increases in smoking followed by dramatic increases in lung cancer death rates and, more recently, decreases in smoking rates since the 1950s followed by decreases in lung cancer death rates in men since 1990.[34][35]In Western Europe, 10% of cancers in males and 3% of cancers in females are attributed to alcohol exposure, especially liver and digestive tract cancers.[36] Cancer from work-related substance exposures may cause between 2-20% of cases,37] causing at least 200,000 deaths.[38] Cancers such as lung cancer and mesothelioma can come from inhaling tobacco smoke or asbestos fibers, or leukemia from exposure to benzene.[38]Diet and exerciseMain article: Diet and cancerDiet, physical inactivity and obesity are related to up to 30-35% of cancer deaths.[5][39] In the United States excess body weight is associated with the development of many types of cancer and is a factor in 14-20% of cancer deaths.[39] A UK study including data on over 5 million people showed higher body mass index to be related to at least 10 types of cancer and responsible for around 12,000 cases each year in that country.[40] Physical inactivity is believed to contribute to cancer risk, not only through its effect on body weight but also through negative effects on the immune system and endocrine system.[39] More than half of the effect from diet is due to overnutrition eating too much, rather than from eating too few vegetables or other healthful foods.Some specific foods are linked to specific cancers. A high-salt diet is linked to gastric cancer.[41] Aflatoxin B1, a frequent food contaminant, causes liver cancer.[41] Betel nut chewing can cause oral cancer.[41] National differences in dietary practices may partly explain differences in cancer incidence. For example, gastric cancer is more common in Japan due to its high-salt diet[42] while colon cancer is more common in the United States. Immigrant cancer profiles develop mirror that of their new country, often within one generation.[43]InfectionMain article: Infectious causes of cancerWorldwide approximately 18% of cancer deaths are related to infectious diseases.[5] This proportion ranges from a high of 25% in Africa to less than 10% in the developed world.[5] Viruses are the usual infectious agents that cause cancer but cancer bacteria and parasites may also play a role.Oncoviruses viruses that can cause cancer include human papillomavirus cervical cancer, Epstein-Barr virus B-cell lymphoproliferative disease and nasopharyngeal carcinoma, Kaposi's sarcoma herpesvirus Kaposi's sarcoma and primary effusion lymphomas, hepatitis B and hepatitis C viruses hepatocellular carcinoma and human T-cell leukemia virus-1 T-cell leukemias. Bacterial infection may also increase the risk of cancer, as seen in Helicobacter pylori-induced gastric carcinoma.[44][45] Parasitic infections associated with cancer include Schistosoma haematobium squamous cell carcinoma of the bladder and the liver flukes, Opisthorchis viverrini and Clonorchis sinensis cholangiocarcinoma.[46]RadiationMain article: Radiation-induced cancerUp to 10% of invasive cancers are related to radiation exposure, including both ionizing radiation and non-ionizing ultraviolet radiation.[5] Additionally, the majority of non-invasive cancers are non-melanoma skin cancers caused by non-ionizing ultraviolet radiation, mostly from sunlight. Sources of ionizing radiation include medical imaging and radon gas.Ionizing radiation is not a particularly strong mutagen.[47] Residential exposure to radon gas, for example, has similar cancer risks as passive smoking.[47] Radiation is a more potent source of cancer when combined with other cancer-causing agents, such as radon plus tobacco smoke.[47] Radiation can cause cancer in most parts of the body, in all animals and at any age. Children and adolescents are twice as likely to develop radiation-induced leukemia as adults; radiation exposure before birth has ten times the effect.[47]Medical use of ionizing radiation is a small but growing source of radiation-induced cancers. Ionizing radiation may be used to treat other cancers, but this may, in some cases, induce a second form of cancer.[47] It is also used in some kinds of medical imaging.[48]Prolonged exposure to ultraviolet radiation from the sun can lead to melanoma and other skin malignancies.[49] Clear evidence establishes ultraviolet radiation, especially the non-ionizing medium wave UVB, as the cause of most non-melanoma skin cancers, which are the most common forms of cancer in the world.[49]Non-ionizing radio frequency radiation from mobile phones, electric power transmission and other similar sources have been described as a possible carcinogen by the World Health Organization's International Agency for Research on Cancer.[50] However, studies have not found a consistent link between mobile phone radiation and cancer risk.[51]HeredityMain article: Cancer syndromeThe vast majority of cancers are non-hereditary sporadic. Hereditary cancers are primarily caused by an inherited genetic defect. Less than 0.3% of the population are carriers of a genetic mutation that has a large effect on cancer risk and these cause less than 3-10% of cancer.[52] Some of these syndromes include: certain inherited mutations in the genes BRCA1 and BRCA2 with a more than 75% risk of breast cancer and ovarian cancer,52] and hereditary nonpolyposis colorectal cancer HNPCC or Lynch syndrome, which is present in about 3% of people with colorectal cancer,53] among others.Physical agentsSome substances cause cancer primarily through their physical, rather than chemical, effects.[54] A prominent example of this is prolonged exposure to asbestos, naturally occurring mineral fibers that are a major cause of mesothelioma cancer of the serous membrane usually the serous membrane surrounding the lungs.[54] Other substances in this category, including both naturally occurring and synthetic asbestos-like fibers, such as wollastonite, attapulgite, glass wool and rock wool, are believed to have similar effects.[54] Non-fibrous particulate materials that cause cancer include powdered metallic cobalt and nickel and crystalline silica quartz, cristobalite and tridymite.[54] Usually, physical carcinogens must get inside the body such as through inhalation and require years of exposure to produce cancer.[54]Physical trauma resulting in cancer is relatively rare.[55] Claims that breaking bones resulted in bone cancer, for example, have not been proven.[55] Similarly, physical trauma is not accepted as a cause for cervical cancer, breast cancer or brain cancer.[55] One accepted source is frequent, long-term application of hot objects to the body. It is possible that repeated burns on the same part of the body, such as those produced by kanger and kairo heaters charcoal hand warmers, may produce skin cancer, especially if carcinogenic chemicals are also present.[55] Frequent consumption of scalding hot tea may produce esophageal cancer.[55] Generally, it is believed that the cancer arises, or a pre-existing cancer is encouraged, during the process of healing, rather than directly by the trauma.[55] However, repeated injuries to the same tissues might promote excessive cell proliferation, which could then increase the odds of a cancerous mutation.Chronic inflammation has been hypothesized to directly cause mutation.[55][56] Inflammation can contribute to proliferation, survival, angiogenesis and migration of cancer cells by influencing the tumor microenvironment.[57][58] Oncogenes build up an inflammatory pro-tumorigenic microenvironment.[59]HormonesSome hormones play a role in the development of cancer by promoting cell proliferation.[60] Insulin-like growth factors and their binding proteins play a key role in cancer cell proliferation, differentiation and apoptosis, suggesting possible involvement in carcinogenesis.[61]Hormones are important agents in sex-related cancers, such as cancer of the breast, endometrium, prostate, ovary and testis and also of thyroid cancer and bone cancer.[60] For example, the daughters of women who have breast cancer have significantly higher levels of estrogen and progesterone than the daughters of women without breast cancer. These higher hormone levels may explain their higher risk of breast cancer, even in the absence of a breast-cancer gene.[60] Similarly, men of African ancestry have significantly higher levels of testosterone than men of European ancestry and have a correspondingly higher level of prostate cancer.[60] Men of Asian ancestry, with the lowest levels of testosterone-activating androstanediol glucuronide, have the lowest levels of prostate cancer.[60]Other factors are relevant: obese people have higher levels of some hormones associated with cancer and a higher rate of those cancers.[60] Women who take hormone replacement therapy have a higher risk of developing cancers associated with those hormones.[60] On the other hand, people who exercise far more than average have lower levels of these hormones and lower risk of cancer.[60] Osteosarcoma may be promoted by growth hormones.[60] Some treatments and prevention approaches leH16H16H30H48H65H96H127H158H189H220H251H282H313H344H375H406H437H468H499H530H499H468H437H406H375H344H313H282H251H220H189H158H127H96H69verage this cause by artificially reducing hormone levels and thus discouraging hormone-sensitive cancers.[60]Autoimmune diseasesThere is an association between celiac disease and an increased risk of all cancers. People with untreated celiac disease have a higher risk, but this risk decreases with time after diagnosis and strict treatment, probably due to the adoption of a gluten-free diet, which seems to have a protective role against development of malignancy in people with celiac disease. However, the delay in diagnosis and initiation of a gluten-free diet seems to increase the risk of malignancies.[62] Rates of gastrointestinal cancers are increased in people with Crohn's disease and ulcerative colitis, due to chronic inflammation. Also, immunomodulators and biologic agents used to treat these diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur through..these diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur through..these diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur through.. these diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur throughthese diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur throughthese diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur throughthese diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression or disabling of tumor suppressor genes. Typically, changes in multiple genes are required to transform a normal cell into a cancer cell.[65]Genetic changes can occur at different levels and by different mechanisms. The gain or loss of an entire chromosome can occur throughthese diseases may promote developing extra-intestinal malignancies.[63]PathophysiologyMain article: CarcinogenesisCancers are caused by a series of mutations. Each mutation alters the behavior of the cell somewhat.GeneticsCancer is fundamentally a disease of tissue growth regulation. In order for a normal cell to transform into a cancer cell, the genes that regulate cell growth and differentiation must be altered.[64]The affected genes are divided into two broad categories. Oncogenes are genes that promote cell growth and reproduction. Tumor suppressor genes are genes that inhibit cell division and survival. Malignant transformation can occur through the formation of novel oncogenes, the inappropriate over-expression of normal oncogenes, or by the under-expression o||title=Large Content 27,350 chars test from API - About Cancer from Wikipedia||wasCleanedUp=2||wasTruncated=true||found=true</t>
+  </si>
+  <si>
+    <t>OPQA-4035</t>
+  </si>
+  <si>
+    <t>OPQA-4036</t>
+  </si>
+  <si>
+    <t>OPQA-4037</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-4037_id)</t>
+  </si>
+  <si>
+    <t>{ "targetType":"posts", "targetId":"(OPQA-4037_id)", "content":"Comment test on supported tags emphasis, strong. Example on emphasis tag: &lt;em&gt;This is emphasis tag &lt;/em&gt;  Example on strong tag: &lt;strong&gt;This is strong tag &lt;/strong&gt;" }</t>
+  </si>
+  <si>
+    <t>OPQA-286_5||OPQA-4037</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=posts||comments.targetId=(OPQA-4037_id)||comments.content=Comment test on supported tags emphasis, strong. Example on emphasis tag: &lt;em&gt;This is emphasis tag &lt;/em&gt;  Example on strong tag: &lt;strong&gt;This is strong tag &lt;/strong&gt;||comments.status=PUBLISHED||comments.wasCleanedUp=0||comments.wasTruncated=false||found=true</t>
+  </si>
+  <si>
+    <t>{ "targetType":"posts", "targetId":"(OPQA-4037_id)", "content":"Edit Comment test with supported tags emphasis, strong tags for a post. Example on emphasis tag: &lt;em&gt;This is edited emphasis tag &lt;/em&gt;   Example on strong tag: &lt;strong&gt;This is edited strong tag &lt;/strong&gt;" }</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4037_id)||userId=(SYS_USER2)||title=Supported tags test from API - Edited Post||content=''||wasCleanedUp=0||wasTruncated=false||found=true</t>
+  </si>
+  <si>
+    <t>OPQA-4038</t>
+  </si>
+  <si>
+    <t>OPQA-4039</t>
+  </si>
+  <si>
+    <t>OPQA-4040</t>
+  </si>
+  <si>
+    <t>OPQA-4041</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-4041_id)</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4041_id)||userId=(SYS_USER2)||title=Large Content 27,350 chars test from API - About Cancer from Wikipedia||content=''||wasCleanedUp=0||wasTruncated=false||found=true</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-4039_comments.id)</t>
+  </si>
+  <si>
+    <t>OPQA-4037||OPQA-4039</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4039_comments.id)||userId=(SYS_USER2)||targetType=posts||targetId=(OPQA-4037_id)||content=Edit Comment test with supported tags emphasis, strong tags for a post. Example on emphasis tag: &lt;em&gt;This is edited emphasis tag &lt;/em&gt;   Example on strong tag: &lt;strong&gt;This is edited strong tag &lt;/strong&gt;||wasCleanedUp=0||wasTruncated=false||found=true</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4039_comments.id)||userId=(SYS_USER2)||targetType=posts||targetId=(OPQA-4037_id)||content=''||wasCleanedUp=0||wasTruncated=false||found=true</t>
   </si>
 </sst>
 </file>
@@ -1471,7 +1615,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1513,6 +1657,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1810,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" topLeftCell="I50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L50" sqref="L2:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1870,23 +2017,23 @@
     </row>
     <row r="2" spans="1:12" s="17" customFormat="1" ht="45">
       <c r="A2" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>397</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>398</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="18" t="s">
         <v>399</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>400</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="1"/>
@@ -1894,7 +2041,7 @@
         <v>11</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L2"/>
     </row>
@@ -1909,7 +2056,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
@@ -1918,7 +2065,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>11</v>
@@ -1946,11 +2093,11 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>93</v>
@@ -1979,13 +2126,13 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>407</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>20</v>
@@ -2013,10 +2160,10 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>26</v>
@@ -2045,13 +2192,13 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>409</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>410</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>20</v>
@@ -2079,10 +2226,10 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>25</v>
@@ -2111,13 +2258,13 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>412</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>413</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9"/>
@@ -2143,13 +2290,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>96</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K10" s="8"/>
       <c r="L10"/>
@@ -2175,13 +2322,13 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>416</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>417</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11"/>
@@ -2207,13 +2354,13 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>96</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12"/>
@@ -2266,10 +2413,10 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14"/>
@@ -2359,13 +2506,13 @@
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>96</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K17" s="8"/>
       <c r="L17"/>
@@ -2391,7 +2538,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>96</v>
@@ -2647,7 +2794,7 @@
         <v>96</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26"/>
@@ -2677,7 +2824,7 @@
         <v>106</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K27" s="8"/>
       <c r="L27"/>
@@ -2703,13 +2850,13 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>425</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>426</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>20</v>
@@ -2737,13 +2884,13 @@
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>139</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29"/>
@@ -2773,7 +2920,7 @@
         <v>139</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K30" s="8"/>
       <c r="L30"/>
@@ -2829,7 +2976,7 @@
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>135</v>
@@ -2915,7 +3062,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
@@ -2924,7 +3071,7 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>29</v>
@@ -2943,7 +3090,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>0</v>
@@ -2952,7 +3099,7 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>11</v>
@@ -3057,7 +3204,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>0</v>
@@ -3066,7 +3213,7 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>11</v>
@@ -3097,7 +3244,7 @@
         <v>96</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K41" s="8"/>
       <c r="L41"/>
@@ -3123,10 +3270,10 @@
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>11</v>
@@ -3305,7 +3452,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>0</v>
@@ -3314,7 +3461,7 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>11</v>
@@ -3326,10 +3473,10 @@
     </row>
     <row r="49" spans="1:12" ht="240">
       <c r="A49" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>441</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>442</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>14</v>
@@ -3344,13 +3491,13 @@
         <v>21</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>94</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K49" s="8" t="s">
         <v>20</v>
@@ -3367,7 +3514,7 @@
         <v>14</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>19</v>
@@ -3378,7 +3525,7 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>11</v>
@@ -3394,10 +3541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="J44" workbookViewId="0">
-      <selection activeCell="L51" sqref="L2:L51"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3905,7 +4052,7 @@
       <c r="E16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="8"/>
@@ -3921,50 +4068,48 @@
       <c r="K16" s="8"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A17" s="8" t="s">
-        <v>212</v>
+    <row r="17" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A17" t="s">
+        <v>480</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>211</v>
+        <v>467</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>200</v>
+        <v>464</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="H17" s="4"/>
       <c r="I17" s="8" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>201</v>
+        <v>465</v>
       </c>
       <c r="K17" s="8"/>
       <c r="L17"/>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>16</v>
@@ -3977,174 +4122,173 @@
         <v>17</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="K18" s="8"/>
       <c r="L18"/>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="4" t="s">
-        <v>18</v>
+      <c r="H19" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>268</v>
+        <v>208</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" ht="30">
-      <c r="A20" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>59</v>
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A20" t="s">
+        <v>481</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>466</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>36</v>
+      <c r="D20" s="8" t="s">
+        <v>468</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="4" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>469</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" ht="30">
+    <row r="21" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A21" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>67</v>
+        <v>216</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>215</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>41</v>
+      <c r="D21" s="8" t="s">
+        <v>230</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>178</v>
+        <v>16</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>268</v>
       </c>
       <c r="K21" s="8"/>
+      <c r="L21"/>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A22" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>229</v>
+      <c r="D22" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="H22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>25</v>
+      <c r="H22" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="K22" s="8"/>
       <c r="L22"/>
     </row>
     <row r="23" spans="1:12" ht="30">
       <c r="A23" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>231</v>
+      <c r="D23" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="8"/>
       <c r="I23" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>25</v>
+      <c r="J23" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:12" ht="45">
+    <row r="24" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A24" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>14</v>
@@ -4156,7 +4300,7 @@
         <v>16</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="4" t="s">
@@ -4165,455 +4309,463 @@
       <c r="I24" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K24" s="8"/>
+      <c r="L24"/>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="A25" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>41</v>
+        <v>231</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="I25" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>182</v>
+      <c r="J25" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="K25" s="8"/>
     </row>
-    <row r="26" spans="1:12" ht="30">
+    <row r="26" spans="1:12" ht="45">
       <c r="A26" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I26" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>183</v>
+      <c r="J26" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:12" ht="30">
       <c r="A27" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>84</v>
+        <v>222</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>272</v>
+        <v>41</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+      <c r="G27" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="H27" s="8"/>
-      <c r="I27" s="8" t="s">
-        <v>450</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>280</v>
+      <c r="I27" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:12" ht="30">
       <c r="A28" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>85</v>
+        <v>223</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>271</v>
+        <v>179</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="G28" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="H28" s="8"/>
-      <c r="I28" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>279</v>
+      <c r="I28" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="K28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="45">
+    <row r="29" spans="1:12" ht="30">
       <c r="A29" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>232</v>
+        <v>272</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="8"/>
-      <c r="G29" s="8" t="s">
-        <v>184</v>
-      </c>
+      <c r="G29" s="8"/>
       <c r="H29" s="8"/>
-      <c r="I29" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>269</v>
+      <c r="I29" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>280</v>
       </c>
       <c r="K29" s="8"/>
     </row>
-    <row r="30" spans="1:12" ht="45">
+    <row r="30" spans="1:12" ht="30">
       <c r="A30" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="8" t="s">
-        <v>187</v>
-      </c>
+      <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J30" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" ht="45">
+      <c r="A31" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" ht="45">
+      <c r="A32" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="K30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" ht="30">
-      <c r="A31" s="8" t="s">
+      <c r="K32" s="8"/>
+    </row>
+    <row r="33" spans="1:12" ht="30">
+      <c r="A33" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="C33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="4" t="s">
+      <c r="E33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="3" t="s">
+      <c r="G33" s="8"/>
+      <c r="H33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="I33" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="K31" s="8"/>
-    </row>
-    <row r="32" spans="1:12" ht="30">
-      <c r="A32" s="8" t="s">
+      <c r="K33" s="8"/>
+    </row>
+    <row r="34" spans="1:12" ht="30">
+      <c r="A34" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="8" t="s">
+      <c r="C34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="4" t="s">
+      <c r="E34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="K32" s="8"/>
-    </row>
-    <row r="33" spans="1:12" ht="45">
-      <c r="A33" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K33" s="8"/>
-    </row>
-    <row r="34" spans="1:12" ht="45">
-      <c r="A34" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>360</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>177</v>
+        <v>89</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>199</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>362</v>
+        <v>203</v>
       </c>
       <c r="K34" s="8"/>
     </row>
-    <row r="35" spans="1:12" ht="30">
+    <row r="35" spans="1:12" ht="45">
       <c r="A35" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>301</v>
+        <v>309</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>305</v>
+        <v>243</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G35" s="8"/>
-      <c r="H35" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>307</v>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="K35" s="8"/>
     </row>
-    <row r="36" spans="1:12" ht="30">
+    <row r="36" spans="1:12" ht="45">
       <c r="A36" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>302</v>
+        <v>372</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>357</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>305</v>
+        <v>358</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>23</v>
+        <v>359</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>314</v>
+        <v>360</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>309</v>
+        <v>361</v>
       </c>
       <c r="K36" s="8"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" ht="30">
       <c r="A37" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B37" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>186</v>
-      </c>
       <c r="E37" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8" t="s">
-        <v>185</v>
+      <c r="H37" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="K37" s="8"/>
     </row>
     <row r="38" spans="1:12" ht="30">
       <c r="A38" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="K38" s="8"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K39" s="8"/>
+    </row>
+    <row r="40" spans="1:12" ht="30">
+      <c r="A40" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="K38" s="8"/>
-    </row>
-    <row r="39" spans="1:12" ht="30">
-      <c r="A39" t="s">
-        <v>247</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" t="s">
-        <v>249</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G39" t="s">
-        <v>250</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="30">
-      <c r="A40" t="s">
-        <v>252</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>253</v>
+      <c r="B40" s="9" t="s">
+        <v>356</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>14</v>
@@ -4630,54 +4782,51 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="3" t="s">
-        <v>244</v>
+        <v>177</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>254</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="K40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>179</v>
+      <c r="D41" t="s">
+        <v>249</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G41" s="8"/>
-      <c r="H41" s="5" t="s">
-        <v>274</v>
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>250</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>244</v>
+        <v>177</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30">
       <c r="A42" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>19</v>
@@ -4688,233 +4837,231 @@
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="3" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>229</v>
+        <v>179</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="5" t="s">
-        <v>17</v>
+        <v>274</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="J43" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="45">
+    <row r="44" spans="1:12" ht="30">
       <c r="A44" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="30">
+      <c r="A45" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="2" customFormat="1" ht="45">
-      <c r="A45" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="E45" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>21</v>
+      <c r="F45" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="45">
+      <c r="A46" t="s">
+        <v>263</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="2" customFormat="1" ht="45">
+      <c r="A47" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="1:12" ht="30">
+      <c r="A48" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="I45" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L45"/>
-    </row>
-    <row r="46" spans="1:12" ht="30">
-      <c r="A46" s="8" t="s">
+      <c r="E48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="K48" s="8"/>
+    </row>
+    <row r="49" spans="1:11" ht="30">
+      <c r="A49" t="s">
         <v>355</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="I46" s="8" t="s">
+      <c r="B49" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="J46" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="K46" s="8"/>
-    </row>
-    <row r="47" spans="1:12" ht="30">
-      <c r="A47" t="s">
-        <v>356</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="5" t="s">
+      <c r="E49" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="30">
-      <c r="A48" t="s">
+      <c r="I49" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="30">
+      <c r="A50" t="s">
+        <v>373</v>
+      </c>
+      <c r="B50" s="13" t="s">
         <v>374</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="G48" s="8"/>
-      <c r="H48" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="I48" s="8"/>
-      <c r="J48" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" t="s">
-        <v>374</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="K49" s="8"/>
-    </row>
-    <row r="50" spans="1:11" ht="60">
-      <c r="A50" t="s">
-        <v>381</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>380</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>14</v>
@@ -4926,17 +5073,15 @@
         <v>16</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="I50" s="8" t="s">
-        <v>376</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="I50" s="8"/>
       <c r="J50" s="5" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>38</v>
@@ -4944,32 +5089,336 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="8" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" t="s">
+        <v>373</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="K51" s="8"/>
+    </row>
+    <row r="52" spans="1:11" ht="60">
+      <c r="A52" t="s">
+        <v>380</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="G52" s="8"/>
+      <c r="H52" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="J51" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="K51" s="8"/>
+      <c r="B53" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" t="s">
+        <v>380</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="K53" s="8"/>
+    </row>
+    <row r="54" spans="1:11" ht="75">
+      <c r="A54" t="s">
+        <v>482</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>455</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="8"/>
+      <c r="H54" s="19" t="s">
+        <v>471</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="75">
+      <c r="A55" t="s">
+        <v>489</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H55" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="I55" t="s">
+        <v>482</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="45">
+      <c r="A56" t="s">
+        <v>490</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="8"/>
+      <c r="H56" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="60">
+      <c r="A57" t="s">
+        <v>491</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="I57" t="s">
+        <v>496</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="45">
+      <c r="A58" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" t="s">
+        <v>490</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="30">
+      <c r="A59" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" t="s">
+        <v>482</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="210">
+      <c r="A60" t="s">
+        <v>492</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" s="8"/>
+      <c r="H60" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="J60" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="30">
+      <c r="A61" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" t="s">
+        <v>492</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>494</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4978,10 +5427,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="I18" workbookViewId="0">
-      <selection activeCell="L24" sqref="L2:L24"/>
+    <sheetView topLeftCell="I21" workbookViewId="0">
+      <selection activeCell="L26" sqref="L2:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5039,16 +5488,16 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>0</v>
@@ -5057,7 +5506,7 @@
         <v>27</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
@@ -5065,10 +5514,10 @@
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -5086,18 +5535,18 @@
         <v>284</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -5109,21 +5558,24 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>21</v>
+        <v>359</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="75">
+        <v>451</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45">
       <c r="A5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -5135,137 +5587,140 @@
         <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="75">
+      <c r="A6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="H6" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="K6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30">
-      <c r="A6" t="s">
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>318</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>317</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="75">
+      <c r="A8" t="s">
         <v>335</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>319</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>318</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="75">
-      <c r="A7" t="s">
-        <v>336</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>294</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="B8" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>293</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="H8" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="30">
-      <c r="A8" t="s">
-        <v>337</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>319</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="I8" t="s">
-        <v>318</v>
+        <v>475</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>321</v>
+        <v>312</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>437</v>
+        <v>336</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>435</v>
+        <v>287</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>291</v>
+        <v>318</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="I9" t="s">
-        <v>438</v>
+        <v>317</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>439</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
-      <c r="A10" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>394</v>
+      <c r="A10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>434</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>390</v>
+        <v>290</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>0</v>
@@ -5274,276 +5729,270 @@
         <v>27</v>
       </c>
       <c r="I10" t="s">
+        <v>437</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="11" spans="1:12" ht="30">
-      <c r="A11" t="s">
-        <v>340</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>339</v>
+      <c r="A11" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>393</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>292</v>
+        <v>389</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G11" t="s">
-        <v>322</v>
+      <c r="F11" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="I11" t="s">
-        <v>318</v>
+        <v>437</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>323</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>341</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>293</v>
+        <v>339</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>324</v>
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>321</v>
       </c>
       <c r="I12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="K12" t="s">
-        <v>38</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
+        <v>340</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>293</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="I13" t="s">
+        <v>317</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="K13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>318</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>340</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" t="s">
         <v>348</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>319</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>341</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45">
-      <c r="A14" t="s">
-        <v>349</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>333</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" t="s">
-        <v>331</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30">
-      <c r="A15" t="s">
-        <v>350</v>
-      </c>
       <c r="B15" s="13" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>333</v>
+        <v>453</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>296</v>
+        <v>27</v>
       </c>
       <c r="I15" t="s">
-        <v>331</v>
+        <v>450</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>333</v>
+        <v>453</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>296</v>
+        <v>377</v>
       </c>
       <c r="I16" t="s">
-        <v>331</v>
+        <v>450</v>
       </c>
       <c r="J16" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30">
+      <c r="A17" t="s">
+        <v>350</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>332</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="I17" t="s">
+        <v>330</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="45">
-      <c r="A17" t="s">
-        <v>352</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="18" spans="1:11" ht="45">
+      <c r="A18" t="s">
+        <v>351</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="45">
-      <c r="A18" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>353</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="H18" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="I18" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="45">
+      <c r="A19" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" ht="60">
-      <c r="A19" t="s">
-        <v>354</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="14" t="s">
-        <v>343</v>
-      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30">
-      <c r="A20" s="8" t="s">
-        <v>367</v>
+        <v>351</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="60">
+      <c r="A20" t="s">
+        <v>353</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>345</v>
+      <c r="D20" t="s">
+        <v>15</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>16</v>
@@ -5551,122 +6000,182 @@
       <c r="F20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="I20" t="s">
-        <v>341</v>
+      <c r="H20" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>340</v>
       </c>
       <c r="J20" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="K20" s="8"/>
-    </row>
-    <row r="21" spans="1:11" ht="30">
-      <c r="A21" t="s">
-        <v>368</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>360</v>
+        <v>23</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8" t="s">
-        <v>361</v>
+        <v>305</v>
       </c>
       <c r="I21" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>346</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" t="s">
-        <v>396</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>391</v>
+        <v>367</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>302</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="I22" t="s">
+        <v>366</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30">
+      <c r="A23" t="s">
+        <v>395</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="45">
-      <c r="A23" t="s">
-        <v>397</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s">
-        <v>291</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="45">
-      <c r="A24" s="8" t="s">
+      <c r="A24" t="s">
+        <v>396</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>290</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45">
+      <c r="A25" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>448</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" t="s">
-        <v>354</v>
-      </c>
-      <c r="J24" s="4" t="s">
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" t="s">
+        <v>353</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="8"/>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" ht="30">
+      <c r="A26" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" t="s">
+        <v>335</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>472</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated 1PSEARCHV4 dependent test cases in Authoring, ProjectContainer, WatchlistContainer
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Authoring-wos and patents" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="501">
   <si>
     <t>GET</t>
   </si>
@@ -1212,114 +1212,15 @@
     <t>Verify that to get articles for query</t>
   </si>
   <si>
-    <t>1PSEARCHV3</t>
-  </si>
-  <si>
     <t>/wos/search</t>
   </si>
   <si>
     <t>?query=biology</t>
   </si>
   <si>
-    <t>hits.hits[0]._id||hits.hits[1]._id</t>
-  </si>
-  <si>
     <t>OPQA-896_1</t>
   </si>
   <si>
-    <t>/comments/count/(OPQA-896_1_hits.hits[0]._id)/wos</t>
-  </si>
-  <si>
-    <t>?id=(OPQA-896_1_hits.hits[0]._id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment test from API by User 1"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=Comment test from API by User 1</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment test from API by User 1 and Created within 60 sec of previous comment"}</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"mohana.yalamarthi@thomsonreuters.com        http://thomsonreuters.com/en.html         +91 8197818719"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Wrong data test : server error expectation"}</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while creating comment by User 1&lt;abcd&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=Tags clean up surround tags like abcd while creating comment by User 1</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while editing comment by User 1&lt;abcd&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||content=Tags clean up surround tags like abcd while editing comment by User 1||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"FUCK"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=****</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||content=****</t>
-  </si>
-  <si>
-    <t>status=200||size=(OPQA-331_counterValue)||found=true||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Update own comment"}</t>
-  </si>
-  <si>
-    <t>status=200||content=Update own comment||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Edited content"}</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-236_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-315_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||content=HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-245_comments.id)||content=""</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"hi"}</t>
-  </si>
-  <si>
-    <t>/comments/count/(OPQA-896_1_hits.hits[0]._id)/</t>
-  </si>
-  <si>
-    <t>/comments/(OPQA-896_1_hits.hits[0]._id)/wos</t>
-  </si>
-  <si>
-    <t>status=200||found=true||targetType=wos||targetId=(OPQA-896_1_hits.hits[0]._id)||id=(OPQA-236_comments.id)</t>
-  </si>
-  <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment report tesintg"}</t>
-  </si>
-  <si>
     <t>Verfiy that the Drafts Post tab displays the count of the saved drafts correctly</t>
   </si>
   <si>
@@ -1344,9 +1245,6 @@
     <t>Verify that API truncated the comment length to 2500 characters while creating/Editing the comment</t>
   </si>
   <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits.hits[0]._id)","content":"Comment Max Length Test: As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher,&gt;1500I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge...! &gt;2500"}</t>
-  </si>
-  <si>
     <t>/comments/comment/(OPQA-682_comments.id)</t>
   </si>
   <si>
@@ -1362,9 +1260,6 @@
     <t>/comments/comment/(OPQA-1093_comments.id)</t>
   </si>
   <si>
-    <t>status=200||size=eval$(OPQA-344_1_counterValue)+1||comments.userId=(SYS_USER1)||comments.targetId=(OPQA-896_1_hits.hits[0]._id)||comments.targetType=wos||comments.content=Comment Max Length Test: As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher,&gt;1500I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge...!||comments.wasTruncated=true</t>
-  </si>
-  <si>
     <t>OPQA-377||OPQA-385</t>
   </si>
   <si>
@@ -1513,12 +1408,124 @@
   </si>
   <si>
     <t>status=200||id=(OPQA-4039_comments.id)||userId=(SYS_USER2)||targetType=posts||targetId=(OPQA-4037_id)||content=''||wasCleanedUp=0||wasTruncated=false||found=true</t>
+  </si>
+  <si>
+    <t>/comments/count/(OPQA-896_1_hits[0].id)/wos</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-896_1_hits[0].id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"Comment test from API by User 1"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits[0].id)||comments.content=Comment test from API by User 1</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"Comment test from API by User 1 and Created within 60 sec of previous comment"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"mohana.yalamarthi@thomsonreuters.com        http://thomsonreuters.com/en.html         +91 8197818719"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits[0].id)||comments.content=mohana.yalamarthi@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"Wrong data test : server error expectation"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while creating comment by User 1&lt;abcd&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits[0].id)||comments.content=Tags clean up surround tags like abcd while creating comment by User 1</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"&lt;abcd&gt;Tags clean up surround tags like abcd while editing comment by User 1&lt;abcd&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||content=Tags clean up surround tags like abcd while editing comment by User 1||targetType=wos||targetId=(OPQA-896_1_hits[0].id)||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"FUCK"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits[0].id)||comments.content=****</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=(OPQA-896_1_hits[0].id)||content=****</t>
+  </si>
+  <si>
+    <t>status=200||size=(OPQA-331_counterValue)||found=true||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits[0].id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"Update own comment"}</t>
+  </si>
+  <si>
+    <t>status=200||content=Update own comment||targetType=wos||targetId=(OPQA-896_1_hits[0].id)||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"Edited content"}</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits[0].id)||id=(OPQA-236_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits[0].id)||id=(OPQA-315_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER1)||comments.targetType=wos||comments.targetId=(OPQA-896_1_hits[0].id)||comments.content=Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;"}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||targetType=wos||targetId=(OPQA-896_1_hits[0].id)||content=HTML edited content Test:: Hello &lt;b&gt;I am in bold&lt;/b&gt; and &lt;i&gt;I am in italic&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>status=200||targetType=wos||targetId=(OPQA-896_1_hits[0].id)||id=(OPQA-245_comments.id)||content=""</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"hi"}</t>
+  </si>
+  <si>
+    <t>/comments/count/(OPQA-896_1_hits[0].id)/</t>
+  </si>
+  <si>
+    <t>/comments/(OPQA-896_1_hits[0].id)/wos</t>
+  </si>
+  <si>
+    <t>status=200||found=true||targetType=wos||targetId=(OPQA-896_1_hits[0].id)||id=(OPQA-236_comments.id)</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"Comment report tesintg"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"wos","targetId":"(OPQA-896_1_hits[0].id)","content":"Comment Max Length Test: As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher,&gt;1500I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters’ research content so that I can discover new data, contribute to the knowledge...! &gt;2500"}</t>
+  </si>
+  <si>
+    <t>status=200||size=eval$(OPQA-344_1_counterValue)+1||comments.userId=(SYS_USER1)||comments.targetId=(OPQA-896_1_hits[0].id)||comments.targetType=wos||comments.content=Comment Max Length Test: As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher,&gt;1500I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge base, make connections to my peers and gain exposure to others in my field. As a researcher, I want to interact with Thomson Reuters? research content so that I can discover new data, contribute to the knowledge...!||comments.wasTruncated=true</t>
+  </si>
+  <si>
+    <t>1PSEARCHV4</t>
+  </si>
+  <si>
+    <t>hits[0].id||hits[1].id</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1957,24 +1964,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L50" sqref="L2:L50"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="68.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="119.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="43.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="80.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="47.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="68.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="119.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2015,25 +2022,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="17" customFormat="1" ht="45">
+    <row r="2" spans="1:12" s="17" customFormat="1" ht="30">
       <c r="A2" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>397</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>497</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>398</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>399</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="1"/>
@@ -2041,9 +2048,11 @@
         <v>11</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>401</v>
-      </c>
-      <c r="L2"/>
+        <v>498</v>
+      </c>
+      <c r="L2" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A3" s="8" t="s">
@@ -2056,7 +2065,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>403</v>
+        <v>464</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
@@ -2065,7 +2074,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>11</v>
@@ -2073,7 +2082,9 @@
       <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3"/>
+      <c r="L3" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A4" s="8" t="s">
@@ -2093,17 +2104,19 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>404</v>
+        <v>465</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>93</v>
       </c>
       <c r="K4" s="8"/>
-      <c r="L4"/>
+      <c r="L4" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A5" s="8" t="s">
@@ -2126,18 +2139,20 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>405</v>
+        <v>466</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>406</v>
+        <v>467</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L5"/>
+      <c r="L5" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A6" s="8" t="s">
@@ -2160,16 +2175,18 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="5" t="s">
-        <v>407</v>
+        <v>468</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="L6"/>
+      <c r="L6" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A7" s="8" t="s">
@@ -2192,18 +2209,20 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
-        <v>408</v>
+        <v>469</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>409</v>
+        <v>470</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L7"/>
+      <c r="L7" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A8" s="8" t="s">
@@ -2226,16 +2245,18 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5" t="s">
-        <v>410</v>
+        <v>471</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="L8"/>
+      <c r="L8" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A9" s="8" t="s">
@@ -2258,16 +2279,18 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="5" t="s">
-        <v>411</v>
+        <v>472</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>412</v>
+        <v>473</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="L9"/>
+      <c r="L9" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A10" s="8" t="s">
@@ -2290,16 +2313,18 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="5" t="s">
-        <v>413</v>
+        <v>474</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>96</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>414</v>
+        <v>475</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10"/>
+      <c r="L10" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A11" s="8" t="s">
@@ -2322,16 +2347,18 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="4" t="s">
-        <v>415</v>
+        <v>476</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>416</v>
+        <v>477</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="L11"/>
+      <c r="L11" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A12" s="8" t="s">
@@ -2354,16 +2381,18 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="4" t="s">
-        <v>415</v>
+        <v>476</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>96</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>417</v>
+        <v>478</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12"/>
+      <c r="L12" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A13" s="8" t="s">
@@ -2391,7 +2420,9 @@
       <c r="K13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L13"/>
+      <c r="L13" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A14" s="8" t="s">
@@ -2413,13 +2444,15 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>418</v>
+        <v>479</v>
       </c>
       <c r="K14" s="8"/>
-      <c r="L14"/>
+      <c r="L14" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A15" s="8" t="s">
@@ -2451,7 +2484,9 @@
         <v>25</v>
       </c>
       <c r="K15" s="8"/>
-      <c r="L15"/>
+      <c r="L15" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A16" s="8" t="s">
@@ -2483,7 +2518,9 @@
         <v>25</v>
       </c>
       <c r="K16" s="8"/>
-      <c r="L16"/>
+      <c r="L16" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A17" s="8" t="s">
@@ -2506,16 +2543,18 @@
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="5" t="s">
-        <v>419</v>
+        <v>480</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>96</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>420</v>
+        <v>481</v>
       </c>
       <c r="K17" s="8"/>
-      <c r="L17"/>
+      <c r="L17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
@@ -2538,7 +2577,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="4" t="s">
-        <v>421</v>
+        <v>482</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>96</v>
@@ -2547,7 +2586,9 @@
         <v>29</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18"/>
+      <c r="L18" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
@@ -2579,7 +2620,9 @@
         <v>99</v>
       </c>
       <c r="K19" s="8"/>
-      <c r="L19"/>
+      <c r="L19" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A20" s="8" t="s">
@@ -2611,7 +2654,9 @@
         <v>108</v>
       </c>
       <c r="K20" s="8"/>
-      <c r="L20"/>
+      <c r="L20" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A21" s="8" t="s">
@@ -2643,7 +2688,9 @@
         <v>25</v>
       </c>
       <c r="K21" s="8"/>
-      <c r="L21"/>
+      <c r="L21" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A22" s="8" t="s">
@@ -2673,7 +2720,9 @@
         <v>101</v>
       </c>
       <c r="K22" s="8"/>
-      <c r="L22"/>
+      <c r="L22" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="23" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A23" s="8" t="s">
@@ -2705,7 +2754,9 @@
         <v>102</v>
       </c>
       <c r="K23" s="8"/>
-      <c r="L23"/>
+      <c r="L23" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="24" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A24" s="8" t="s">
@@ -2737,7 +2788,9 @@
         <v>109</v>
       </c>
       <c r="K24" s="8"/>
-      <c r="L24"/>
+      <c r="L24" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="25" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A25" s="8" t="s">
@@ -2767,7 +2820,9 @@
         <v>29</v>
       </c>
       <c r="K25" s="8"/>
-      <c r="L25"/>
+      <c r="L25" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="26" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A26" s="8" t="s">
@@ -2794,10 +2849,12 @@
         <v>96</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="K26" s="8"/>
-      <c r="L26"/>
+      <c r="L26" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="27" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A27" s="8" t="s">
@@ -2824,10 +2881,12 @@
         <v>106</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>423</v>
+        <v>484</v>
       </c>
       <c r="K27" s="8"/>
-      <c r="L27"/>
+      <c r="L27" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="28" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A28" s="8" t="s">
@@ -2850,18 +2909,20 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5" t="s">
-        <v>424</v>
+        <v>485</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>445</v>
+        <v>411</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>425</v>
+        <v>486</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L28"/>
+      <c r="L28" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="29" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A29" s="8" t="s">
@@ -2884,16 +2945,18 @@
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="5" t="s">
-        <v>426</v>
+        <v>487</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>139</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>427</v>
+        <v>488</v>
       </c>
       <c r="K29" s="3"/>
-      <c r="L29"/>
+      <c r="L29" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="30" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A30" s="8" t="s">
@@ -2920,10 +2983,12 @@
         <v>139</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>428</v>
+        <v>489</v>
       </c>
       <c r="K30" s="8"/>
-      <c r="L30"/>
+      <c r="L30" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="31" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A31" s="8" t="s">
@@ -2953,7 +3018,9 @@
         <v>25</v>
       </c>
       <c r="K31" s="8"/>
-      <c r="L31"/>
+      <c r="L31" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="32" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A32" s="8" t="s">
@@ -2976,7 +3043,7 @@
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="5" t="s">
-        <v>429</v>
+        <v>490</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>135</v>
@@ -2985,7 +3052,9 @@
         <v>25</v>
       </c>
       <c r="K32" s="8"/>
-      <c r="L32"/>
+      <c r="L32" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="33" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A33" s="8" t="s">
@@ -3017,7 +3086,9 @@
         <v>25</v>
       </c>
       <c r="K33" s="8"/>
-      <c r="L33"/>
+      <c r="L33" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="34" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A34" s="8" t="s">
@@ -3049,7 +3120,9 @@
         <v>25</v>
       </c>
       <c r="K34" s="8"/>
-      <c r="L34"/>
+      <c r="L34" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="35" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A35" s="8" t="s">
@@ -3062,7 +3135,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>430</v>
+        <v>491</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
@@ -3071,13 +3144,15 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K35" s="3"/>
-      <c r="L35"/>
+      <c r="L35" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="36" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A36" s="8" t="s">
@@ -3090,7 +3165,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>431</v>
+        <v>492</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>0</v>
@@ -3099,13 +3174,15 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K36" s="8"/>
-      <c r="L36"/>
+      <c r="L36" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="37" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A37" s="8" t="s">
@@ -3133,7 +3210,9 @@
         <v>29</v>
       </c>
       <c r="K37" s="8"/>
-      <c r="L37"/>
+      <c r="L37" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="38" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A38" s="8" t="s">
@@ -3163,7 +3242,9 @@
         <v>29</v>
       </c>
       <c r="K38" s="8"/>
-      <c r="L38"/>
+      <c r="L38" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="39" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A39" s="8" t="s">
@@ -3191,7 +3272,9 @@
         <v>29</v>
       </c>
       <c r="K39" s="8"/>
-      <c r="L39"/>
+      <c r="L39" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="40" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A40" s="8" t="s">
@@ -3204,7 +3287,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>431</v>
+        <v>492</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>0</v>
@@ -3213,13 +3296,15 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K40" s="8"/>
-      <c r="L40"/>
+      <c r="L40" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="41" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A41" s="8" t="s">
@@ -3244,10 +3329,12 @@
         <v>96</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>432</v>
+        <v>493</v>
       </c>
       <c r="K41" s="8"/>
-      <c r="L41"/>
+      <c r="L41" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="42" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A42" s="8" t="s">
@@ -3270,10 +3357,10 @@
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="4" t="s">
-        <v>433</v>
+        <v>494</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>11</v>
@@ -3281,7 +3368,9 @@
       <c r="K42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L42"/>
+      <c r="L42" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="43" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A43" s="8" t="s">
@@ -3313,7 +3402,9 @@
         <v>25</v>
       </c>
       <c r="K43" s="8"/>
-      <c r="L43"/>
+      <c r="L43" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="44" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A44" s="8" t="s">
@@ -3345,7 +3436,9 @@
         <v>166</v>
       </c>
       <c r="K44" s="8"/>
-      <c r="L44"/>
+      <c r="L44" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="45" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A45" s="8" t="s">
@@ -3377,7 +3470,9 @@
         <v>168</v>
       </c>
       <c r="K45" s="8"/>
-      <c r="L45"/>
+      <c r="L45" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="46" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A46" s="8" t="s">
@@ -3407,7 +3502,9 @@
         <v>11</v>
       </c>
       <c r="K46" s="8"/>
-      <c r="L46"/>
+      <c r="L46" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="47" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A47" s="8" t="s">
@@ -3439,7 +3536,9 @@
         <v>25</v>
       </c>
       <c r="K47" s="8"/>
-      <c r="L47"/>
+      <c r="L47" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="48" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A48" s="8" t="s">
@@ -3452,7 +3551,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>403</v>
+        <v>464</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>0</v>
@@ -3461,7 +3560,7 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>11</v>
@@ -3469,14 +3568,16 @@
       <c r="K48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L48"/>
+      <c r="L48" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="49" spans="1:12" ht="240">
       <c r="A49" s="8" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>441</v>
+        <v>408</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>14</v>
@@ -3490,17 +3591,21 @@
       <c r="F49" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="G49"/>
       <c r="H49" s="14" t="s">
-        <v>442</v>
+        <v>495</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>94</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>448</v>
+        <v>496</v>
       </c>
       <c r="K49" s="8" t="s">
         <v>20</v>
+      </c>
+      <c r="L49" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="2" customFormat="1" ht="45">
@@ -3514,7 +3619,7 @@
         <v>14</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>443</v>
+        <v>409</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>19</v>
@@ -3525,13 +3630,15 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="5" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K50" s="8"/>
-      <c r="L50"/>
+      <c r="L50" t="s">
+        <v>500</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3543,24 +3650,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="58.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="45" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="133.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="42.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="58.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="80.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="133.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3631,7 +3738,9 @@
       <c r="K2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L2"/>
+      <c r="L2" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A3" s="8" t="s">
@@ -3663,7 +3772,9 @@
       <c r="K3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L3"/>
+      <c r="L3" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A4" s="8" t="s">
@@ -3695,7 +3806,9 @@
         <v>26</v>
       </c>
       <c r="K4" s="3"/>
-      <c r="L4"/>
+      <c r="L4" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A5" s="8" t="s">
@@ -3723,7 +3836,9 @@
         <v>180</v>
       </c>
       <c r="K5" s="8"/>
-      <c r="L5"/>
+      <c r="L5" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A6" s="8" t="s">
@@ -3753,7 +3868,9 @@
         <v>180</v>
       </c>
       <c r="K6" s="8"/>
-      <c r="L6"/>
+      <c r="L6" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A7" s="8" t="s">
@@ -3781,7 +3898,9 @@
         <v>178</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7"/>
+      <c r="L7" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A8" s="8" t="s">
@@ -3811,7 +3930,9 @@
         <v>265</v>
       </c>
       <c r="K8" s="8"/>
-      <c r="L8"/>
+      <c r="L8" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A9" s="8" t="s">
@@ -3841,7 +3962,9 @@
       <c r="K9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L9"/>
+      <c r="L9" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A10" s="8" t="s">
@@ -3873,7 +3996,9 @@
         <v>238</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10"/>
+      <c r="L10" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="8" t="s">
@@ -3905,6 +4030,9 @@
         <v>181</v>
       </c>
       <c r="K11" s="8"/>
+      <c r="L11" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A12" s="8" t="s">
@@ -3936,7 +4064,9 @@
         <v>241</v>
       </c>
       <c r="K12" s="8"/>
-      <c r="L12"/>
+      <c r="L12" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="8" t="s">
@@ -3970,6 +4100,9 @@
       <c r="K13" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="L13" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A14" s="8" t="s">
@@ -4003,7 +4136,9 @@
       <c r="K14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L14"/>
+      <c r="L14" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="8" t="s">
@@ -4035,6 +4170,9 @@
         <v>266</v>
       </c>
       <c r="K15" s="8"/>
+      <c r="L15" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A16" s="8" t="s">
@@ -4066,37 +4204,41 @@
         <v>267</v>
       </c>
       <c r="K16" s="8"/>
-      <c r="L16"/>
+      <c r="L16" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A17" t="s">
-        <v>480</v>
+        <v>445</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>467</v>
+        <v>432</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>464</v>
+        <v>429</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="8" t="s">
-        <v>463</v>
+        <v>428</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>465</v>
+        <v>430</v>
       </c>
       <c r="K17" s="8"/>
-      <c r="L17"/>
+      <c r="L17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
@@ -4128,7 +4270,9 @@
         <v>201</v>
       </c>
       <c r="K18" s="8"/>
-      <c r="L18"/>
+      <c r="L18" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
@@ -4160,37 +4304,41 @@
         <v>208</v>
       </c>
       <c r="K19" s="8"/>
-      <c r="L19"/>
+      <c r="L19" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A20" t="s">
-        <v>481</v>
+        <v>446</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>466</v>
+        <v>431</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>468</v>
+        <v>433</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="8" t="s">
-        <v>463</v>
+        <v>428</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="8" t="s">
         <v>214</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>469</v>
+        <v>434</v>
       </c>
       <c r="K20" s="8"/>
-      <c r="L20"/>
+      <c r="L20" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A21" s="8" t="s">
@@ -4222,7 +4370,9 @@
         <v>268</v>
       </c>
       <c r="K21" s="8"/>
-      <c r="L21"/>
+      <c r="L21" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A22" s="8" t="s">
@@ -4252,7 +4402,9 @@
         <v>29</v>
       </c>
       <c r="K22" s="8"/>
-      <c r="L22"/>
+      <c r="L22" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="30">
       <c r="A23" s="8" t="s">
@@ -4282,6 +4434,9 @@
         <v>178</v>
       </c>
       <c r="K23" s="8"/>
+      <c r="L23" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="24" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A24" s="8" t="s">
@@ -4313,7 +4468,9 @@
         <v>25</v>
       </c>
       <c r="K24" s="8"/>
-      <c r="L24"/>
+      <c r="L24" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="A25" s="8" t="s">
@@ -4345,6 +4502,9 @@
         <v>25</v>
       </c>
       <c r="K25" s="8"/>
+      <c r="L25" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="45">
       <c r="A26" s="8" t="s">
@@ -4376,6 +4536,9 @@
         <v>25</v>
       </c>
       <c r="K26" s="8"/>
+      <c r="L26" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="30">
       <c r="A27" s="8" t="s">
@@ -4405,6 +4568,9 @@
         <v>182</v>
       </c>
       <c r="K27" s="8"/>
+      <c r="L27" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="30">
       <c r="A28" s="8" t="s">
@@ -4434,6 +4600,9 @@
         <v>183</v>
       </c>
       <c r="K28" s="8"/>
+      <c r="L28" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="30">
       <c r="A29" s="8" t="s">
@@ -4455,12 +4624,15 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8" t="s">
-        <v>449</v>
+        <v>414</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>280</v>
       </c>
       <c r="K29" s="8"/>
+      <c r="L29" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="30">
       <c r="A30" s="8" t="s">
@@ -4488,6 +4660,9 @@
         <v>279</v>
       </c>
       <c r="K30" s="8"/>
+      <c r="L30" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="45">
       <c r="A31" s="8" t="s">
@@ -4517,6 +4692,9 @@
         <v>269</v>
       </c>
       <c r="K31" s="8"/>
+      <c r="L31" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="45">
       <c r="A32" s="8" t="s">
@@ -4546,6 +4724,9 @@
         <v>270</v>
       </c>
       <c r="K32" s="8"/>
+      <c r="L32" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="30">
       <c r="A33" s="8" t="s">
@@ -4577,6 +4758,9 @@
         <v>204</v>
       </c>
       <c r="K33" s="8"/>
+      <c r="L33" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="30">
       <c r="A34" s="8" t="s">
@@ -4608,6 +4792,9 @@
         <v>203</v>
       </c>
       <c r="K34" s="8"/>
+      <c r="L34" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="45">
       <c r="A35" s="8" t="s">
@@ -4637,6 +4824,9 @@
         <v>11</v>
       </c>
       <c r="K35" s="8"/>
+      <c r="L35" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="45">
       <c r="A36" s="8" t="s">
@@ -4668,6 +4858,9 @@
         <v>361</v>
       </c>
       <c r="K36" s="8"/>
+      <c r="L36" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="30">
       <c r="A37" s="8" t="s">
@@ -4699,6 +4892,9 @@
         <v>306</v>
       </c>
       <c r="K37" s="8"/>
+      <c r="L37" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="30">
       <c r="A38" s="8" t="s">
@@ -4730,6 +4926,9 @@
         <v>308</v>
       </c>
       <c r="K38" s="8"/>
+      <c r="L38" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="8" t="s">
@@ -4759,6 +4958,9 @@
         <v>310</v>
       </c>
       <c r="K39" s="8"/>
+      <c r="L39" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="30">
       <c r="A40" s="8" t="s">
@@ -4788,6 +4990,9 @@
         <v>246</v>
       </c>
       <c r="K40" s="8"/>
+      <c r="L40" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" t="s">
@@ -4805,14 +5010,20 @@
       <c r="E41" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="F41"/>
       <c r="G41" t="s">
         <v>250</v>
       </c>
+      <c r="H41"/>
       <c r="I41" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>251</v>
+      </c>
+      <c r="K41"/>
+      <c r="L41" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30">
@@ -4842,6 +5053,10 @@
       <c r="J42" s="5" t="s">
         <v>254</v>
       </c>
+      <c r="K42"/>
+      <c r="L42" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" t="s">
@@ -4871,6 +5086,10 @@
       </c>
       <c r="J43" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="K43"/>
+      <c r="L43" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30">
@@ -4900,6 +5119,10 @@
       <c r="J44" s="5" t="s">
         <v>260</v>
       </c>
+      <c r="K44"/>
+      <c r="L44" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="30">
       <c r="A45" t="s">
@@ -4930,6 +5153,10 @@
       <c r="J45" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="K45"/>
+      <c r="L45" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="45">
       <c r="A46" t="s">
@@ -4960,6 +5187,10 @@
       <c r="J46" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="K46"/>
+      <c r="L46" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="47" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A47" s="8" t="s">
@@ -4993,7 +5224,9 @@
       <c r="K47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L47"/>
+      <c r="L47" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="48" spans="1:12" ht="30">
       <c r="A48" s="8" t="s">
@@ -5025,6 +5258,9 @@
         <v>365</v>
       </c>
       <c r="K48" s="8"/>
+      <c r="L48" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="49" spans="1:11" ht="30">
       <c r="A49" t="s">
@@ -5055,6 +5291,10 @@
       <c r="J49" s="5" t="s">
         <v>368</v>
       </c>
+      <c r="K49"/>
+      <c r="L49" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="50" spans="1:11" ht="30">
       <c r="A50" t="s">
@@ -5085,6 +5325,9 @@
       </c>
       <c r="K50" s="3" t="s">
         <v>38</v>
+      </c>
+      <c r="L50" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -5115,6 +5358,9 @@
         <v>378</v>
       </c>
       <c r="K51" s="8"/>
+      <c r="L51" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="52" spans="1:11" ht="60">
       <c r="A52" t="s">
@@ -5147,6 +5393,9 @@
       </c>
       <c r="K52" s="3" t="s">
         <v>38</v>
+      </c>
+      <c r="L52" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -5177,13 +5426,16 @@
         <v>383</v>
       </c>
       <c r="K53" s="8"/>
+      <c r="L53" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="54" spans="1:11" ht="75">
       <c r="A54" t="s">
-        <v>482</v>
+        <v>447</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>455</v>
+        <v>420</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>14</v>
@@ -5199,30 +5451,33 @@
       </c>
       <c r="G54" s="8"/>
       <c r="H54" s="19" t="s">
-        <v>471</v>
+        <v>436</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>315</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>474</v>
+        <v>439</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="L54" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="55" spans="1:11" ht="75">
       <c r="A55" t="s">
-        <v>489</v>
+        <v>454</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>456</v>
+        <v>421</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>483</v>
+        <v>448</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>16</v>
@@ -5230,22 +5485,27 @@
       <c r="F55" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="G55"/>
       <c r="H55" s="19" t="s">
-        <v>476</v>
+        <v>441</v>
       </c>
       <c r="I55" t="s">
-        <v>482</v>
+        <v>447</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>477</v>
+        <v>442</v>
+      </c>
+      <c r="K55"/>
+      <c r="L55" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="45">
       <c r="A56" t="s">
-        <v>490</v>
+        <v>455</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>457</v>
+        <v>422</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>14</v>
@@ -5261,30 +5521,33 @@
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="5" t="s">
-        <v>484</v>
+        <v>449</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>485</v>
+        <v>450</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>486</v>
+        <v>451</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="L56" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="57" spans="1:11" ht="60">
       <c r="A57" t="s">
-        <v>491</v>
+        <v>456</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>458</v>
+        <v>423</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>495</v>
+        <v>460</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>16</v>
@@ -5294,18 +5557,22 @@
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="19" t="s">
-        <v>487</v>
+        <v>452</v>
       </c>
       <c r="I57" t="s">
-        <v>496</v>
+        <v>461</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>497</v>
+        <v>462</v>
+      </c>
+      <c r="K57"/>
+      <c r="L57" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="45">
       <c r="A58" s="8" t="s">
-        <v>444</v>
+        <v>410</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>75</v>
@@ -5314,7 +5581,7 @@
         <v>14</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>495</v>
+        <v>460</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>19</v>
@@ -5325,15 +5592,19 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
       <c r="I58" t="s">
-        <v>490</v>
+        <v>455</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>498</v>
+        <v>463</v>
+      </c>
+      <c r="K58"/>
+      <c r="L58" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="30">
       <c r="A59" s="8" t="s">
-        <v>459</v>
+        <v>424</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>303</v>
@@ -5342,7 +5613,7 @@
         <v>14</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>483</v>
+        <v>448</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>19</v>
@@ -5353,18 +5624,22 @@
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" t="s">
-        <v>482</v>
+        <v>447</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>488</v>
+        <v>453</v>
+      </c>
+      <c r="K59"/>
+      <c r="L59" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="210">
       <c r="A60" t="s">
-        <v>492</v>
+        <v>457</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>470</v>
+        <v>435</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>14</v>
@@ -5380,21 +5655,24 @@
       </c>
       <c r="G60" s="8"/>
       <c r="H60" s="19" t="s">
-        <v>478</v>
+        <v>443</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>459</v>
+        <v>424</v>
       </c>
       <c r="J60" s="19" t="s">
-        <v>479</v>
+        <v>444</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="L60" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="61" spans="1:11" ht="30">
       <c r="A61" s="8" t="s">
-        <v>461</v>
+        <v>426</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>303</v>
@@ -5403,7 +5681,7 @@
         <v>14</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>493</v>
+        <v>458</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>19</v>
@@ -5414,10 +5692,14 @@
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
       <c r="I61" t="s">
-        <v>492</v>
+        <v>457</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>494</v>
+        <v>459</v>
+      </c>
+      <c r="K61"/>
+      <c r="L61" t="s">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -5429,23 +5711,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="I21" workbookViewId="0">
-      <selection activeCell="L26" sqref="L2:L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="98.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="80.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="98.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -5491,7 +5773,7 @@
         <v>337</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>434</v>
+        <v>401</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
@@ -5505,11 +5787,17 @@
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
       <c r="J2" s="5" t="s">
-        <v>435</v>
+        <v>402</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
@@ -5531,19 +5819,24 @@
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G3"/>
       <c r="H3" s="1" t="s">
         <v>284</v>
       </c>
+      <c r="I3"/>
       <c r="J3" s="5" t="s">
         <v>311</v>
       </c>
       <c r="K3" t="s">
         <v>38</v>
       </c>
+      <c r="L3" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>450</v>
+        <v>415</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>316</v>
@@ -5560,14 +5853,19 @@
       <c r="F4" s="5" t="s">
         <v>359</v>
       </c>
+      <c r="G4"/>
       <c r="H4" s="1" t="s">
-        <v>451</v>
-      </c>
+        <v>416</v>
+      </c>
+      <c r="I4"/>
       <c r="J4" s="5" t="s">
-        <v>452</v>
+        <v>417</v>
       </c>
       <c r="K4" t="s">
         <v>38</v>
+      </c>
+      <c r="L4" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45">
@@ -5589,11 +5887,17 @@
       <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G5"/>
       <c r="H5" s="1" t="s">
         <v>285</v>
       </c>
+      <c r="I5"/>
       <c r="J5" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="75">
@@ -5615,14 +5919,19 @@
       <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="G6"/>
       <c r="H6" s="1" t="s">
         <v>391</v>
       </c>
+      <c r="I6"/>
       <c r="J6" s="5" t="s">
         <v>294</v>
       </c>
       <c r="K6" t="s">
         <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
@@ -5641,11 +5950,18 @@
       <c r="E7" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
       <c r="I7" t="s">
         <v>317</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>319</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="75">
@@ -5653,7 +5969,7 @@
         <v>335</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>454</v>
+        <v>419</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
@@ -5667,17 +5983,21 @@
       <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="G8"/>
       <c r="H8" s="14" t="s">
         <v>331</v>
       </c>
       <c r="I8" t="s">
-        <v>475</v>
+        <v>440</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>312</v>
       </c>
       <c r="K8" t="s">
         <v>38</v>
+      </c>
+      <c r="L8" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
@@ -5699,6 +6019,7 @@
       <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G9"/>
       <c r="H9" s="1" t="s">
         <v>289</v>
       </c>
@@ -5708,13 +6029,17 @@
       <c r="J9" s="5" t="s">
         <v>320</v>
       </c>
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>436</v>
+        <v>403</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>434</v>
+        <v>401</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
@@ -5728,11 +6053,17 @@
       <c r="F10" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="G10"/>
+      <c r="H10"/>
       <c r="I10" t="s">
-        <v>437</v>
+        <v>404</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>438</v>
+        <v>405</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
@@ -5754,11 +6085,17 @@
       <c r="F11" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="G11"/>
+      <c r="H11"/>
       <c r="I11" t="s">
-        <v>437</v>
+        <v>404</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>439</v>
+        <v>406</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
@@ -5777,14 +6114,20 @@
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="F12"/>
       <c r="G12" t="s">
         <v>321</v>
       </c>
+      <c r="H12"/>
       <c r="I12" t="s">
         <v>317</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>322</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
@@ -5806,6 +6149,7 @@
       <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G13"/>
       <c r="H13" s="1" t="s">
         <v>323</v>
       </c>
@@ -5817,6 +6161,9 @@
       </c>
       <c r="K13" t="s">
         <v>38</v>
+      </c>
+      <c r="L13" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
@@ -5835,11 +6182,18 @@
       <c r="E14" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
       <c r="I14" t="s">
         <v>340</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>325</v>
+      </c>
+      <c r="K14"/>
+      <c r="L14" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
@@ -5853,7 +6207,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>453</v>
+        <v>418</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>19</v>
@@ -5861,11 +6215,17 @@
       <c r="F15" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="G15"/>
+      <c r="H15"/>
       <c r="I15" t="s">
-        <v>450</v>
+        <v>415</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
@@ -5879,7 +6239,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>453</v>
+        <v>418</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>19</v>
@@ -5887,11 +6247,17 @@
       <c r="F16" s="5" t="s">
         <v>377</v>
       </c>
+      <c r="G16"/>
+      <c r="H16"/>
       <c r="I16" t="s">
-        <v>450</v>
+        <v>415</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
@@ -5913,11 +6279,17 @@
       <c r="F17" s="5" t="s">
         <v>295</v>
       </c>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="I17" t="s">
         <v>330</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="K17"/>
+      <c r="L17" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="45">
@@ -5939,6 +6311,7 @@
       <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="G18"/>
       <c r="H18" s="1" t="s">
         <v>341</v>
       </c>
@@ -5951,10 +6324,13 @@
       <c r="K18" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="L18" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="45">
       <c r="A19" s="8" t="s">
-        <v>446</v>
+        <v>412</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>75</v>
@@ -5980,6 +6356,9 @@
         <v>11</v>
       </c>
       <c r="K19" s="8"/>
+      <c r="L19" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="A20" t="s">
@@ -6000,6 +6379,7 @@
       <c r="F20" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="G20"/>
       <c r="H20" s="14" t="s">
         <v>342</v>
       </c>
@@ -6011,6 +6391,9 @@
       </c>
       <c r="K20" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="L20" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30">
@@ -6043,6 +6426,9 @@
         <v>343</v>
       </c>
       <c r="K21" s="8"/>
+      <c r="L21" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" t="s">
@@ -6073,6 +6459,10 @@
       <c r="J22" s="5" t="s">
         <v>345</v>
       </c>
+      <c r="K22"/>
+      <c r="L22" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" t="s">
@@ -6093,8 +6483,15 @@
       <c r="F23" s="5" t="s">
         <v>295</v>
       </c>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
       <c r="J23" s="5" t="s">
         <v>388</v>
+      </c>
+      <c r="K23"/>
+      <c r="L23" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="45">
@@ -6116,13 +6513,20 @@
       <c r="F24" s="5" t="s">
         <v>295</v>
       </c>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
       <c r="J24" s="5" t="s">
         <v>388</v>
       </c>
+      <c r="K24"/>
+      <c r="L24" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="45">
       <c r="A25" s="8" t="s">
-        <v>460</v>
+        <v>425</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>75</v>
@@ -6131,7 +6535,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>447</v>
+        <v>413</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>19</v>
@@ -6148,10 +6552,13 @@
         <v>11</v>
       </c>
       <c r="K25" s="8"/>
+      <c r="L25" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" s="8" t="s">
-        <v>473</v>
+        <v>438</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>303</v>
@@ -6160,7 +6567,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>462</v>
+        <v>427</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>19</v>
@@ -6174,7 +6581,11 @@
         <v>335</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>472</v>
+        <v>437</v>
+      </c>
+      <c r="K26"/>
+      <c r="L26" t="s">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for Authoring image/media, video related tags support
</commit_message>
<xml_diff>
--- a/src/test/test-data/AuthoringTestData.xlsx
+++ b/src/test/test-data/AuthoringTestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Authoring-wos and patents" sheetId="1" r:id="rId1"/>
     <sheet name="Authoring-Posts" sheetId="2" r:id="rId2"/>
     <sheet name="Authoring-Drafts" sheetId="3" r:id="rId3"/>
+    <sheet name="Authoring-Img-Video" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="542">
   <si>
     <t>GET</t>
   </si>
@@ -1515,17 +1516,139 @@
     <t>hits[0].id||hits[1].id</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>{ "title":"Test Post with invalid img src and invalid iframe src", "content":"Testing of image with invalid src &lt;img class=\"fr-dib fr-draggable\" src=\"http://www.enr.com/ext/resources/images/articles/HOV_DirectConnect_900.jpg\" style=\"width: 300px;\" alt=\"Test third party photo in post\" width=\"200\" height=\"200\"&gt; &lt;/img&gt; &lt;/br&gt; Testing iframe with invalid src: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"http://yahoo.com/foo\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; &lt;/br&gt; Make sure above img, iframe are stripped out as those are invalid content." }</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a post with invalid image src, invalid iframe src and check the invalid content is stripped out from the post and pusblished using API.</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a post image using authoring media API.</t>
+  </si>
+  <si>
+    <t>/authoring-media/cud</t>
+  </si>
+  <si>
+    <t>mediaId</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a post with valid youtube links and invalid youtube urls are stripped out from the post and pusblished using API.</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||title=Test Post with invalid img src and invalid iframe src||content=Testing of image with invalid src  Testing iframe with invalid src:  Make sure above img, iframe are stripped out as those are invalid content.||wasCleanedUp=2||wasTruncated=false||found=true||coverImageId=""</t>
+  </si>
+  <si>
+    <t>OPQA-1076_6</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a post with valid media id for image src and post is pusblished using API.</t>
+  </si>
+  <si>
+    <t>Verify that user able to create a draft post with valid image media id using API</t>
+  </si>
+  <si>
+    <t>{"content":"Draft Post test with image with valid media ID &lt;img class=\"fr-dib fr-draggable\" src=\"/api/media/1723214b-30dc-42a5-aa1c-a3e911f6b71c\" style=\"width: 300px;\" alt=\"Editor photo\" width=\"200\" height=\"200\"&gt; &lt;/img&gt; ", "title":"Draft Post with image", "topics":[]}</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||title=Draft Post with image||content=""||found=true||coverImageId=1723214b-30dc-42a5-aa1c-a3e911f6b71c</t>
+  </si>
+  <si>
+    <t>OPQA-1090_1</t>
+  </si>
+  <si>
+    <t>Verify that user is able to edit existing post with valid media id for image src and valid youtube urls for videos working as expected using API.</t>
+  </si>
+  <si>
+    <t>OPQA-1076_7</t>
+  </si>
+  <si>
+    <t>OPQA-1076_8</t>
+  </si>
+  <si>
+    <t>Verify that user able to edit a draft post with valid image media id, youtube links using API</t>
+  </si>
+  <si>
+    <t>{"content":"Testing of image with valid media ID &lt;img class=\"fr-dib fr-draggable\" src=\"/api/media/1723214b-30dc-42a5-aa1c-a3e911f6b71c\" style=\"width: 300px;\" alt=\"Post with valid media image\" width=\"200\" height=\"200\"&gt; &lt;/img&gt; &lt;/br&gt; Valid youtube link: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"http://youtube.com/foo\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; &lt;/br&gt; Testing of vimeo with valid src: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"https://vimeo.com/172911816\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; &lt;/br&gt; &lt;/br&gt;&lt;/br&gt;Make sure above media image along with youtube/vimeo links will be visible from draft UI. ", "title":"Edit Draft Post with image, youtube links", "topics":[]}</t>
+  </si>
+  <si>
+    <t>{ "title":"Test Post with valid youtube/vimeo links", "content":"Testing of youtube with valid youtube link &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"http://youtube.com/foo\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; &lt;/br&gt; Testing of vimeo with valid src: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"https://vimeo.com/172911816\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; &lt;/br&gt; &lt;/br&gt;Testing of invalid link in iframe: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"http://yahoo.com/foo\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; &lt;/br&gt;&lt;/br&gt;Make sure above invalid youtube and vimeo links are stripped out as those are invalid content." }</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||title=Test Post with valid youtube/vimeo links||content=Testing of youtube with valid youtube link &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"http://youtube.com/foo\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; Testing of vimeo with valid src: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"https://vimeo.com/172911816\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; Testing of invalid link in iframe:  Make sure above invalid youtube and vimeo links are stripped out as those are invalid content.||wasCleanedUp=2||wasTruncated=false||found=true||coverImageId=""</t>
+  </si>
+  <si>
+    <t>OPQA-4772</t>
+  </si>
+  <si>
+    <t>OPQA-4773</t>
+  </si>
+  <si>
+    <t>{"targetType": "posts", "targetId": "(OPQA-4773_id)", "mediaType": "image/png", "mediaExt": "image/png", "mediaCategory": "posts", "mediaContent": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASsAAAErCAMAAACxelWGAAADAFBMVEX////Z2dmenp7AwMDNzc3Pz8/FxcWXl5exsbG5ubnW1tbT09Ourq6bm5ucnJzd3d2ampqWlpapqamZmZnh4eHJycmzs7OoqKi0tLTk4+SMjIyLior3+Pe1tbWwsLC2traVlZWUlJS7u7vDw8O3t7fKysqhoaGkpKS6urqvr6/ExMTb29vIyMjLy8va2tq9vb3CwsJ9fX3Hx8fR0dHQ0NDo6Oi8vLzU1NSJiYmSkpKTk5OQkJC+vr6RkZHX19erq6v//v+srKzBwcHr6+uPj4/9/P3c3NyCgYKfn5+mpqaNjY3i4uKgoKB8e3z///6lpaXt7e3f39/w8PCIh4d6enn5+vqGhobl5eX8/Pt1dXWDg4Pm5uaFhYV/f3/n5+dxcXH7//2EhITy8vKbl5Zsa2t+AAT19fX6+/p4d3iFAARDAQObmJrFAgZ1cnPLAQahl5ZkAgRwbm5qAANvAAPs7OygnZ+XlJRWAAJ1AAPx8fGdmZ2XmpqWmZaMAASMhomEe3yIgIReAQOimpqolpZYGBcfAQF/dXhgEBBoZWU2AQL29vZ+WFwPBQRPAQKQAASbn566tbh2aWrCvsHZAAa/uLyBYmSTlpZlNze5uL6aAATJwcHQAAa0ure+BQUpAAHUAAaojI63sbX/9/bYycy3vbmRi4y4vL7Rx8XeAAbnenxWMTOVjo/oo6TDMTFfJibXv8DkvsGjAAWqmZqUAASsoqVyTEvgtrVSQkTgYWHQyMy2BAWyq6+wlZbWTk03LSvkAQexubLKxMbjlpfRNjSnnp7SW1uxsbXbcHDFFRD1s7Pwj467FA69IR+tAAV7gn+UT0/BxMByWFb4oZ68vLNuQUDGu767wb3KIyCSgoPLQUC+s7a3paXiyM19ODrCvrr+2tmWn51fTUzGy8Z/b279zsypr6+GaGpvLjAhGxqrZmamd3aISEhCGhn/7+33vcGeXV7Nurr+4uLdrqr96OqxhobaiYhzGRiMGxrPGRTFgYGqKinc1Nfr7ezX19GtEw/16vJfHUokAABKXklEQVR42ux9228bZ5anSlUsVbEoUaJ4lUXSZvF+qzJv5UuZFEmbFk1ZIqXIVCxHkIWF1EALBhZQHpTeP2DhFxsdo2HEDoLYQWcMJIgfBkYuCOAk4ySOs8AgRjpow0iCRedhHhJ0T6OBmV7szv5OUZLt7umskXidpMWfRZPUhZffd875zvVjTxdddNFFF1100UUXXXTxk8LY4hwwOdnTxf+LqbFLly5NTnapeggcGpsb6+niocSqS9VDY3HsUJerh0SXqofH5KGeLh6SqsmuWD28b9X1FR5arha7cvXQWJzr6eIh5eqvuOrK2d/C2GQ3EHz4fXCuS9XDk7XSFayH5mrykOFjdQl7KLZ6Fhe7Zuuh0c1fddFFF1100UUXXXTRRRdddNFFF108HkxuZmMW5/BvBU1Yi4vdzMx/hq0a6mQH3QzWw6JLVBddbB+MPS51NwzL5NbNe/cen3X+m88zuQj8rZfw2F7eXz7n5Lf/fG7yfnwfd2Jz03x8K/GYQfK2SJijf5P3L/u3vN0x4ob+aG7u0KFDi3Mri9toA/0rubrv9iabs4v3AYZkcWxxsWds4+7D+Wk9fxf4VrWZW5mb7HDyQLva5CI6srr9a9+p1NxtdOiiiy666KKLLrrooosuuuiiiy5++hibm1uZNbCy0h31/xaaZmdHZ++B7q106frPMHv69OnRv8Lp0S5bf03VMuH0MjGGL1wIy8tLy7M9XdyHudml9aWlpfXlDcLAGN3At+i7092B4/swuj49vb6+vrQFg6cOf/jR9EpPF5titb7WXJ826JreYmy9c59QrXbJ2sBKswOwgouBdQLdMH5Q7ZK1gbHmQhVYWwMra5u0bfK0BlTza/l812YR1ufbC3mgeh+aHZ46d/CjhUa16zvAWfC05xfa8/kOwMz9vG18d77d9kx3yeqptjxtD/hqz88vLCzkFxbmAYOhhc5t/AQ/t88v92x3zLVa9lbDY6DdBmVt4xZRBBjfbtg9jVaj1dXC5ZrVam017PYNvjrsbFw1Gnb8wN6yg1CrZ7Rnm6ORqNVAFgBWGvgyCNq4bm3AamCtZ3tj2syk04mawUXrr2DdQA1IFBvb22+Ys2rFIsMw6QSJ1xY2bhNDhDRDv2JmTvdsZyybJU0zd+hKJzqogRyDO1ylGQPFolkratL2VsKqyZSVQJdGjDH3YYsj/AQXicB5erYz5lNcLittsgUUDeC6c0XflgymsqYsV+vZxpizpjjOlMsZfG1Spt27YZAE5HImU45LaT3bGCtMJgW2DL6yhA47G9wZ3wFLXAchB9ezjbFilpPJEOjahInQucFtIZVKhUIOR4ZP9WxjrGiVTNLhCIW4vwmDJkcymcnwcUfPNsacpMR5ns8QXakQIWWAo5sOA0QSIR5X2W3N1ZgUYNV4HGwlk44koUMQ3SaSOpBlWVUrrF7Y1lz1mEWFVVVZJuHCha4MbNwHi8QTC+iKLm5r296TFgM6iKjIJFxxgN8A3TPkSa0QT0A04N3WPkOPXRQLBUVnKxVV/guolQpoMogKAFFRFOw92xnNgjMQjQYKus4SwM496DrJUwE/Fw14he0dD47yFj9oiEK4FL1DmL4BsFQIdIgK+v1er7ssbu9k35hm8Xm9/iDoEiFfgYJSKIChjtIRS8EgaHIKguCLuRzbPIlsF0pOp9MrBg01ixowbnR4gkC5nU5fzBIrl22Nnu2N9ULE5xMEvxD0B4MGYRsk0cULzSORKhNTEfd2L+SMaTZX2Ve2eAU3mPF7SZIAp5sgGLpnKVtK5SlbmNv2zUVNd8Rms5QFH3hxOvFFxgn3CDGLxVKGSJVsoKpc7dnmGFvhxqfqpbKtHPNtIGbZQJlgs9nq9Xo4PJza5pYd0XNPsz4wBdEqlw16DIZKpVK5ZCO4XPV6JByZCO+0NXu6GDMNToTrEK1NbNJUB6amIuGJifGB4YHtHd9sYoXdOR6BHhrSBECYXERTBAiPg6iB/r4hx/auDW5hurwvHKnbSqWOSLk25CkcHh8YH+8f7O/rG1G2u7+wpYUL433hqbrNVtriKgLVG+8liRoc3rVvR3nbuwv3hgBa/f0dwSoRWaR/4fFeELVz1669B/bPCNM9XWzuhT2tifGpkrEVEl0Qq4mBgcG+vqF9B0f2zIjbuzb/Fz7WXE+6bvMJHT+9XHJNRcb7h4f27d8zMvLUAbmrgA/MK/XMhYJGrkr0O4VYqR4ZH+zbd2TPid3HvJ5t74M+cKzU3OhoPosioSMuV5Qoknrl+sTwvj1PHd9hY7q+wn1YWa82EhrHoZ1B4lIOHrWtgCjYhkd2lbi17mfg3m+qmvYaA5a0GpNmihKVm0NJXtXd9QL1PM7NjXW5MjDaXPA0qPmxZUVrH1rSzJqEBgYqNqsBbRaGbGVutjsxYVBVNZq00RiK5llwhX4rkCUZLSCcypryKz1jXXNFWFnLL2z2+TcgWTXq4itqm91EphDPW5e61oowZ3T7UxN7w05KaDVaQxmjQY1a1aCNppQpsU089m8VidP5NuYiqNm/0Wk4rtU2u2iLANOBxGnfJll/BwqKKVNMteGC+dKxueXljbf0wPZf9XjmiagGiVSHqbTB1QboTgL/o6eWRKuzI87hvxUMjGPE/u+AJqJkuVnNz3ta1jRjtTJMzWpvr8/ONpvLmJHfeofLjYansaF66EDu0JTe4Gqzh7tG8oZvLZxeGV0+De7XMMu0hlE5Y8zw9MrsT9uYjc0uV1tMltOYhNXTyBvDk83l5emFVsuzkK9On541Tl1Yarc8DTLnTNGwTpsMETo3jfEAY5SC5A6skhjaQV7LqmWZRNrarjanf8Ix9cpy3uOxSiFOS1hJJFqeahME0YhbE7PLp5eb840qTYCP5lsAJMrccRA0rUgwyNogrcOVx9Oye9qNdKI9vbRsTPUuNZt5j5XRshxXxFr8NE8kWJnOL3isGhfKpa0Jc5bLFWuaZvVY01a7Z6Gax4Bgc3l2dCnfbjeX84aZAlXZTl8t2DKbDa42dZBUEBcSLDL+1gYeAXLVaC9UsQiMtUV0mbiafb7502tymG63ijn09WtMOmeCe8SYYYqsrTaJlaedx2igpwXO1k8vzTfmPbTz1Rgth3CGR69oTqKG/01NLNJYQHpTuuhX7bWap+OyNhoYSkkU8SdazZqWsDIJT37pp2Hox4xwbanZSEupUNaskaQ4ONgTz9r0NPQG51Isj44uL615Opivri9VWzTjliA9yqisyjuILGljcKKIL+MWzQPgesNywfoZs7x5TwP3ILH4fdDFmHNcVqrZ88s/el0EUbNNT6tWlECQhP9TPM8VYabW4C40m53jKbDHz87NzeIbC7Q72ufzC62ODnFJVgzq8SRJVtZgy/BDtY2xkg1oZobBLuBZhsewsoIHO42H8oBqzhHiTBoC7qRDSrfm107/qD8pfmVpPoGVTfJJTspxGVxliy0KXDzwF2BtPDBhnjZ2+iqEa3b29FIVxhq7Gi4JMBtS3bZyVCWuTCBrM7wxQDF0p2M7BX2DdLWqS8vTa9hW1xbymBvHlacmcckUl5LM2ZSDg/K3qj/amGi2WSPRKOiZXNYhq/EMx2DI254wTLMVsmMna1WtEmELCJPX1k+PLk9jYNegCsYqXogM2EQ1E+oY+E2SsnQhotCvzatoJXXkJDMesdEZ7bWTUpqtCwvVtYUafi2Jn2sSViokFYu16o8v4Tw2u9RM57h41K9kkpk4W0ly2PQaNU3KZWGXE/a83ePJrxknLcDOzHsw3g0i89OwXOQtpPHueMW390A9IGccqc0pE1wwU4JrkqgkH68g7RctqBBbmMAWZSXytCsmrLBiaabWggQnjHVyIPGVUXSHSUpXp39cPupstSY5WNEfkJHGVBQ5JaXt2JYMs2O20n63vETHfc31kImZha/QXABZ89gL4R2BKkbKOVRvGEliJZ5xhDbnS3KG4tEllOFlVg/40THjFNmMCWqYnl9eXociVucX5ls1hqF1kciTY3IZWUXbd5IvBKM8p9XyPx7hmvVoIVZ0e1meV6Lo8ExqcAByKS5rMplbeeMginzDk8+3Ggtr0+s4fGiUzPJydYHeZMtO0Y+WhVjZ9u8+EmOJqxT42YKhfhmkkgui02exuUqCWAnltHTCszy2QsetYV+dXoNNpKQzB5GzelpaRq0Ynd9sNMDypmJty6X/wfKqKys4/GzBxLOBqD9QEdHgqXKSlmBMnClLr7oNdbOaNQZGywozTk4CeZAwW82l0ZXZ9bwRpmCrx8apCr0nj/b52TiGJVJ/OYOTjFdAld9nq09M1G1CIM5lDeNdtaetCx57uwr1BvdWhkoayRxjbTBJdDMXomxccQoBnjPVmiudXMcPcjTbGL5mmwmO9ZfLQpQVBX8gHsqZ0xLtg9jGauQ2ppHZBFd0bEB+Pj/fgBtqp8MqFhqe6tLo6SXaB2GsTKl4dGpw5PiEWOEdSUfowaGuJCmgIvpRzxkf7O+NlNxKhtNg0z1tOsvBWmRaNcnc2liZbAi7cK6Y0FDXUKKVuKwLPjGezCWac1RO+wG2xjHYnvWGxIs+i88tKgFfTORTkuRQ1TjvIEWgyEaCf0RBDXnrTdrgpxEFrk8316rgCC4QzoWhMFDLpTK6ZXBi6IhNkeOZDMi6Bwzj8EQVbJWtPrD3yIGdA5GynyUHLm2dR5ZhDceBIJrC6hTxrNgpIFwpR8YhaWmJZ6Nut4hub0FwBzJaY/2HoApY9uTivDPmF4POmM8blblsKM6yEIE4nBuSFbjfyMAQKyCu5UlABJAebs9DoEaXq22kYaCC2L9oD1SDkZ3lXTsFnY/T4JIxrrR54VEm1AOi0+LqPXDsqZm9w2GXj54OyYs2zneir3y70Uoj5JZM2CGx/eZQW+QrcZNZC6miL+YtsMFy3QJdtC79EFyNMWqFZ91Ov1AqOwsyl2KjMO6sznMSHHZO4ii9wJixOdnXp6stGFwwY8fCJ8Bbm5z4ZttIq1OOQFWEwT7vgWGvnuQzxNUWkqSAKguuhHJkaO/Q8d0ju/rDNqeCDc7MWCGXYIkSY3h4a61Ixh2iXDQhZOBVhU2apFDU6Q/CQIg+m1CIc40fIHMzTSN8ogWdPz6vgkWE54MrHsKUYtVUlmJfLYcXzqWsVSjfQq0IOWDsDaZGkmZPWBeaaw1k84pSLpRR3fWDMfEImSuDK3yFDJ46Q5VwFxSsyUBfPB88emL/0EDEIrJJCBZigXTLDtXTYCGlYq1Gz5mFRGvZFK+yFbWiqyEuxLqFctktijGB5VXusZN1OlTh49ESuvJFlo16MRniFyvJXC7JRqNy1mwm4SKPkguZEhQQLsEPYrREGrLQYvDmjJNQrCR4JvjYimXwiBo8OBVQwZUhVaFNrkiw4hgW9KL2XGoutQaOjhwYnqgLCk8SBKNYZLIm8iqy4AuyjG1XSqqqA6sEgZThvSq8I6O4bXUbLGtB5lW+OdbzOGPF0WwlkwmUbD5vQPF6g36nn02GeJaQyeJVxvksgjNTKJXTTClzul3Frg62Wgz8IkpsWtPYxHCPzBqCG299f3+yvresqNC/0MYo6pYa8hARyJVtSEWmTxo5fGDfcMSGJwRZDDivaRw5rSEOOyBpvwa2WFFnZU6CckeD0YAoVrCPCmhidqpxOVNJzD0uqsZ6xtZg1mVsTX4xILoFtz/AykabRkEla8UjTsFL4nLkZplSOqs6cmk4o2trHmTNGyAqXTTX7NailCXnideD5f4ZIRQeEnT8JbjacBZSncldEqyKLjptA0otbW95nxrZPzQxBfOOQKqYJvdMM5tMSDTgCeGuILPDS+YUq6hYMS6lBkQ/xgiCOivGYvWpKB5M0ZuPySWFj1J1IIagJfOimSwmkl0oBL0iy0kpuZJM8XLSIcdDJi7JmTJJs+yql91sKkH5JhIsxDQJBiEzw3WGvFVRiBw4kOT7B90sn6FMQgdbjEGy1ErAXw4X8g2EQ30nj+zs6y279XiK9kLso5oZbkcKyxLKmaBjGVw4LevQA1HsNw5ewUCP4AsWAui4ibEO7EDcY+o3HTuUT8k8Xn3Q5xR8FkFUZT0YDCh4VaQrlQofSqqVOJdK4k2mkDzOinXYF1byIN6Zh1AVYbNqrQQyC3yFxkwDQn1wpm7mh8f9bKZzQIPJhJj5Ab9dZqOxCR1UF62Fk3v29/XXsUYQXaOdJsdpIB6/iFtyBbP4chLrACOfUSD62HJ0yBZerDMadUdpmXXm/2+IuPFRfLOH/oNjsQey7pLFa/EXWFZ0uqMsdJLCEAQWmO5WCqocyphgL6QEPNGFdtZtK2ievFH9QsBTa8y3zJyDr5Boun313v17WFNyMCyqSYexIyARg+yCAYO0VJKvFJxhbxphtpUZPDyya7jX5i7EYaPIcyiaNI3DytDaGBadnDJF4UP4DhvEi2LjcbFcxuiK162omHFVKolHnWienLzn5q6Mrsxd+sMXX/zxPy6fwyByxV+yxWDU/YLgxQLzsFvegi4W2EoBr8YYWZYY8LSG3DrqCIlKIAH7XqVCfJ4SomZTMo49ymsp28L9+2bqXEgcrAeQFDXyfA8ApCHIg1Wr+8wtlO1bhZmZkb6BKR+eF5JkKlbXcFadPZ0NQayMfARUmVV0BRObeBkZXvRGRUVmgz4oAvQAi8myjsYoPjDwEZqtyUtzh/Boi4vGZzxe+sONWx//+V+uPff558/J3kjdJwYtdVvZG4+T1yB6YwgnYN4DekXReQ2+IWWGaWMym1Oclka+AVwZJ4fm7ZophO08CLdnaqDvyLEB/J7Qj4QMxGrz7J17ILo4hxwo+bRWOo2I3DezY39fuCTAxXCEklxrPl81+kbsTKbCwyeWVWP+F9ufCieWTfGw7k5RL7gxb2eJKRVe1pVQcwU4tIK3tjL6KD4/cXLy0soYuFqkm3/85MNnT736yWu3n3uuInohzhZIdVDXoxhgQ1YpKLhFFUOkIlx3xoMSVsrEIYUJA19stRueJlFFUkUlHMbk4A2q6gP9QzuO98vFHOcfsLCUE+0wVTQb0Kj6RZ0fSE1XfDa+Zm0jM1wb2XFkH4WFSgW6L+fI80DwSalSq5mrBBRorK6whSgCoyDyj7DmQXfMVhaR1omEfawcr0Tj/+uPXwOHDl26tPJojNfc7Oih2dlFg/cvPrvwwq0rN3//+XP6bwJ+Xxk66I0GMBAJwYYm+gs4XCGoJCkDIHEmbNc5BwxztoWKMAoTCJmJqrYHgS4Dv6JiUBXu33t8j5Ay8Y6cO+xTHZQ8pprERjGVMf5jjKY1jg+Ulfzy+vpa22o5PrO3r7fug+9UCCipooQMe87Bk3202uGLssYIeSHqxBoGBCEoQiPFGLI5ftFrq4tsXC788o271/70p3ff/eLSo+kVHDs0S0WEWeMjLic/+PDZN29885r+3KfnLn4VifhEOHkQLbfTi9E+IYBlrGQ4KV3TEOTzcHKoiFNrry0vGQcbr0P7iCo7dkKNy8hwmMpT4307ju91UzKPDTnrTjlkokJNh6YHCvVFDdum7vO2mtBCrcj1nRzZNRimvm7oPW9KwaXDg0DhUw4pm8DGwZMGyjCifq9g7NYFyBm80ZIbw5tKBQ7PG5ev/vufP/7zn75+NB/2emiRuFrsqOMnty6svvrK3V9++um5819FXEI0KAilKVsJkZYT+zHCnAwyuyZZVkTeUeErSUlCJLhunGNsKGAVTDWM1F4uFSeq6r0798zU+VQolZHjSWfdD5+MqLqfp4SBdAJscbJY5uGUoyhrlnedHNk3jHmwssUZVI0jnqDyyPUjdYwvDYkz5GoDAV0PCoAzBhPh90cLSBdCHcAbe/7TN+7e/O3qqc/+2PNIcIg+42EjdPrm1dVTH1+5++mnt2//8uz773udMWfZVi/HBLcbUuUURF5isnyUzHsUoaJDSlC5C6HNGqEKpvIGVWlqo0qqUW+s3rv32C4HY7xROD1uW1BOmaiX4T6Jwml9VJ9PJ4zcqW7RzVbqDbF6uCO7dxzcOdwbsfn8isnetlODjWRKVioynypEUSNkoJmKHxlbrGNUgHEt2wQ4pW5LuF4WlYJyPpm6++8fXli90vMoMAaqVjZuf/H66gvP37j52ue3b790/v2YDRtgrF7HlQ9T2z5fgdO0kA7bhQ2RNBHvjGnMo2th6xjjBaOxhbpAEdjAOSxHBkZGwhlPm8nxFR5ZL8EmxlM5cPWA9nXaPhI1o9tB9kaloomxzuen14LHj56YObhrMFL2BjImo2WE4p2sQ2XlgFjwBwsZLZ3lA4LP78ZSwrvC5G/ZBy/HAkUMIL/869T/vvb286uf/a7nEWBs7NDpjd300kerz56CBoKq31z86swZTKm5SpjiLuHpBa/OZ+BXu30CZt7ZEPZ8M4oDRRQHPQsbJxnPG2fzdroWEPsg9WbrnxmsZHMppm0NyXFVL8TKUZ5cS4OlTaoM/QNTRkowxIsxjpKsbVjwYnn37pmTR4bGXU4xnpNyJgeVJKUsLROCcRHwsxSdsjDw8AF90AKXyxbD68U3UDp76SU2dffdV0/dev3SIzBY91y1yZvvXXj2ww+++f2dO+fi70e+/LJehqmylS11yHMcWzKSV7pc8BYyCE9CFZaHgKCno0FVQOO4Z6RAO41mGvxKpFjc9aGDZUki9csmGIdeqLAQTp77C7m6J1tMEX/JRwUt7ykiSGohDTrx5O4TM/sHw2W/bMJ+m6XEjK6nzAwqz0j/i7rX4g6kEEv7Bb/PjVUt2cCVzYYRshjcwNsvFUx3b95YPXXrZs8jwNZe+ofXn/+H1bdv3j33+Z1P7/zjM1/W6z7BZimBLS9bYZ0+Y+o9wCdNJhWOAyGu0aHFKEpsnPfcor5G6u7nkLopuCN9w4rHw0iUSOCKEo9QySeAq03bvrkVbvZhMeRiheIBgU8wkB3sdOY0F/7Z7uN7dg64nKxJonwFYhrsDkmodE4yyaLo9tM5GDqWMirGXMYsIphy2aZ6e0tR/Tei/7nL33z03uqbN75+BIK15Tp89Pyzq6++ezV+/qXb50pPnznzj676VN2CDUVX3HBIUbJDyOUIUeoErgw8m4pDaxmdeA0q4bRw23i7WY4Cu6gv3F/iGHMLGawMl01mNCleKAjgKsV1eq/ghN4P3EMbMgWQbr+WQE4PxiudbqVmjh6fOTgU8QUcGqQug3BGV3kWxVwVxTeNY1kl6Bf9WEUVjmw9AgWsu0o+mys8OO7DaUhnb8NvuHHrwpuf9Dw6fPPehRf+7YOrl8+eFQu+Z56JhF1T4YhQiMIhnXKRTIk8UrZi0Bso0DrKlFrJpq1GVg9dUrhKmA2Fw49Er6/eH1bStTQKL+QJoaYfknIq60UdDxFd9sGWjw5yndozYjohZJZg1bLoVWC44d27T+7YP1DGHlxL57AMFNtExQBbCTqDesaB1Bi8KXhVZeScyUZ2znewRQYG6ljTXwf/+eW7r8BveO+LnkeEya/fXr3w/NuvXP70xXOi4Jo4E3n66bAlUAi6BZuNfGGkHeD5sVF/zOmFm4XVZGVkeKl7qpiAN1Qs0ptHaYUt+AW4CuFgSkNXlUSZp4Q5JCNvnDNVfILR95EDQfgyMgz38jLIlVKZXg/GVPyZcSArzNOuw7uPn9wxFHbzEqqnqUyIlx0YR2GRToOgK2JAhsfFwl+3QPl8ou6OxVyRCE4twJhr+de/1s/f/p+mqx98eOrDK4/Ccycc+ujUqdVX/3T15Tt3xLO2MwNnnq6/dT5YjtTxvDYhGFBRvMMGqONSKfgrcQUOFic5QgZBlIejNpcQEjAiKnzhgbrCwYB3+tiyKVNRysgwV1xGQN6A0pogaIOjrcyoI2OcrIZKQ9DCahIDidWw36kHD++GFu4bt7CcueUpdoqubEBXdZhzN+qWASXAGoGnAIcBwatScLswdx4eh2C9eP78+eu/efnyK6+urr76xfcga+6+zfCb906devODm6+duwMTGR444wqef1+w2Gh5fIE4spo+5NFizijcYjXoZdVoJVfEK086OFRg+CQEAu+Sysau8ETEb0KaT8qZNZBCHW08WfY4UoSZIN5KJZ50bCSPkTHdOvKRzjIEUKEQhQKF1iYGvTdWe/nJnz3xxNEdQ1MBR5ZBbpqaA/ioN1iQdXewAL6COoomhTgPq1p2RaB/WFp3vXci3DsQfuvc+YvXL8K8X7m1eurKoe/uhK7cu/OH1//tAgz75ZfvnI0667+Ycrq/IjnGnLsAkXJbBBz+YovR9if6CwWVB1FtOpU+E4RpQsoI/mnQR8I/MDwRtaKnqIGtLAU1MyPi1RxQVhNEBqVhizeqIAWAEIWKhGAorsoqmSBdR+hLh4fBGgpe5EAbLTTVIsbUBp588smf7d6z06Zz1Ms3j2qalpIDQVg/EcZNDBZ8XhExhVJh/Sjwh12RsFMREYeOTwzUveLF6/5PL5PFWn3vOzqkNBd6T66+vrJ64dTHf7r28ll3IOD1Wb6K9Pb3PdNrQ70ZUSnyZ0hiYbmi5LOrIUmjbsSkSUs07I7Irv27dvX1D/dC5Ad6S6gaWqtNSvi1rQz1oiHSTXI8ZYJTLNxpi5OEQNGNo+c6RxgWCjTHG9w8DUsE/X6t4VmjR2GkYotBiWbwZ0cP7wiLmWwRBXr6qpkp2RVQKJcWEMqlGDJ8Tjp2LDYRjkAVLb6g1zbef6Z8+/rFO3feuXz1yv859eHrl74bVwgC74nYJ5+98Oybr//ry5/jFQcvWqbODIbrUxApr6tUrpdiJZ/o9uFYKj+6iTgGJjsV51MaZXpzuYyb/OMAdiTR6Ve1Rj5vfJbLPPzTRiuRCpmQbzC6FTI5LuCPlQWn2yviL3B6ITgCSYQgZcrdOPnKbRyqJghFo6l2oYY+SCMmSE/87OjRY4MCj3yiPW1KwaOoUUDE+oPYlitRlHuROy4LCkmlDZIV6Q27nP5yv+u6O3D2zqfxu6+8jRD65nf96L8tsZr84rcIbn777tWXrwcviq4zA7/41YDNWzjri6E077KVYr4y5CGK1L/CmfHWec7oPpajfFKGs1QMIeeeCUlZ2Gw+KWHrs9OHk3gINaopwG7zLK/HTSGxbPEJdKYazgUjijpHqLnpKCfAh2vUIemwsFx1Pg8Ht9VopDV46imzeOKJ3U8c3iVUwFIrYTbJFd6EUElzQOi8eEwLLIS/7MQLjkFwLXR6Qf9AXfC9dV08f/7967++fPfKx6cu3Pj6O1mr0ZV7GvjB86dOffzBtavnnNfdzvFd/61vwBJVAqW6zYn4BoLgtPgAL4o4WUg+V2RQdHI4KqzsiFOrCvJJGQ7OUA60oFiO35KKdrjzNH9jZTg+5EglkR/X5RRriRkPRcdegaTOsWCdY4rQB4ArC6U0wBWXp3gpi0eLx+FBwUMNP7Ub6IsVUIaUQhQQZijLqBktdM6gKMTclhIdiQEXRyg4SzhHZBhFs7euB7ATXr/+ztWbN54/9dkn38mw3zNWkx/deuHCrRvX7j4n+M97678amsIKBwVbOFx3wQ3GO8F9FJ8QXSCuQG6SZ2V4hKiyy3IG5TpiSJI6dSv6D3WVON6j1DL6+bBvYaM0Wjt0NhCjQgsAgvDAxpEfro3DiaboilQJ56vFeNgjGVX4zsm2IeoMj+3Yffip3UdKgXhWwrbAVjhzLoRqjomLBygNYoGpECw+21TZK7ioscE3sOvnzzz95Vfn3Nev3/70javvfrx66u3vmcj63W9P/QMFN8/d9p0/H0M5IlYKhy0+8FSeigjeklFESobiimrieLLHsDEBvGJHRdZDUgoFd1OWQn1qU0hRu1HIwcOZ5h3wkVq1Gnz3DKRKZis6XAoiyIBBk3HgTiS8AZxRhMSGBRIXi7KhkJrEBimDrTgVX6Wce+ToycO797pE2ZQN8eC/kjHiR6TReC86J92WWAyyGYmUKcoRIWr1oV2/+LJ+9kVv7Padd964duPWqQ8/mvteDvvrzz/77K0r1y7fjkGz3y/FymF4JhGXawopUTrizBfA0uqqKZfiC7AFFT5AxpnP5czWhGcBtslDIyXUvGem+EaBeqLoo1LrUY6hpBSDpi0dnj7CthjIMo4DI3EimiYmJga20DsRqZdJsGJBOmKbr2CPhH/O4kHhiuV8O44ePnxybymopjJk7bBiioxCdBLipwa8ODcSWli2uCJTYdQ0BDc67MK/+NUZ/507zhfPnn/jNRKs3/7u+zjsn7x5AQm+V1775+vi2bMvQqSenohNRUqR3ik8m6/kjeroMJShXHIQPQ06Sqp+Jc6Z0aBWXaBedo+1VV3D7ocJnAaMTDoLfaHjaOPJDBhLwv4y2A8q8Av8QS+0pETHpgGdo3YGBwf7hoA+YLi/N0xcoWLkZRHv4dAGBZxzNBNmjBPIO544/NTJnS6BDRWwK3ijKOwGIYJog8tkqIOSTDtqIRakRZGb6e2tv/XW1Jel22e9758/985rN2+8ufrhla+/R8j86uoLpIEvO4krGKmJsC0Shr+O6MoCB52FAxpyxJELxXtAAFZgHZq1gY2Opt7yyC/UsO/h07do3LvVoLQMyVdchUSwlJCQObOELF08igS43+mkWGAqgmPT4I/h+Ji+nfv27T1w4ODBA/v27RweGI+4wJUbCWE9itQrlR01CXYcOX7Kxif7dwOHR/psBUdS98aCquiGuyFGkxInswgMWQRYrrLFHwtP2OqDw/Wpf7J99ZUg+hGEnD33zrVPXn3++Y8/+c5a+PUNuAsfX7l29ffeiy8hj/Lz4b5wGX3AUJUyugr9QlTOUIU+oNB5ltG4CUlcqJ3hDjgKXkupjmwEAJtcyMA7tVJZgkFCQMaaR+FLi4EQlZQzbDBaIC+qTHHTBCSqfxhHEu09eGRkZMeOHSMjB/YN9Y+HEQFDBRFMsQ4qjZm4FLVpIWik7geHWt9x+PDRJ3Yf2zVlaiWyGQXJT72AdvioXuBDKtYxzvrhfOBJJgawJ5Yiz0B6XQJMB8J9+eq1D/7H6urb31ELxy598tmpZ6GBV985674YeDEyMDg03Ds1MYDDloIsbAL0L+CGx+OtIEsb5VGZo+ZQRuKdU4N7R47smJmZOXH8+OHDx0+eOHYS9bywRcxIlMSC1c3gTB0UOZ2iw8TBw4KkbHHVS0Tt2rf3yJGRmROHDx+eGTmyt2+wNzwFc+N0QvdFuGXU4qhSLB7p79t7ZMcePNmxI/t3nDi6+/CJoUyrgdbKbJJCVacTQY7gx/bD0uoogsVVD9MhbRFXeHx8PGKDLwePTn/tGkLoC89/cumhnYUHNZC8UGjg5Re9F6NnSz/v+/lQJIxQRfCiKOJXAnSGrDcK3yUarWQTVppry+nl8aH9IyMHD+yFTIzgPewxGDtx7Njxp6Ahx/ba9JRGeheqBAWn34tkoYND7KfAI+9wNQFPcSd0D49y4vDIzpHdMwf39Q2M0zlrZciV1x2L0qkpBd/43sNP/tf/Avz3DRzfe+DgHjzfLiFjTliBohRi/RafKOte5CLJZLgDyv9t71rAojrPdBwuM1OZ0xkmAgsBZmDCAFEBtcowEByXlhkK0nSQRyiUUtxI5WJsF7MLVAy1Rje1KJKEAEaJCiiJutYbEi8kBo2m1ks1xrSoGJNu4jbG5tbt5dn3/c8MgtGE7pONze68c86ZMwNze//v/l9OXBC6JlJBVCBo1iuQFCKFClK3/GbX4WMIut+bPpoem1lIAoc/84c9e9euPXL4emfEwba26N6qMr2ktdvx3ug9CsfIgOxADL0KUqkxBmGMWCTAxytVb7WmWS0WK4jKAKhBzkTSlQ/pyi0sBF+gKxZiMcVnUrIpiEEnInwWeU3hMlcwVeAqBW/kTA/OVknpuWmkCqk6AhTQi2huUoRNmV4ElogFuMl8LUhPy7BmJIakFRTow2IxHXYi6PJODgiIM8UEmExhqmR0gEDfpoaj5GDPNEtKeA1MlgKCTAOdnc8+V7n62NHpo8gAgeFihY6bV9e2Hnnp2ZbB06aODRv8zVWIcJhmoNM7HL+KPagwIF5I/aB593mbzEYLLLElKcmo0xmNUCIrdANEJYYA5Ks4Nz8hAXRl5erDxyE2HRcZroJs+oVH+sKbmhAGCblSaKCCsFUhBSnIQ7ILnCkaF1V+6IcEuYFJWUXLXEQVubCA1BUl5Iq2SS9ML040ZKvHie6y+++dgT5BFSJSRG0YR4BUIEgd5JCwiqlSp9crQkXKGT2ucxt79Z57bxRj9UaK1cyZv/+vcpbYd3WePq/uaOtvqK6OijEFpapQX7EhWRCL8JomjP3qN+7+5kQQpQVHVouR/t1otcJzJYEsGGc3EnMhWgUFoAt8ZRXqQlF5GecFgvxsYUEIK70gZGGyvdK6uHJmYtx8qjPEoIACBkID/TCMPiDAlgiiQBN4yivKyxtiC1teTkJhem5uMWQYBiDD4FD7kC2OngjH+myBMf4IeMKRpacGxIWa4W21eqXGzxRqglR79W2DxarcOwrBgmiNEKv3XkJy8+phUBU60BQRZL9ovtLfj8Ag1J+GEW7EFOE1RayYMM3LodcZDTDHSr3SYLEk4dySFuyEtc0tAIrz82WanLnF6YU4SU9IyMopVIZzJTA1pCXGFuAVD+sXFkOuEFghqIK5Kzb4q5DwZoQoFXYHxIrpFNxtQEwBuCJPC3hHvnAAWPYrzaFxdwaD6ZDgFGtGmj51BvIpjm2KREqowoAiRLsxcRGioBEjlpd0mNREc1/ntk17K0dXep81fYQGHkNote/Z33SiR7JtZa8DTPmpgmzoAonyt2H4p2ncGJrz+8ap7AYLiDKCKKWgisKUkWKUAemCYqbAcjnz4dMKC6EfBen5hTlZWU5zcmRychASGnj3qRHhAchCUGJGqM6AIS3RGWVL9YsIDQ5WZkYFkio/cAUV9CteBnIgRRQl3BE8I1tZCVA/pzMxOCPNAjE3JKVZjfbQe+9jl9LYSDWoQg8BSlhoaVVqkDogkAmBKi7ChILDQOc1Dm/46yhK77PnDn+ErtOuyueOblvfFHS2raO5fceVK2F+2UxvsgPRezpuypiJ33jgft8Asz4lRQlJ1oGqJGsSuEkyCD1MQgyZFiwQAoijE9qRzoAxH04RIhCsSo6IM6X6ga4gxA8QK3QPQTFAVUqw04gOvaDkUGuGFv49lRoIa8XAohDiRHaIChBUCoFKIArRFkh0aBxD0iwWo8Wg1KVkIOLIVnuPYUeuj29cjJnClG3OZlgVhpquXZkZFB0R3dzcNn7rtqOvlpe/cuFvihdmvrensmv1scO71resbGvr6Gjv7Q+NKkOTa6JQB4i7F/Px7vuKtwm2kQG1pFRqtTprmkWp1/IZY0qaFUfyRqmyEhSs3ILiYgQPuYVZ+F3FxVCYAnMcSkz+oF9FywWxQniIt8M7hCRKKCiqp6qsVj24glCxhkW58k9YsGBOUWkeaAJAFQE5TSBPuU60C6QqGHdJBoPRwKVb4XS0qTPGPAC2pt0bFx1mUzkctCNhiM9sAYFmv1A1uYrvufbyS0fK13xa6X3uLMwCHOkDNx1bewAauLXzfNOGg2fb+vsDqwy1WgnKrUbXMHpmJnjZtDqlzqCFh1diiUaLEXwpYWgMhiQDZAz3Qv/o+wGyxXBLNlm071lZ6Qk5eelSuDoaXSwO9LqoIFY07RJNOyyzwhETqo6wZaRoGIbGyFwFwA3mzAFBgqeKCpzlgPrj6ekQ1uJitIczJCMlLYPqFxKcgSZDOokYBBs62iZ+g925yX7+LGZlSoqo1NAwNAMMlgl9Oh3j+rYefa4cY0Fu3wvN0WhzR8jYyy9Wri5/8YNd6weC2ja0Nbf31lzU1EpRgeHIk8dOQXU2LIpfAYkHmNLoMY0Bv5C6R6MFnmCoZK7AlixYMGJgioBgpYOtrAToDURLh/GAqmxzgNolVlFQQbwqJDHFnqpCZc+RYZCQ7FKuwgRXKkcOlS+vNA8s4Q0SCMpUQS4ilJAMK0UKn5lihHymWZLQfEqNkoFMkhTjOw3DbXymRIY5xExEfJojFIMbTNEULPXg4LVdL6F7b8/s21dBbx5ZemFf+eq1x/Zc7xls2xCx4Wz4jqqGi7UaRVj0+CljJ0+IV5nh75RalmLh8nRGJU7AEuRKr+dfCDwAKGiCuSQaeJgvOdDKTYdloWhBskqNYMQWGKRWcclVuCVYdtCb61SabWEQtSirUjK7uFKpGLw6ShdArMCUADJAYQGFejuhgsFWinMSPhN+ht7GCIejlEQjWvRmVew0MVLAyyYJN6JH4YGV5egOWPfBzq0ISCuP/H7mbVVw1k154KaPV69dAw30Bt0YKuswVGcibzpxLzLUGQHZGjQUFnF2saFBRQC8MYfTgS+NxD8pAQMJQvOmUKqgFfSONPciTQRZgq2cnLy8jEBYIUSKNqbadkaiFmtIcbCEYXD+ZrM9RWln4YpSRQSozIyqyBUtFDUPcQkD3mB8QHAGP5FA6CLaykg5B21yExotOn2UKpJ9teMj41IVZoVOq9Q60F/Q3LHh4OnOnr5te46sLb9tn87NA5bhA9d2sZNrfV97BHqNUtFFK0Zl+IyfmqpQGgwayBF0j8xosGkoYVo9jgoFzkga7bowVPjyGaQphJAdIh8hQ0wHEqhDFUUh8N4mFb2gmV4QohCc6zSiWoX4JFuycMltxgsqF+wVJApMuYHUCfGbEwE7+EojK5RmgmUvg+DMAJWUxR3PSv4RSL9R/EcIrcWcYEWgOq65eUPb6YH1fVtfQNxw29L7rJuoem8ffOBe5IGdTStXRmMAviOUc/DGYciUFh8uKTTgwwCVgwxBiAieQMDYhATXwhZIIWCr0lJIlxOg8cUponiZK6Co1OmPUc2oXTHBkfQoxgQXh+ix2j1cSbaEiZWOQHJFwSIkihTCTt65CANX1EBBF6Q3SdCEUOaGNWDpQiQV9NWIcKKCItG/PSnelGo2SwaNn7opIvr0abUPXOFhDIu8Ten95rHdz2C0MUvs18aeOY8BaHFq1tMn+KoDYb1pwvnZWpkfMgRhsiuod9RBCruRoJ0nSB6EjOkOIMx7gTAsTnpEGHe4MZjq7IgAjF7JhgoycbZCBTMkMxxVlD8SXDs6JWBTiLAYcKXMI2TZwpYlc0VNzAWcIAsaCCulg2mgnKNVXUqgZ7LMp/VoEE1qBEcu+071889USkGNTRHhG9SRkzu3vrCvsvXY0c82VsCpI9DAv35wfX1LU0QHusa90K3khYiNn4xGh9sjM6BKQZXL5FEvkyIogkQzmKStogqKegPsCLJoudmhJpAtJD1I24RgwaEVqiKQFgZmM2/WI2THf1gV5iitBNnK1JiRpoe5uPJDHpQCc0WZkpUPMRXIp/ZlAEMJaBrowvehGsjFaHgd6ANkjfqJ34J7mPVkdsN5qf0l//NNp1FNQbmnheNmKp+7RUB6z81UXXhx7YHWvSix+wxEx3V0YFpNpJpMsVVwg6YxLbBjyxQr9VPQjTqAVp5ZL7IbC0D5YiwKkLVggOEV00KqIIw7yw5Zwrob4qKDYkT5mKVjiyXDmZumidIopczM1GwNbHyMKoY6SLnyswUjXsjiK2Vk3XCDTG6CrUxI2VSQLnwx0AXZp4Dxu8PUQsIoXvKdZJuKOasoL4c1nQk9G96hHvjLpBb0QmNw8jOf5Gr2TRq4p7zrwN7Xnt21/sTptg5OgVVFgQ56PX6oDPIUlSn3HQDyH2CSgSRKOeJRflUyFELAlfOHFDCZxj1/VgHjUZazwFWOYwaGyqMGECXkymjNKMhP0ymN0Hj/GLPkYOUYZUWSBdhCIIlCsAAIpqyBua7SD3YAlVRwRBuFjIv2AJ6HIFmQLn5vkAi1hFkxm7xQa2wcOLOho6NZPdVn7Jltm460tt6iy/5msXr5Y5cGdp4+eDb+THNMJpjQKDWAgmoHmhQgivJEzYOMA1BCZBMIrqB6dH9WHuC1AeoBvzIaGZVOSBbUDxvMSzrLDSjPlFY41TPikDr7kSy0P/LK3PSQFGRPOkeY2aB0+AWEsmiqkjulUwsgVywpEG7BojLSvEOwUGu0wvXiHqrGgI9KJwJSNrJd2A+txt3IVBZzwIxJsU0DG852NMc1xU7r2frsa5Wrj3xycPL0kY8uIFxohQ/cur4FY7P7e6vQCHx3QELvShQCXckOavgx1ESqnQvwflb8QGFF5TZk49GKMQ4VAQRYZKLmLCZPDEezqEulWl+xVkw4u7yohzprfmFiWlKKxW7zz03Qo1QWbsIsQ7AVgEDeVlzE1CYL/NBWQaKckCkXEgEkzrBXiEYBNBa/DzRD+EF8MbS1+G56UkZDr5V0Rsm24Ux88tmO5KlNTX9af2brplfXfvrgZKGBlQdWr4EPnNJ3Rn3QLFVX02ewQah2OAi7DVliIDXkj8ESRR50AvxeAkPi5M5xoJBy0YHxFcgisujHAmNjfeM5DM0Uimqf2a4PTkgIhg5rHbaQOTlSILgKUoeHAuEmzMLLzWMUihfLKWCBUD/Sw7g3RVTP+IG0XEwZmDfo6LkR5OKEPkoBf0sgNKTcaZGtK/wDpnp1xDVi4smf+s48+1Ll2sp9733q4ORTa1Z3VR774671PXFh5prqGh3YB0GwsRRehpwQryj2tMAI6PlBRnbdafAPdPeQeFIECHkSO74gf4IgC7LF2AobI3fwRLYqikMxpoFTeeO4DhGvAJBYmpBhtSgdgWlzlmVJDnCFOZ2EGohxCh8ouCJbUGeXaAmni2o/hVsLIPrIyICokyC4HLY5W5h08RsrIAGMo8GhHv9b5mg/e7a5uVH9Fx/frR+8Aot19NO4uoDx/pVMbtarsi/WVFfX1MOAkyi4XWHJcS6BIjlHFgGfROuFjwVDejSTmys3ZSL+G4qw2PJCCWnbqYLMCCsSoyMjMUaSZKFPNiYwU1eQlxCcYrBn6xYsm1OqyLbFIL8GWL+MiPZz5uVQsEgUmRKRiBvIcWAn6YDZ7YCvLRIc5NGMTWUrT9UTjoqhIXc4SDjHBu38+eYrHZgMOegzruX6S8iIX7sw89M0cDU18Pr684cMF6urG6oUACNz2kMqnhwM19TU6Bi5yCxp8aFiK9ODzzIwWqYHBGtCuODXAGrfUOmPJmvx4sXo+kQWnBLd6OviKoITIjOTCivAlT5KW7pszrIcSUyPcpG1sikacpXFyAqBAsNPOVYHMgAwJdyK7I+NFH6ha/A91E08h52WVqRo4kxBRuGpasqqS2obsvtXnhj4y5S+ay+8srrr4023rzecOtK1Fnng+d9cq6+XGhrsmVVV9RKJ4l5Si7ev0Uj4g6LB3mBXKGDNqtFnWFZdjTNNtVRVVcUOYz0IYlgljDlUwirbK/wEOcKCTDFoL14MIBjNyyuJa4yNpA4mkyvMk0vLKSpMtFZVJbALIkeDST8MGmCugtrbV7b35mMUnwuULgbsCEbJVpoQKkQJ2AGlQG0N01ZtQwOG2eksQiUZYwkJIDQ0x7T4aOJaXRkmrEwYM+7Mrpf2Hlj73G0LWW+g67R1zR74wFRNQ2YDINoEIW+JrkRLt1eFEakcGd5ABiUR1ikIumK5V528oFEtTxifkGFBG9MNiiB+48ZFi5yLmObUFS4uXgwtOo74SvJqjHdxFW0KSDVrnHl5hU6jFLJMcKUVXAUEAShe9fc7CkUplIThHURegwPhZP2KjIEPahs2ETOALkCLVqZuiNBKKf4BRAE0bhQw/tgy/NU//P7JvluffRF97oefuc3ghT1QUYxiv7a+95DUcBGAySrTl+hLJKmKMoatCjIk86SAgJEjNk5NrZHlooVJtYSwnjBVcpbjChfkfCcRPBGiOnocgM3KOW6O83JzxSWuopQFebBXyuAidpIuyNE7yJWAKuCgShWVQJroP+sS6vIX5y52AiLFCQZwAsgxw1AIyvaWtKRLgs0VgQ8tq4tQWbpEjC3GnCgUXmNOtLy8Zy+KLW98/dYa+Gor/nj4+m8GSqSaGlLVUM3wMzOzSiHVV0kKMAW2oqqqFLjhT/oa0UI1aLuS2pISfKHahbqFtQsFLN0Lk8hWt7W7eyNvAHNC6iAscm4+qWIRKyfdcRZkxXu5uaK5ykuwpuUtA1WQK6WbK3El0CthDTnE0qV1TAiZ3BQLCx8i6OomWN+AMAOMhXWuvFkDzihoWjQ29IMJPy2ZW8RocWXC9LrsaV8ZuPbsK5Vda25dyHoDMoehVi909u2waxQNDRgcAV4w4Er2dGDMrqiCgQJqamCmiGqATyn1kCfAYHzCiM2gWwiaEChQoIAUgAEPAbpAlozjhXV1dVnOGC+vEydmyFxhhKIiLasoLz0kC1Shv2ZOjs6ROsQVk2ddaenSrKVLWWQvPM4eoWJyP+QMN6algSwYLvTCidglCSUHyD3z1SFAukSJRAYegzGZR7sQrwl/8j6zjcP0jrx8C8H6AzSQw413teyAsmXCLoEpShLjEE1NWU21RiqroXWHJccGorDzAOiUTwwHzOoTSUnYYOHBEiHKojQn2MEWx80g7F5chxRnUf+JgRMzZK6igzCtKTinKC+/sIgd8OxKNmQP40rV22tZCplKqCusE0VRvFOuKPEsYoBFULxYMYPFxMb8RrYJItfCATRlylJFUSIzInWTYy/oKm5lvesnD7acgmDdqpD1daSLXehmvn7en7xTHqurqyA0UPIaqYFPNGgaaqQajeZijYC+rIRYqMQGstgwiOnkiiQPLHoj5YcXJ5hHy32E+FUFzsWL4ATBFGvuG9sjvU5ERsY3emEeflBqtjIxYUEpRnZQqiBXeQbEogEqF1XgauNS4QcTRF8gPIRzsXMRXAbNOsYxZYg6WRo+W+SjopNE9ohy7Ow6Z3gl5Ir7UEVACBkzouozX53QuG0Txr4cO3WTYE2f+XsYq9WIQl+vr5VcaKB1IklkHMYIOzmCqtXgJgw4boDQePC10CibKrLFnFkUHqCMcibIwTPYu4ND8MsKihcjJ6w7npNVWqprRsgQGRvZ6NWIUfO92cbCUiTHpCpPcGUEV6HhsrnyU7X3LoYPRBoJx5Bel473wR4Cn0EVpEAxHAVLLPaBJgB0kS3XSEqCpLn6TcgZIXNltyuikPVCndrHju27dp1jqvZduEmq3tjX2oVu5g9e31FTC3YoPJqaGqgYIkwZeuyw4DDj2hK4RpzUKmspP7W1ulodGCJTJbhh0y3kE90u4mDaFhrLktIWoc8ZWpMIh5iYm5gLcwUfWJdVWpbcF9vS6EvBQjenf1VG3oKiiqI5YiwHRKvU4PBjH6pMVtiVwHwwlQDHkC8HCblQ6UTAXdFHs1C2wBcTZ4AckTN3KCqD1nxY8gr+XIRJvKuuMh88G7nr6F9bu8pHjiGdeQEdN8iZD7+wrlpZW4IXlSD81vMN6kdg/vyS+dx5Ay9DWEi7bgAzQ4Bf1JKtFGd6QumyZZd279//Oxn79+/ffWlOXlHO8fxzl998/PGl1cmxjX19LbHgaupKlb8UsgCGCrsA7FWSmfUrmaywK1ds6QlL89BFL9uzvKzjzsRcBiTC1YZwS+umX4FkgStSJECWPoGhEIs1QJwCIkCFGb54sX/yNWY6rS/+foQWnnp19YGuyj2nnt++vawebGwfzs/N+IkMnuEG8Jwvwg6sK5nffa7uMnCSDP30Z7fB7/bvPrlzybyruw/FJvv2NfZRCZtWBjjKisXYM5ABqioqFlTQXoWGuskKqMKb4l3d70vuL2GcWoLz3Mbuhd3dSd3dEGkIFFgiWTyRDehwvqCDQ3c6l1i5i4GCsZonLl6Z1rPr6LHK1jWbLozouGk9cKDr46MvPP882NqOI8DzYZAJev75dT9Z90m8f+5tSMjjjz2289dPbt685erV5U8//fRPsY8EnhP4GW74rT9dvuKRh+dd3REf6dvY4tsHrqaqex1lC5aBqFULVq3CWD2M15tj9ccALXfYHtPe/Tu8Uob77QRnEFdwtqpuETgrmV82v6Ssur7eJfdKiro7nxfccJd7LGhlGIrqa0EYWROgg+/HuJl9a1orn3v5hhai67TrwIEDL+556T8E3n33VzfhnV+948Jv3/ktNhfe+u1bxJYtSx5dsmLezcAzt8JyGU9jX/HwQ4/MW/L6ifh431hoYUtjRJufY+Pu322+dGn35s37N0Nkru7f7fTHVLkgF1dh59dd/SleircZjqF2WH5189XNT17aefKxN8+9fe7cunVsYUJI/Q2roVRiU8rnMMZgi5YYGQrMMp6oL2GqG9W76+gr5V17D78x3b3C1alXWkFV1+rWY3t/+e9P/eKpX/z85z/+8Q+If5LxLyPxox9hG8IPf/jD4efA8POHxIF45KFHZDz8MLYVK1bg/pEV85Y/eb7lhO+gL7hq9Io4aDtUt/np5WB0SBD3n0vtbQ8NCm8LDyVZveuuLp/3sADeYSTwFOBqI5wsAbZs2fLWzncef/fNt99+e9370AuhMTJ92AEYkhugQXaZHYhW/esvY6mFta+e+k8XV2+8tqZLUFVevmbv3l+68O8ynnoKmxugcQg/d90R4NYNkEyaieFsAzLNgIs8EjZvydWn6wZaBvt6Jk3imuOQq+1vblm+QoYshpu7d7S3Y2prG8kKVZ1//+q8hx9hE7AhfoTbiHYicC63kLtt8GmPfvjQo49++OGHv33nV796912hPm//B+h7X2Dd++vAISwMrAwo5BGM/QQPr596sfVA5Z43ps8kVbP/+INf7iWGCBqixs0DNpkEbEMUjGCCZ+RjSASHvj4O/FFkB0d89SEBgEzN23nppGNw0LuvZ/zgINf8D/Lf/ubVeUJg3IQ92f16+8pQNcjCqO7w9nbIFf4BUgrCyBM+jB9946vwNgJDf+Au6wUPYv/wo7dwgz2BfQGLAJkEh7j9Efhg0761B1Z/7Br1/sy7K4Za5sbvEo3CuxF4VL59BpbAfN0K0IfNWzZjc+HJzZdOrsoeGBz06emZMGHQ94RXRKj/9pNQweG2bXd3r2pluFrA1Na2cuPV5VdpDLEDZJWsPSTTRjrc+DEa+eeQf7Q2Dtjkc+DGgXAROpzVX3z01EcfffRfwHMvfnzgwOryfRfEElnf++7JJ2+DXwvs/PVOGSd3PrbzscceO4n9k3jcffc4tht4UxyIVY+/uerNVauwu4Boc9myxQPxkyZM8wEmjG+hXJVcgpcbhp/tru/lQkwbMFs5Lq45Qv36nEsngUu0/3C6+JqbtwBLtrCJ0FJuySWFQiGHkeimB0wNAYYExoWgvXGZHmgYj79cs6aytetA19qPXaX3md8/fWjjuXMbN55DJQ44J2PxuUXnkLaNQN3iujrsWXXI43BGLMWjrKXuBwK4G4nSpRUV8t3SyxUVeCCORQyh6ptavCf7PDA4Hgv29DWCK+Wq3SOxaodfO6a3JXsRkY1N7XWgmRtCURG0gnbEVydPLiOFbFO5id96EgwSj24Bgw9DbWVNGfI+I1gU1oUUgjZBEwDTtKa8vLK8EgsuvPaH6YIrYPrXn3nwQV7o59viamK4GOc/cMnUiV994JtYZwj4Dmco341JLvdjYhb6/E/ERR9kR7G9ASm1dBEFRZTha+V0kcFMEuJBJs+oyWzM2Oga4Y5SH6qi4DwftItaX36gF2Ymjxk/5ivTejr74rFY1MWcZRS6y9gRY1WsWrXIrIqeKlbgBBCERZQULbhcdLkiD1sFtlUV4P4yH5RersDrxI2Hx5kVEJB0waKLR0giKaQowi7IDtkFMCkIBNxWEAxC4H7w0bbh6TPgPuXtlgCv2IAby7POevBf/4xlHSdi2jom6aEXj2hv7+9v7xcTlmPkK8o7Uh2E+ZD50CEUROYrwK4G5ZsrZwenTMNKO9N8Jvfc63sCXOUfz5HHVGHjkIW0wPYIL16TBODyH8lm9p+iUiGwcRFScTaBa3RXIh7KcKJRoBx15+qEPmCT4RL9y0svX4ZlAI+y9XjnsXd2UhgZMIJDQtjehx8Fg4+sWLL+rtGB1GEf3eynf/v+t/7xO9/86p+mje3pi21sampa2bQS0zSbcUPHAtw/pq/3+tl6U1N7MXi6jVxNEzO/vMcNnui4cjEtBJmvhZCHQ2htoaBKLL3t7e09OHj2CopSSlFnRAZmD/TjkrnjMHkfw+0fuFtcXOi7YrFXTj3/i3dLeCDgcOw4lL3jEGHGvp033GPfsWPH62KTTw7t2F6/ffuO7c/zoRvnBzr/4a7/HYBYHmXMevD73/oaputM8+lrxEjfZnVzW3h4P+DX24vR7G0zJnBNCy6yA08IrjKfsLAezYy2pKR2odFi9zNF+o6/15vAv3nH92tqMCQzakfT5Lu/NWumwI2PG1ESIO758zSyeDdsydf+/Gcs3Pn9B3H9Na7BKtqfoA2aOUJ9prte/PWZ35Pf6PNZKHJ03AlgoMm/fu2BseM7gLY2qCgmH4dG9vSsn0KquDZBfHN/lNG4sKxeqqpHd1s9qjkWe1h07HheLwfAP3pPCkexNrvxO9NHdelaF5E8c+EzvuaNVw6r7n1eaxiNmq5hl/0aE9ncpF4ZiqGzB5P7enp6fMRqBJNaZjTFRBmfqNWgHwQFfvYK1xobYqJPTJrg4soHSqi2223/+D/79l+UdHyOAG/fHjs12oQlfPyaffswDxfWCGY7Pm6lX7VFp2XXZmaUKIrXWrQ2U7KvWD7bu4f2alJ/Vfa3v9CGvvO4Z+JUk8ocFRPdGB9LJ4d0ME4dgAUPlRr0G5mzATNquoakTFUEL1sl1nmintoyJ7qp+kIvGnFHMeu+CH9Jn4oZC8kYazk1Wo3ZS9pgTKw0c7YgEAi2lCEp2QGYfwtCfWN9Z3glB5ljZK6/+CtXzr6DFwO7a+6YVKNFwsKzKg7HxnB2ZUiw1hwoVo4BMOKdi+BnKGwBmLUjFi4y+UVpvkmmPp+Fsf/2lWnvmfV5L5E/asyeaAvmFCMOqMHcLmcGR6ah9sIFr8JNASo/hz0lPz0kSUOtNGMAd4rVfNedgzzTee5ddwr/dvdkX6/k5Bm+47ynfOU+XpSYuJsXcLyfl1CNN9miJHSxc92PmIhxE//5rjsIXjvx7+vKj3/f8FDloep/AXPvyLUev6TAYobA3NmzP59LL/yfxnTZGwK8u3MxxJcCIIvAkbgjod6XByBrGDwxxKditosmj2SNArM8ZP0NmD57LgiTrbyHrFHaLVAFeLzhZ5LllishWJ/TVcH+j2KYjfdw9RmYO5KrezzRw6dX/25wNctj4j+LLkajIO2u2XeuBvhlgWtV8rkyU0OM3cna/N8vZt96HZXpd7DW/KUB1JFUeazXqAKJWa4w1SNYoykGYrVW4P9xP8Zou7tvJNZD3YnT/9+S9hlcYcTSbGwypstPedTRAw888MADDzzwwAMPPPDAAw888MADDzzwwAMPPPDAAw888MADDzzwwAMPPPDAAw888MADDzzwwAMPPPDAAw888MCDLxD/DbR1sNMFnIBwAAAAAElFTkSuQmCC" }</t>
+  </si>
+  <si>
+    <t>entityId=(OPQA-4773_id)||entityType=posts||mediaType=image/png||context=1p-authoring</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-4773_id)</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4773_id)||userId=(SYS_USER2)||title=Test Post with invalid img src and invalid iframe src||content=''||wasCleanedUp=0||wasTruncated=false||found=true||coverImageId=""</t>
+  </si>
+  <si>
+    <t>OPQA-4774</t>
+  </si>
+  <si>
+    <t>{ "title":"Test Post with valid media id in the image src", "content":"Testing of image with valid media ID &lt;img class=\"fr-dib fr-draggable\" src=\"/api/media/(OPQA-4774_mediaId)\" style=\"width: 300px;\" alt=\"Post with valid media image\" width=\"200\" height=\"200\"&gt; &lt;/img&gt; &lt;/br&gt;&lt;/br&gt;Make sure above media will be visible from UI." }</t>
+  </si>
+  <si>
+    <t>OPQA-1076_6||OPQA-4774</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||title=Test Post with valid media id in the image src||content=Testing of image with valid media ID &lt;img class=\"fr-dib fr-draggable\" src=\"/api/media/(OPQA-4774_mediaId)\" style=\"width: 300px;\" alt=\"Post with valid media image\" width=\"200\" height=\"200\"&gt; Make sure above media will be visible from UI.||wasCleanedUp=2||wasTruncated=false||found=true||coverImageId=(OPQA-4774_mediaId)</t>
+  </si>
+  <si>
+    <t>{ "title":"Test Edit Post with valid media id in the image src and youtube links", "content":"Testing of image with valid media ID &lt;img class=\"fr-dib fr-draggable\" src=\"/api/media/(OPQA-4774_mediaId)\" style=\"width: 300px;\" alt=\"Post with valid media image\" width=\"200\" height=\"200\"&gt; &lt;/img&gt; &lt;/br&gt; Valid youtube link: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"http://youtube.com/foo\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; &lt;/br&gt; Testing of vimeo with valid src: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"https://vimeo.com/172911816\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; &lt;/br&gt; &lt;/br&gt;&lt;/br&gt;Make sure above media image along with youtube/vimeo links will be visible from UI." }</t>
+  </si>
+  <si>
+    <t>OPQA-4775</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-4775_id)</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4775_id)||userId=(SYS_USER1)||title=Test Post with valid youtube/vimeo links||content=''||wasCleanedUp=0||wasTruncated=false||found=true</t>
+  </si>
+  <si>
+    <t>OPQA-4776</t>
+  </si>
+  <si>
+    <t>/posts/post/(OPQA-4776_id)</t>
+  </si>
+  <si>
+    <t>OPQA-4776||OPQA-4774</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4776_id)||userId=(SYS_USER1)||title=Test Edit Post with valid media id in the image src and youtube links||content=Testing of image with valid media ID &lt;img class=\"fr-dib fr-draggable\" src=\"/api/media/1723214b-30dc-42a5-aa1c-a3e911f6b71c\" style=\"width: 300px;\" alt=\"Post with valid media image\" width=\"200\" height=\"200\"&gt; Valid youtube link: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"http://youtube.com/foo\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; Testing of vimeo with valid src: &lt;iframe scrolling=\"no\" frameborder=\"0\" src=\"https://vimeo.com/172911816\" width=\"0\" height=\"0\"&gt;&lt;/iframe&gt; Make sure above media image along with youtube/vimeo links will be visible from UI.||wasCleanedUp=2||wasTruncated=false||found=true||coverImageId=(OPQA-4774_mediaId)</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4776_id)||userId=(SYS_USER1)||title=Test Edit Post with valid media id in the image src and youtube links||content=''||wasCleanedUp=0||wasTruncated=false||found=true||coverImageId=""</t>
+  </si>
+  <si>
+    <t>OPQA-4777</t>
+  </si>
+  <si>
+    <t>OPQA-4771</t>
+  </si>
+  <si>
+    <t>/drafts/draft/(OPQA-4771_id)</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4771_id)||userId=(SYS_USER1)||title=Edit Draft Post with image, youtube links||content=""||found=true||coverImageId=1723214b-30dc-42a5-aa1c-a3e911f6b71c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1964,24 +2087,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="43.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="80.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="47.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="68.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="119.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="68.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="119.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2050,9 +2173,7 @@
       <c r="K2" s="16" t="s">
         <v>498</v>
       </c>
-      <c r="L2" t="s">
-        <v>500</v>
-      </c>
+      <c r="L2"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A3" s="8" t="s">
@@ -2082,9 +2203,7 @@
       <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
-        <v>500</v>
-      </c>
+      <c r="L3"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A4" s="8" t="s">
@@ -2114,9 +2233,7 @@
         <v>93</v>
       </c>
       <c r="K4" s="8"/>
-      <c r="L4" t="s">
-        <v>500</v>
-      </c>
+      <c r="L4"/>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A5" s="8" t="s">
@@ -2150,9 +2267,7 @@
       <c r="K5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L5" t="s">
-        <v>500</v>
-      </c>
+      <c r="L5"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A6" s="8" t="s">
@@ -2184,9 +2299,7 @@
         <v>26</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="L6" t="s">
-        <v>500</v>
-      </c>
+      <c r="L6"/>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A7" s="8" t="s">
@@ -2220,9 +2333,7 @@
       <c r="K7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L7" t="s">
-        <v>500</v>
-      </c>
+      <c r="L7"/>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A8" s="8" t="s">
@@ -2254,9 +2365,7 @@
         <v>25</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="L8" t="s">
-        <v>500</v>
-      </c>
+      <c r="L8"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A9" s="8" t="s">
@@ -2288,9 +2397,7 @@
         <v>473</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="L9" t="s">
-        <v>500</v>
-      </c>
+      <c r="L9"/>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A10" s="8" t="s">
@@ -2322,9 +2429,7 @@
         <v>475</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10" t="s">
-        <v>500</v>
-      </c>
+      <c r="L10"/>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A11" s="8" t="s">
@@ -2356,9 +2461,7 @@
         <v>477</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="L11" t="s">
-        <v>500</v>
-      </c>
+      <c r="L11"/>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A12" s="8" t="s">
@@ -2390,9 +2493,7 @@
         <v>478</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12" t="s">
-        <v>500</v>
-      </c>
+      <c r="L12"/>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A13" s="8" t="s">
@@ -2420,9 +2521,7 @@
       <c r="K13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L13" t="s">
-        <v>500</v>
-      </c>
+      <c r="L13"/>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A14" s="8" t="s">
@@ -2450,9 +2549,7 @@
         <v>479</v>
       </c>
       <c r="K14" s="8"/>
-      <c r="L14" t="s">
-        <v>500</v>
-      </c>
+      <c r="L14"/>
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A15" s="8" t="s">
@@ -2484,9 +2581,7 @@
         <v>25</v>
       </c>
       <c r="K15" s="8"/>
-      <c r="L15" t="s">
-        <v>500</v>
-      </c>
+      <c r="L15"/>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A16" s="8" t="s">
@@ -2518,9 +2613,7 @@
         <v>25</v>
       </c>
       <c r="K16" s="8"/>
-      <c r="L16" t="s">
-        <v>500</v>
-      </c>
+      <c r="L16"/>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A17" s="8" t="s">
@@ -2552,9 +2645,7 @@
         <v>481</v>
       </c>
       <c r="K17" s="8"/>
-      <c r="L17" t="s">
-        <v>500</v>
-      </c>
+      <c r="L17"/>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
@@ -2586,9 +2677,7 @@
         <v>29</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" t="s">
-        <v>500</v>
-      </c>
+      <c r="L18"/>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
@@ -2620,9 +2709,7 @@
         <v>99</v>
       </c>
       <c r="K19" s="8"/>
-      <c r="L19" t="s">
-        <v>500</v>
-      </c>
+      <c r="L19"/>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A20" s="8" t="s">
@@ -2654,9 +2741,7 @@
         <v>108</v>
       </c>
       <c r="K20" s="8"/>
-      <c r="L20" t="s">
-        <v>500</v>
-      </c>
+      <c r="L20"/>
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A21" s="8" t="s">
@@ -2688,9 +2773,7 @@
         <v>25</v>
       </c>
       <c r="K21" s="8"/>
-      <c r="L21" t="s">
-        <v>500</v>
-      </c>
+      <c r="L21"/>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A22" s="8" t="s">
@@ -2720,9 +2803,7 @@
         <v>101</v>
       </c>
       <c r="K22" s="8"/>
-      <c r="L22" t="s">
-        <v>500</v>
-      </c>
+      <c r="L22"/>
     </row>
     <row r="23" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A23" s="8" t="s">
@@ -2754,9 +2835,7 @@
         <v>102</v>
       </c>
       <c r="K23" s="8"/>
-      <c r="L23" t="s">
-        <v>500</v>
-      </c>
+      <c r="L23"/>
     </row>
     <row r="24" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A24" s="8" t="s">
@@ -2788,9 +2867,7 @@
         <v>109</v>
       </c>
       <c r="K24" s="8"/>
-      <c r="L24" t="s">
-        <v>500</v>
-      </c>
+      <c r="L24"/>
     </row>
     <row r="25" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A25" s="8" t="s">
@@ -2820,9 +2897,7 @@
         <v>29</v>
       </c>
       <c r="K25" s="8"/>
-      <c r="L25" t="s">
-        <v>500</v>
-      </c>
+      <c r="L25"/>
     </row>
     <row r="26" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A26" s="8" t="s">
@@ -2852,9 +2927,7 @@
         <v>483</v>
       </c>
       <c r="K26" s="8"/>
-      <c r="L26" t="s">
-        <v>500</v>
-      </c>
+      <c r="L26"/>
     </row>
     <row r="27" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A27" s="8" t="s">
@@ -2884,9 +2957,7 @@
         <v>484</v>
       </c>
       <c r="K27" s="8"/>
-      <c r="L27" t="s">
-        <v>500</v>
-      </c>
+      <c r="L27"/>
     </row>
     <row r="28" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A28" s="8" t="s">
@@ -2920,9 +2991,7 @@
       <c r="K28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L28" t="s">
-        <v>500</v>
-      </c>
+      <c r="L28"/>
     </row>
     <row r="29" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A29" s="8" t="s">
@@ -2954,9 +3023,7 @@
         <v>488</v>
       </c>
       <c r="K29" s="3"/>
-      <c r="L29" t="s">
-        <v>500</v>
-      </c>
+      <c r="L29"/>
     </row>
     <row r="30" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A30" s="8" t="s">
@@ -2986,9 +3053,7 @@
         <v>489</v>
       </c>
       <c r="K30" s="8"/>
-      <c r="L30" t="s">
-        <v>500</v>
-      </c>
+      <c r="L30"/>
     </row>
     <row r="31" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A31" s="8" t="s">
@@ -3018,9 +3083,7 @@
         <v>25</v>
       </c>
       <c r="K31" s="8"/>
-      <c r="L31" t="s">
-        <v>500</v>
-      </c>
+      <c r="L31"/>
     </row>
     <row r="32" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A32" s="8" t="s">
@@ -3052,9 +3115,7 @@
         <v>25</v>
       </c>
       <c r="K32" s="8"/>
-      <c r="L32" t="s">
-        <v>500</v>
-      </c>
+      <c r="L32"/>
     </row>
     <row r="33" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A33" s="8" t="s">
@@ -3086,9 +3147,7 @@
         <v>25</v>
       </c>
       <c r="K33" s="8"/>
-      <c r="L33" t="s">
-        <v>500</v>
-      </c>
+      <c r="L33"/>
     </row>
     <row r="34" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A34" s="8" t="s">
@@ -3120,9 +3179,7 @@
         <v>25</v>
       </c>
       <c r="K34" s="8"/>
-      <c r="L34" t="s">
-        <v>500</v>
-      </c>
+      <c r="L34"/>
     </row>
     <row r="35" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A35" s="8" t="s">
@@ -3150,9 +3207,7 @@
         <v>29</v>
       </c>
       <c r="K35" s="3"/>
-      <c r="L35" t="s">
-        <v>500</v>
-      </c>
+      <c r="L35"/>
     </row>
     <row r="36" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A36" s="8" t="s">
@@ -3180,9 +3235,7 @@
         <v>11</v>
       </c>
       <c r="K36" s="8"/>
-      <c r="L36" t="s">
-        <v>500</v>
-      </c>
+      <c r="L36"/>
     </row>
     <row r="37" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A37" s="8" t="s">
@@ -3210,9 +3263,7 @@
         <v>29</v>
       </c>
       <c r="K37" s="8"/>
-      <c r="L37" t="s">
-        <v>500</v>
-      </c>
+      <c r="L37"/>
     </row>
     <row r="38" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A38" s="8" t="s">
@@ -3242,9 +3293,7 @@
         <v>29</v>
       </c>
       <c r="K38" s="8"/>
-      <c r="L38" t="s">
-        <v>500</v>
-      </c>
+      <c r="L38"/>
     </row>
     <row r="39" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A39" s="8" t="s">
@@ -3272,9 +3321,7 @@
         <v>29</v>
       </c>
       <c r="K39" s="8"/>
-      <c r="L39" t="s">
-        <v>500</v>
-      </c>
+      <c r="L39"/>
     </row>
     <row r="40" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A40" s="8" t="s">
@@ -3302,9 +3349,7 @@
         <v>11</v>
       </c>
       <c r="K40" s="8"/>
-      <c r="L40" t="s">
-        <v>500</v>
-      </c>
+      <c r="L40"/>
     </row>
     <row r="41" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A41" s="8" t="s">
@@ -3332,9 +3377,7 @@
         <v>493</v>
       </c>
       <c r="K41" s="8"/>
-      <c r="L41" t="s">
-        <v>500</v>
-      </c>
+      <c r="L41"/>
     </row>
     <row r="42" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A42" s="8" t="s">
@@ -3368,9 +3411,7 @@
       <c r="K42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L42" t="s">
-        <v>500</v>
-      </c>
+      <c r="L42"/>
     </row>
     <row r="43" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A43" s="8" t="s">
@@ -3402,9 +3443,7 @@
         <v>25</v>
       </c>
       <c r="K43" s="8"/>
-      <c r="L43" t="s">
-        <v>500</v>
-      </c>
+      <c r="L43"/>
     </row>
     <row r="44" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A44" s="8" t="s">
@@ -3436,9 +3475,7 @@
         <v>166</v>
       </c>
       <c r="K44" s="8"/>
-      <c r="L44" t="s">
-        <v>500</v>
-      </c>
+      <c r="L44"/>
     </row>
     <row r="45" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A45" s="8" t="s">
@@ -3470,9 +3507,7 @@
         <v>168</v>
       </c>
       <c r="K45" s="8"/>
-      <c r="L45" t="s">
-        <v>500</v>
-      </c>
+      <c r="L45"/>
     </row>
     <row r="46" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A46" s="8" t="s">
@@ -3502,9 +3537,7 @@
         <v>11</v>
       </c>
       <c r="K46" s="8"/>
-      <c r="L46" t="s">
-        <v>500</v>
-      </c>
+      <c r="L46"/>
     </row>
     <row r="47" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A47" s="8" t="s">
@@ -3536,9 +3569,7 @@
         <v>25</v>
       </c>
       <c r="K47" s="8"/>
-      <c r="L47" t="s">
-        <v>500</v>
-      </c>
+      <c r="L47"/>
     </row>
     <row r="48" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A48" s="8" t="s">
@@ -3568,9 +3599,7 @@
       <c r="K48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L48" t="s">
-        <v>500</v>
-      </c>
+      <c r="L48"/>
     </row>
     <row r="49" spans="1:12" ht="240">
       <c r="A49" s="8" t="s">
@@ -3591,7 +3620,6 @@
       <c r="F49" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G49"/>
       <c r="H49" s="14" t="s">
         <v>495</v>
       </c>
@@ -3603,9 +3631,6 @@
       </c>
       <c r="K49" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="L49" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="2" customFormat="1" ht="45">
@@ -3636,9 +3661,7 @@
         <v>11</v>
       </c>
       <c r="K50" s="8"/>
-      <c r="L50" t="s">
-        <v>500</v>
-      </c>
+      <c r="L50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3650,24 +3673,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="I60" workbookViewId="0">
+      <selection activeCell="L61" sqref="L2:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="58.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="45.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="80.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="133.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="58.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="45" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="133.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3738,9 +3761,7 @@
       <c r="K2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L2" t="s">
-        <v>500</v>
-      </c>
+      <c r="L2"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A3" s="8" t="s">
@@ -3772,9 +3793,7 @@
       <c r="K3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
-        <v>500</v>
-      </c>
+      <c r="L3"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A4" s="8" t="s">
@@ -3806,9 +3825,7 @@
         <v>26</v>
       </c>
       <c r="K4" s="3"/>
-      <c r="L4" t="s">
-        <v>500</v>
-      </c>
+      <c r="L4"/>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A5" s="8" t="s">
@@ -3836,9 +3853,7 @@
         <v>180</v>
       </c>
       <c r="K5" s="8"/>
-      <c r="L5" t="s">
-        <v>500</v>
-      </c>
+      <c r="L5"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A6" s="8" t="s">
@@ -3868,9 +3883,7 @@
         <v>180</v>
       </c>
       <c r="K6" s="8"/>
-      <c r="L6" t="s">
-        <v>500</v>
-      </c>
+      <c r="L6"/>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A7" s="8" t="s">
@@ -3898,9 +3911,7 @@
         <v>178</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" t="s">
-        <v>500</v>
-      </c>
+      <c r="L7"/>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A8" s="8" t="s">
@@ -3930,9 +3941,7 @@
         <v>265</v>
       </c>
       <c r="K8" s="8"/>
-      <c r="L8" t="s">
-        <v>500</v>
-      </c>
+      <c r="L8"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A9" s="8" t="s">
@@ -3962,9 +3971,7 @@
       <c r="K9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L9" t="s">
-        <v>500</v>
-      </c>
+      <c r="L9"/>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A10" s="8" t="s">
@@ -3996,9 +4003,7 @@
         <v>238</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10" t="s">
-        <v>500</v>
-      </c>
+      <c r="L10"/>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="8" t="s">
@@ -4030,9 +4035,6 @@
         <v>181</v>
       </c>
       <c r="K11" s="8"/>
-      <c r="L11" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A12" s="8" t="s">
@@ -4064,9 +4066,7 @@
         <v>241</v>
       </c>
       <c r="K12" s="8"/>
-      <c r="L12" t="s">
-        <v>500</v>
-      </c>
+      <c r="L12"/>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="8" t="s">
@@ -4100,9 +4100,6 @@
       <c r="K13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L13" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A14" s="8" t="s">
@@ -4136,9 +4133,7 @@
       <c r="K14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L14" t="s">
-        <v>500</v>
-      </c>
+      <c r="L14"/>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="8" t="s">
@@ -4170,9 +4165,6 @@
         <v>266</v>
       </c>
       <c r="K15" s="8"/>
-      <c r="L15" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A16" s="8" t="s">
@@ -4204,9 +4196,7 @@
         <v>267</v>
       </c>
       <c r="K16" s="8"/>
-      <c r="L16" t="s">
-        <v>500</v>
-      </c>
+      <c r="L16"/>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A17" t="s">
@@ -4236,9 +4226,7 @@
         <v>430</v>
       </c>
       <c r="K17" s="8"/>
-      <c r="L17" t="s">
-        <v>500</v>
-      </c>
+      <c r="L17"/>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
@@ -4270,9 +4258,7 @@
         <v>201</v>
       </c>
       <c r="K18" s="8"/>
-      <c r="L18" t="s">
-        <v>500</v>
-      </c>
+      <c r="L18"/>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
@@ -4304,9 +4290,7 @@
         <v>208</v>
       </c>
       <c r="K19" s="8"/>
-      <c r="L19" t="s">
-        <v>500</v>
-      </c>
+      <c r="L19"/>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A20" t="s">
@@ -4336,9 +4320,7 @@
         <v>434</v>
       </c>
       <c r="K20" s="8"/>
-      <c r="L20" t="s">
-        <v>500</v>
-      </c>
+      <c r="L20"/>
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A21" s="8" t="s">
@@ -4370,9 +4352,7 @@
         <v>268</v>
       </c>
       <c r="K21" s="8"/>
-      <c r="L21" t="s">
-        <v>500</v>
-      </c>
+      <c r="L21"/>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A22" s="8" t="s">
@@ -4402,9 +4382,7 @@
         <v>29</v>
       </c>
       <c r="K22" s="8"/>
-      <c r="L22" t="s">
-        <v>500</v>
-      </c>
+      <c r="L22"/>
     </row>
     <row r="23" spans="1:12" ht="30">
       <c r="A23" s="8" t="s">
@@ -4434,9 +4412,6 @@
         <v>178</v>
       </c>
       <c r="K23" s="8"/>
-      <c r="L23" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="24" spans="1:12" s="2" customFormat="1" ht="30">
       <c r="A24" s="8" t="s">
@@ -4468,9 +4443,7 @@
         <v>25</v>
       </c>
       <c r="K24" s="8"/>
-      <c r="L24" t="s">
-        <v>500</v>
-      </c>
+      <c r="L24"/>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="A25" s="8" t="s">
@@ -4502,9 +4475,6 @@
         <v>25</v>
       </c>
       <c r="K25" s="8"/>
-      <c r="L25" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="26" spans="1:12" ht="45">
       <c r="A26" s="8" t="s">
@@ -4536,9 +4506,6 @@
         <v>25</v>
       </c>
       <c r="K26" s="8"/>
-      <c r="L26" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="27" spans="1:12" ht="30">
       <c r="A27" s="8" t="s">
@@ -4568,9 +4535,6 @@
         <v>182</v>
       </c>
       <c r="K27" s="8"/>
-      <c r="L27" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="28" spans="1:12" ht="30">
       <c r="A28" s="8" t="s">
@@ -4600,9 +4564,6 @@
         <v>183</v>
       </c>
       <c r="K28" s="8"/>
-      <c r="L28" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="29" spans="1:12" ht="30">
       <c r="A29" s="8" t="s">
@@ -4630,9 +4591,6 @@
         <v>280</v>
       </c>
       <c r="K29" s="8"/>
-      <c r="L29" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="30" spans="1:12" ht="30">
       <c r="A30" s="8" t="s">
@@ -4660,9 +4618,6 @@
         <v>279</v>
       </c>
       <c r="K30" s="8"/>
-      <c r="L30" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="31" spans="1:12" ht="45">
       <c r="A31" s="8" t="s">
@@ -4692,9 +4647,6 @@
         <v>269</v>
       </c>
       <c r="K31" s="8"/>
-      <c r="L31" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="32" spans="1:12" ht="45">
       <c r="A32" s="8" t="s">
@@ -4724,9 +4676,6 @@
         <v>270</v>
       </c>
       <c r="K32" s="8"/>
-      <c r="L32" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="33" spans="1:12" ht="30">
       <c r="A33" s="8" t="s">
@@ -4758,9 +4707,6 @@
         <v>204</v>
       </c>
       <c r="K33" s="8"/>
-      <c r="L33" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="34" spans="1:12" ht="30">
       <c r="A34" s="8" t="s">
@@ -4792,9 +4738,6 @@
         <v>203</v>
       </c>
       <c r="K34" s="8"/>
-      <c r="L34" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="35" spans="1:12" ht="45">
       <c r="A35" s="8" t="s">
@@ -4824,9 +4767,6 @@
         <v>11</v>
       </c>
       <c r="K35" s="8"/>
-      <c r="L35" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="36" spans="1:12" ht="45">
       <c r="A36" s="8" t="s">
@@ -4858,9 +4798,6 @@
         <v>361</v>
       </c>
       <c r="K36" s="8"/>
-      <c r="L36" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="37" spans="1:12" ht="30">
       <c r="A37" s="8" t="s">
@@ -4892,9 +4829,6 @@
         <v>306</v>
       </c>
       <c r="K37" s="8"/>
-      <c r="L37" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="38" spans="1:12" ht="30">
       <c r="A38" s="8" t="s">
@@ -4926,9 +4860,6 @@
         <v>308</v>
       </c>
       <c r="K38" s="8"/>
-      <c r="L38" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="8" t="s">
@@ -4958,9 +4889,6 @@
         <v>310</v>
       </c>
       <c r="K39" s="8"/>
-      <c r="L39" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="40" spans="1:12" ht="30">
       <c r="A40" s="8" t="s">
@@ -4990,9 +4918,6 @@
         <v>246</v>
       </c>
       <c r="K40" s="8"/>
-      <c r="L40" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" t="s">
@@ -5010,20 +4935,14 @@
       <c r="E41" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F41"/>
       <c r="G41" t="s">
         <v>250</v>
       </c>
-      <c r="H41"/>
       <c r="I41" s="3" t="s">
         <v>177</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>251</v>
-      </c>
-      <c r="K41"/>
-      <c r="L41" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30">
@@ -5053,10 +4972,6 @@
       <c r="J42" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="K42"/>
-      <c r="L42" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" t="s">
@@ -5086,10 +5001,6 @@
       </c>
       <c r="J43" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="K43"/>
-      <c r="L43" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30">
@@ -5119,10 +5030,6 @@
       <c r="J44" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="K44"/>
-      <c r="L44" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="45" spans="1:12" ht="30">
       <c r="A45" t="s">
@@ -5153,10 +5060,6 @@
       <c r="J45" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K45"/>
-      <c r="L45" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="46" spans="1:12" ht="45">
       <c r="A46" t="s">
@@ -5187,10 +5090,6 @@
       <c r="J46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K46"/>
-      <c r="L46" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="47" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A47" s="8" t="s">
@@ -5224,9 +5123,7 @@
       <c r="K47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L47" t="s">
-        <v>500</v>
-      </c>
+      <c r="L47"/>
     </row>
     <row r="48" spans="1:12" ht="30">
       <c r="A48" s="8" t="s">
@@ -5258,9 +5155,6 @@
         <v>365</v>
       </c>
       <c r="K48" s="8"/>
-      <c r="L48" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="49" spans="1:11" ht="30">
       <c r="A49" t="s">
@@ -5291,10 +5185,6 @@
       <c r="J49" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="K49"/>
-      <c r="L49" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="50" spans="1:11" ht="30">
       <c r="A50" t="s">
@@ -5325,9 +5215,6 @@
       </c>
       <c r="K50" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="L50" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -5358,9 +5245,6 @@
         <v>378</v>
       </c>
       <c r="K51" s="8"/>
-      <c r="L51" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="52" spans="1:11" ht="60">
       <c r="A52" t="s">
@@ -5393,9 +5277,6 @@
       </c>
       <c r="K52" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="L52" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -5426,9 +5307,6 @@
         <v>383</v>
       </c>
       <c r="K53" s="8"/>
-      <c r="L53" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="54" spans="1:11" ht="75">
       <c r="A54" t="s">
@@ -5462,9 +5340,6 @@
       <c r="K54" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L54" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="55" spans="1:11" ht="75">
       <c r="A55" t="s">
@@ -5485,7 +5360,6 @@
       <c r="F55" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G55"/>
       <c r="H55" s="19" t="s">
         <v>441</v>
       </c>
@@ -5494,10 +5368,6 @@
       </c>
       <c r="J55" s="5" t="s">
         <v>442</v>
-      </c>
-      <c r="K55"/>
-      <c r="L55" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="45">
@@ -5532,9 +5402,6 @@
       <c r="K56" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L56" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="57" spans="1:11" ht="60">
       <c r="A57" t="s">
@@ -5564,10 +5431,6 @@
       </c>
       <c r="J57" s="5" t="s">
         <v>462</v>
-      </c>
-      <c r="K57"/>
-      <c r="L57" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="45">
@@ -5597,10 +5460,6 @@
       <c r="J58" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="K58"/>
-      <c r="L58" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="59" spans="1:11" ht="30">
       <c r="A59" s="8" t="s">
@@ -5629,10 +5488,6 @@
       <c r="J59" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="K59"/>
-      <c r="L59" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="60" spans="1:11" ht="210">
       <c r="A60" t="s">
@@ -5665,9 +5520,6 @@
       </c>
       <c r="K60" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="L60" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="30">
@@ -5696,10 +5548,6 @@
       </c>
       <c r="J61" s="5" t="s">
         <v>459</v>
-      </c>
-      <c r="K61"/>
-      <c r="L61" t="s">
-        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -5709,25 +5557,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="I26" workbookViewId="0">
+      <selection activeCell="L29" sqref="L2:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="80.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="98.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="98.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -5787,17 +5635,11 @@
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
       <c r="J2" s="5" t="s">
         <v>402</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
@@ -5819,19 +5661,14 @@
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3"/>
       <c r="H3" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="I3"/>
       <c r="J3" s="5" t="s">
         <v>311</v>
       </c>
       <c r="K3" t="s">
         <v>38</v>
-      </c>
-      <c r="L3" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
@@ -5853,19 +5690,14 @@
       <c r="F4" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G4"/>
       <c r="H4" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="I4"/>
       <c r="J4" s="5" t="s">
         <v>417</v>
       </c>
       <c r="K4" t="s">
         <v>38</v>
-      </c>
-      <c r="L4" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45">
@@ -5887,17 +5719,11 @@
       <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5"/>
       <c r="H5" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="I5"/>
       <c r="J5" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="75">
@@ -5919,19 +5745,14 @@
       <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G6"/>
       <c r="H6" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="I6"/>
       <c r="J6" s="5" t="s">
         <v>294</v>
       </c>
       <c r="K6" t="s">
         <v>38</v>
-      </c>
-      <c r="L6" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
@@ -5950,18 +5771,11 @@
       <c r="E7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
       <c r="I7" t="s">
         <v>317</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>319</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="75">
@@ -5983,7 +5797,6 @@
       <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G8"/>
       <c r="H8" s="14" t="s">
         <v>331</v>
       </c>
@@ -5995,9 +5808,6 @@
       </c>
       <c r="K8" t="s">
         <v>38</v>
-      </c>
-      <c r="L8" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
@@ -6019,7 +5829,6 @@
       <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G9"/>
       <c r="H9" s="1" t="s">
         <v>289</v>
       </c>
@@ -6028,10 +5837,6 @@
       </c>
       <c r="J9" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
@@ -6053,17 +5858,11 @@
       <c r="F10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G10"/>
-      <c r="H10"/>
       <c r="I10" t="s">
         <v>404</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>405</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
@@ -6085,17 +5884,11 @@
       <c r="F11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G11"/>
-      <c r="H11"/>
       <c r="I11" t="s">
         <v>404</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
@@ -6114,20 +5907,14 @@
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F12"/>
       <c r="G12" t="s">
         <v>321</v>
       </c>
-      <c r="H12"/>
       <c r="I12" t="s">
         <v>317</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>322</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
@@ -6149,7 +5936,6 @@
       <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G13"/>
       <c r="H13" s="1" t="s">
         <v>323</v>
       </c>
@@ -6161,9 +5947,6 @@
       </c>
       <c r="K13" t="s">
         <v>38</v>
-      </c>
-      <c r="L13" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
@@ -6182,18 +5965,11 @@
       <c r="E14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
       <c r="I14" t="s">
         <v>340</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="K14"/>
-      <c r="L14" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
@@ -6215,17 +5991,11 @@
       <c r="F15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G15"/>
-      <c r="H15"/>
       <c r="I15" t="s">
         <v>415</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="K15"/>
-      <c r="L15" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
@@ -6247,17 +6017,11 @@
       <c r="F16" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="G16"/>
-      <c r="H16"/>
       <c r="I16" t="s">
         <v>415</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="K16"/>
-      <c r="L16" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
@@ -6279,17 +6043,11 @@
       <c r="F17" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G17"/>
-      <c r="H17"/>
       <c r="I17" t="s">
         <v>330</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="K17"/>
-      <c r="L17" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="45">
@@ -6311,7 +6069,6 @@
       <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G18"/>
       <c r="H18" s="1" t="s">
         <v>341</v>
       </c>
@@ -6323,9 +6080,6 @@
       </c>
       <c r="K18" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="L18" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="45">
@@ -6356,9 +6110,6 @@
         <v>11</v>
       </c>
       <c r="K19" s="8"/>
-      <c r="L19" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="A20" t="s">
@@ -6379,7 +6130,6 @@
       <c r="F20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G20"/>
       <c r="H20" s="14" t="s">
         <v>342</v>
       </c>
@@ -6391,9 +6141,6 @@
       </c>
       <c r="K20" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="L20" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30">
@@ -6426,9 +6173,6 @@
         <v>343</v>
       </c>
       <c r="K21" s="8"/>
-      <c r="L21" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" t="s">
@@ -6459,10 +6203,6 @@
       <c r="J22" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="K22"/>
-      <c r="L22" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" t="s">
@@ -6483,15 +6223,8 @@
       <c r="F23" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
       <c r="J23" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="K23"/>
-      <c r="L23" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="45">
@@ -6513,15 +6246,8 @@
       <c r="F24" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
       <c r="J24" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="K24"/>
-      <c r="L24" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="45">
@@ -6552,9 +6278,6 @@
         <v>11</v>
       </c>
       <c r="K25" s="8"/>
-      <c r="L25" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" s="8" t="s">
@@ -6583,12 +6306,401 @@
       <c r="J26" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="K26"/>
-      <c r="L26" t="s">
-        <v>500</v>
+    </row>
+    <row r="27" spans="1:11" ht="60">
+      <c r="A27" t="s">
+        <v>539</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>283</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="I27" t="s">
+        <v>348</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="K27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="135">
+      <c r="A28" t="s">
+        <v>519</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
+        <v>540</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="I28" t="s">
+        <v>539</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" t="s">
+        <v>511</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>540</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" t="s">
+        <v>519</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="40.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="195">
+      <c r="A2" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="273" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>502</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="K3" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="240">
+      <c r="A4" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="75">
+      <c r="A5" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="180">
+      <c r="A6" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="345">
+      <c r="A7" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="90">
+      <c r="A8" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="105">
+      <c r="A9" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>